<commit_message>
Euro 2016 Game_Score id review
Euro 2016 Game_Score id review
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -27406,8 +27406,8 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
-        <f>'2008'!A192+1</f>
-        <v>939</v>
+        <f>'2012'!A188+1</f>
+        <v>1075</v>
       </c>
       <c r="B81" s="4">
         <f>A28</f>
@@ -27427,14 +27427,14 @@
       </c>
       <c r="G81" s="4" t="str">
         <f t="shared" ref="G81:G144" si="10">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A81 &amp; ", " &amp; B81 &amp; ", " &amp; C81 &amp; ", " &amp; D81 &amp; ", " &amp; E81 &amp; ", " &amp; F81 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (939, 236, 33, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1075, 236, 33, null, null, 2);</v>
       </c>
       <c r="H81" s="4"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <f>A81+1</f>
-        <v>940</v>
+        <v>1076</v>
       </c>
       <c r="B82" s="4">
         <f>B81</f>
@@ -27454,14 +27454,14 @@
       </c>
       <c r="G82" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (940, 236, 33, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1076, 236, 33, null, null, 1);</v>
       </c>
       <c r="H82" s="4"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <f t="shared" ref="A83:A146" si="11">A82+1</f>
-        <v>941</v>
+        <v>1077</v>
       </c>
       <c r="B83" s="4">
         <f>B81</f>
@@ -27481,14 +27481,14 @@
       </c>
       <c r="G83" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (941, 236, 40, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1077, 236, 40, null, null, 2);</v>
       </c>
       <c r="H83" s="4"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <f t="shared" si="11"/>
-        <v>942</v>
+        <v>1078</v>
       </c>
       <c r="B84" s="4">
         <f>B81</f>
@@ -27508,14 +27508,14 @@
       </c>
       <c r="G84" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (942, 236, 40, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1078, 236, 40, null, null, 1);</v>
       </c>
       <c r="H84" s="4"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <f t="shared" si="11"/>
-        <v>943</v>
+        <v>1079</v>
       </c>
       <c r="B85" s="4">
         <f>B81+1</f>
@@ -27535,14 +27535,14 @@
       </c>
       <c r="G85" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (943, 237, 355, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1079, 237, 355, null, null, 2);</v>
       </c>
       <c r="H85" s="4"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <f t="shared" si="11"/>
-        <v>944</v>
+        <v>1080</v>
       </c>
       <c r="B86" s="4">
         <f>B85</f>
@@ -27562,14 +27562,14 @@
       </c>
       <c r="G86" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (944, 237, 355, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1080, 237, 355, null, null, 1);</v>
       </c>
       <c r="H86" s="4"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <f t="shared" si="11"/>
-        <v>945</v>
+        <v>1081</v>
       </c>
       <c r="B87" s="4">
         <f>B85</f>
@@ -27589,14 +27589,14 @@
       </c>
       <c r="G87" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (945, 237, 41, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1081, 237, 41, null, null, 2);</v>
       </c>
       <c r="H87" s="4"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <f t="shared" si="11"/>
-        <v>946</v>
+        <v>1082</v>
       </c>
       <c r="B88" s="4">
         <f>B85</f>
@@ -27616,14 +27616,14 @@
       </c>
       <c r="G88" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (946, 237, 41, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1082, 237, 41, null, null, 1);</v>
       </c>
       <c r="H88" s="4"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <f t="shared" si="11"/>
-        <v>947</v>
+        <v>1083</v>
       </c>
       <c r="B89" s="4">
         <f>B85+1</f>
@@ -27643,14 +27643,14 @@
       </c>
       <c r="G89" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (947, 238, 40, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1083, 238, 40, null, null, 2);</v>
       </c>
       <c r="H89" s="4"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <f t="shared" si="11"/>
-        <v>948</v>
+        <v>1084</v>
       </c>
       <c r="B90" s="4">
         <f>B89</f>
@@ -27670,14 +27670,14 @@
       </c>
       <c r="G90" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (948, 238, 40, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1084, 238, 40, null, null, 1);</v>
       </c>
       <c r="H90" s="4"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <f t="shared" si="11"/>
-        <v>949</v>
+        <v>1085</v>
       </c>
       <c r="B91" s="4">
         <f>B89</f>
@@ -27697,14 +27697,14 @@
       </c>
       <c r="G91" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (949, 238, 41, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1085, 238, 41, null, null, 2);</v>
       </c>
       <c r="H91" s="4"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <f t="shared" si="11"/>
-        <v>950</v>
+        <v>1086</v>
       </c>
       <c r="B92" s="4">
         <f>B89</f>
@@ -27724,14 +27724,14 @@
       </c>
       <c r="G92" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (950, 238, 41, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1086, 238, 41, null, null, 1);</v>
       </c>
       <c r="H92" s="4"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <f t="shared" si="11"/>
-        <v>951</v>
+        <v>1087</v>
       </c>
       <c r="B93" s="4">
         <f>B89+1</f>
@@ -27751,14 +27751,14 @@
       </c>
       <c r="G93" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (951, 239, 33, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1087, 239, 33, null, null, 2);</v>
       </c>
       <c r="H93" s="4"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <f t="shared" si="11"/>
-        <v>952</v>
+        <v>1088</v>
       </c>
       <c r="B94" s="4">
         <f>B93</f>
@@ -27778,14 +27778,14 @@
       </c>
       <c r="G94" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (952, 239, 33, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1088, 239, 33, null, null, 1);</v>
       </c>
       <c r="H94" s="4"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <f t="shared" si="11"/>
-        <v>953</v>
+        <v>1089</v>
       </c>
       <c r="B95" s="4">
         <f>B93</f>
@@ -27805,14 +27805,14 @@
       </c>
       <c r="G95" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (953, 239, 355, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1089, 239, 355, null, null, 2);</v>
       </c>
       <c r="H95" s="4"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <f t="shared" si="11"/>
-        <v>954</v>
+        <v>1090</v>
       </c>
       <c r="B96" s="4">
         <f>B93</f>
@@ -27832,14 +27832,14 @@
       </c>
       <c r="G96" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (954, 239, 355, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1090, 239, 355, null, null, 1);</v>
       </c>
       <c r="H96" s="4"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <f t="shared" si="11"/>
-        <v>955</v>
+        <v>1091</v>
       </c>
       <c r="B97" s="4">
         <f>B93+1</f>
@@ -27859,14 +27859,14 @@
       </c>
       <c r="G97" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (955, 240, 40, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1091, 240, 40, null, null, 2);</v>
       </c>
       <c r="H97" s="4"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <f t="shared" si="11"/>
-        <v>956</v>
+        <v>1092</v>
       </c>
       <c r="B98" s="4">
         <f>B97</f>
@@ -27886,14 +27886,14 @@
       </c>
       <c r="G98" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (956, 240, 40, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1092, 240, 40, null, null, 1);</v>
       </c>
       <c r="H98" s="4"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <f t="shared" si="11"/>
-        <v>957</v>
+        <v>1093</v>
       </c>
       <c r="B99" s="4">
         <f>B97</f>
@@ -27913,14 +27913,14 @@
       </c>
       <c r="G99" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (957, 240, 355, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1093, 240, 355, null, null, 2);</v>
       </c>
       <c r="H99" s="4"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <f t="shared" si="11"/>
-        <v>958</v>
+        <v>1094</v>
       </c>
       <c r="B100" s="4">
         <f>B97</f>
@@ -27940,14 +27940,14 @@
       </c>
       <c r="G100" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (958, 240, 355, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1094, 240, 355, null, null, 1);</v>
       </c>
       <c r="H100" s="4"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <f t="shared" si="11"/>
-        <v>959</v>
+        <v>1095</v>
       </c>
       <c r="B101" s="4">
         <f>B97+1</f>
@@ -27967,14 +27967,14 @@
       </c>
       <c r="G101" s="4" t="str">
         <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A101 &amp; ", " &amp; B101 &amp; ", " &amp; C101 &amp; ", " &amp; D101 &amp; ", " &amp; E101 &amp; ", " &amp; F101 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (959, 241, 41, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1095, 241, 41, null, null, 2);</v>
       </c>
       <c r="H101" s="4"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <f t="shared" si="11"/>
-        <v>960</v>
+        <v>1096</v>
       </c>
       <c r="B102" s="4">
         <f>B101</f>
@@ -27994,14 +27994,14 @@
       </c>
       <c r="G102" s="4" t="str">
         <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A102 &amp; ", " &amp; B102 &amp; ", " &amp; C102 &amp; ", " &amp; D102 &amp; ", " &amp; E102 &amp; ", " &amp; F102 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (960, 241, 41, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1096, 241, 41, null, null, 1);</v>
       </c>
       <c r="H102" s="4"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <f t="shared" si="11"/>
-        <v>961</v>
+        <v>1097</v>
       </c>
       <c r="B103" s="4">
         <f>B101</f>
@@ -28021,14 +28021,14 @@
       </c>
       <c r="G103" s="4" t="str">
         <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A103 &amp; ", " &amp; B103 &amp; ", " &amp; C103 &amp; ", " &amp; D103 &amp; ", " &amp; E103 &amp; ", " &amp; F103 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (961, 241, 33, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1097, 241, 33, null, null, 2);</v>
       </c>
       <c r="H103" s="4"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <f t="shared" si="11"/>
-        <v>962</v>
+        <v>1098</v>
       </c>
       <c r="B104" s="4">
         <f>B101</f>
@@ -28048,14 +28048,14 @@
       </c>
       <c r="G104" s="4" t="str">
         <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A104 &amp; ", " &amp; B104 &amp; ", " &amp; C104 &amp; ", " &amp; D104 &amp; ", " &amp; E104 &amp; ", " &amp; F104 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (962, 241, 33, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1098, 241, 33, null, null, 1);</v>
       </c>
       <c r="H104" s="4"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <f t="shared" si="11"/>
-        <v>963</v>
+        <v>1099</v>
       </c>
       <c r="B105" s="4">
         <f>B101+1</f>
@@ -28075,14 +28075,14 @@
       </c>
       <c r="G105" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (963, 242, 4429, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1099, 242, 4429, null, null, 2);</v>
       </c>
       <c r="H105" s="4"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <f t="shared" si="11"/>
-        <v>964</v>
+        <v>1100</v>
       </c>
       <c r="B106" s="4">
         <f>B105</f>
@@ -28102,14 +28102,14 @@
       </c>
       <c r="G106" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (964, 242, 4429, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1100, 242, 4429, null, null, 1);</v>
       </c>
       <c r="H106" s="4"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <f t="shared" si="11"/>
-        <v>965</v>
+        <v>1101</v>
       </c>
       <c r="B107" s="4">
         <f>B105</f>
@@ -28129,14 +28129,14 @@
       </c>
       <c r="G107" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (965, 242, 421, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1101, 242, 421, null, null, 2);</v>
       </c>
       <c r="H107" s="4"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <f t="shared" si="11"/>
-        <v>966</v>
+        <v>1102</v>
       </c>
       <c r="B108" s="4">
         <f>B105</f>
@@ -28156,14 +28156,14 @@
       </c>
       <c r="G108" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (966, 242, 421, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1102, 242, 421, null, null, 1);</v>
       </c>
       <c r="H108" s="4"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <f t="shared" si="11"/>
-        <v>967</v>
+        <v>1103</v>
       </c>
       <c r="B109" s="4">
         <f>B105+1</f>
@@ -28183,14 +28183,14 @@
       </c>
       <c r="G109" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (967, 243, 4420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1103, 243, 4420, null, null, 2);</v>
       </c>
       <c r="H109" s="4"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <f t="shared" si="11"/>
-        <v>968</v>
+        <v>1104</v>
       </c>
       <c r="B110" s="4">
         <f>B109</f>
@@ -28210,14 +28210,14 @@
       </c>
       <c r="G110" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (968, 243, 4420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1104, 243, 4420, null, null, 1);</v>
       </c>
       <c r="H110" s="4"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <f t="shared" si="11"/>
-        <v>969</v>
+        <v>1105</v>
       </c>
       <c r="B111" s="4">
         <f>B109</f>
@@ -28237,14 +28237,14 @@
       </c>
       <c r="G111" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (969, 243, 7, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1105, 243, 7, null, null, 2);</v>
       </c>
       <c r="H111" s="4"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <f t="shared" si="11"/>
-        <v>970</v>
+        <v>1106</v>
       </c>
       <c r="B112" s="4">
         <f>B109</f>
@@ -28264,14 +28264,14 @@
       </c>
       <c r="G112" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (970, 243, 7, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1106, 243, 7, null, null, 1);</v>
       </c>
       <c r="H112" s="4"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <f t="shared" si="11"/>
-        <v>971</v>
+        <v>1107</v>
       </c>
       <c r="B113" s="4">
         <f>B109+1</f>
@@ -28291,14 +28291,14 @@
       </c>
       <c r="G113" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (971, 244, 7, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1107, 244, 7, null, null, 2);</v>
       </c>
       <c r="H113" s="4"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <f t="shared" si="11"/>
-        <v>972</v>
+        <v>1108</v>
       </c>
       <c r="B114" s="4">
         <f>B113</f>
@@ -28318,14 +28318,14 @@
       </c>
       <c r="G114" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (972, 244, 7, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1108, 244, 7, null, null, 1);</v>
       </c>
       <c r="H114" s="4"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <f t="shared" si="11"/>
-        <v>973</v>
+        <v>1109</v>
       </c>
       <c r="B115" s="4">
         <f>B113</f>
@@ -28345,14 +28345,14 @@
       </c>
       <c r="G115" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (973, 244, 421, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1109, 244, 421, null, null, 2);</v>
       </c>
       <c r="H115" s="4"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <f t="shared" si="11"/>
-        <v>974</v>
+        <v>1110</v>
       </c>
       <c r="B116" s="4">
         <f>B113</f>
@@ -28372,14 +28372,14 @@
       </c>
       <c r="G116" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (974, 244, 421, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1110, 244, 421, null, null, 1);</v>
       </c>
       <c r="H116" s="4"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <f t="shared" si="11"/>
-        <v>975</v>
+        <v>1111</v>
       </c>
       <c r="B117" s="4">
         <f>B113+1</f>
@@ -28399,14 +28399,14 @@
       </c>
       <c r="G117" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (975, 245, 4420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1111, 245, 4420, null, null, 2);</v>
       </c>
       <c r="H117" s="4"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <f t="shared" si="11"/>
-        <v>976</v>
+        <v>1112</v>
       </c>
       <c r="B118" s="4">
         <f>B117</f>
@@ -28426,14 +28426,14 @@
       </c>
       <c r="G118" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (976, 245, 4420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1112, 245, 4420, null, null, 1);</v>
       </c>
       <c r="H118" s="4"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <f t="shared" si="11"/>
-        <v>977</v>
+        <v>1113</v>
       </c>
       <c r="B119" s="4">
         <f>B117</f>
@@ -28453,14 +28453,14 @@
       </c>
       <c r="G119" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (977, 245, 4429, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1113, 245, 4429, null, null, 2);</v>
       </c>
       <c r="H119" s="4"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <f t="shared" si="11"/>
-        <v>978</v>
+        <v>1114</v>
       </c>
       <c r="B120" s="4">
         <f>B117</f>
@@ -28480,14 +28480,14 @@
       </c>
       <c r="G120" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (978, 245, 4429, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1114, 245, 4429, null, null, 1);</v>
       </c>
       <c r="H120" s="4"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <f t="shared" si="11"/>
-        <v>979</v>
+        <v>1115</v>
       </c>
       <c r="B121" s="4">
         <f>B117+1</f>
@@ -28507,14 +28507,14 @@
       </c>
       <c r="G121" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (979, 246, 7, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1115, 246, 7, null, null, 2);</v>
       </c>
       <c r="H121" s="4"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <f t="shared" si="11"/>
-        <v>980</v>
+        <v>1116</v>
       </c>
       <c r="B122" s="4">
         <f>B121</f>
@@ -28534,14 +28534,14 @@
       </c>
       <c r="G122" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (980, 246, 7, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1116, 246, 7, null, null, 1);</v>
       </c>
       <c r="H122" s="4"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <f t="shared" si="11"/>
-        <v>981</v>
+        <v>1117</v>
       </c>
       <c r="B123" s="4">
         <f>B121</f>
@@ -28561,14 +28561,14 @@
       </c>
       <c r="G123" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (981, 246, 4429, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1117, 246, 4429, null, null, 2);</v>
       </c>
       <c r="H123" s="4"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <f t="shared" si="11"/>
-        <v>982</v>
+        <v>1118</v>
       </c>
       <c r="B124" s="4">
         <f>B121</f>
@@ -28588,14 +28588,14 @@
       </c>
       <c r="G124" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (982, 246, 4429, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1118, 246, 4429, null, null, 1);</v>
       </c>
       <c r="H124" s="4"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <f t="shared" si="11"/>
-        <v>983</v>
+        <v>1119</v>
       </c>
       <c r="B125" s="4">
         <f>B121+1</f>
@@ -28615,14 +28615,14 @@
       </c>
       <c r="G125" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (983, 247, 421, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1119, 247, 421, null, null, 2);</v>
       </c>
       <c r="H125" s="4"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <f t="shared" si="11"/>
-        <v>984</v>
+        <v>1120</v>
       </c>
       <c r="B126" s="4">
         <f>B125</f>
@@ -28642,14 +28642,14 @@
       </c>
       <c r="G126" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (984, 247, 421, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1120, 247, 421, null, null, 1);</v>
       </c>
       <c r="H126" s="4"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <f t="shared" si="11"/>
-        <v>985</v>
+        <v>1121</v>
       </c>
       <c r="B127" s="4">
         <f>B125</f>
@@ -28669,14 +28669,14 @@
       </c>
       <c r="G127" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (985, 247, 4420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1121, 247, 4420, null, null, 2);</v>
       </c>
       <c r="H127" s="4"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <f t="shared" si="11"/>
-        <v>986</v>
+        <v>1122</v>
       </c>
       <c r="B128" s="4">
         <f>B125</f>
@@ -28696,14 +28696,14 @@
       </c>
       <c r="G128" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (986, 247, 4420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1122, 247, 4420, null, null, 1);</v>
       </c>
       <c r="H128" s="4"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <f t="shared" si="11"/>
-        <v>987</v>
+        <v>1123</v>
       </c>
       <c r="B129" s="4">
         <f>B125+1</f>
@@ -28723,14 +28723,14 @@
       </c>
       <c r="G129" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (987, 248, 48, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1123, 248, 48, null, null, 2);</v>
       </c>
       <c r="H129" s="4"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <f t="shared" si="11"/>
-        <v>988</v>
+        <v>1124</v>
       </c>
       <c r="B130" s="4">
         <f>B129</f>
@@ -28750,14 +28750,14 @@
       </c>
       <c r="G130" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (988, 248, 48, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1124, 248, 48, null, null, 1);</v>
       </c>
       <c r="H130" s="4"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <f t="shared" si="11"/>
-        <v>989</v>
+        <v>1125</v>
       </c>
       <c r="B131" s="4">
         <f>B129</f>
@@ -28777,14 +28777,14 @@
       </c>
       <c r="G131" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (989, 248, 4428, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1125, 248, 4428, null, null, 2);</v>
       </c>
       <c r="H131" s="4"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <f t="shared" si="11"/>
-        <v>990</v>
+        <v>1126</v>
       </c>
       <c r="B132" s="4">
         <f>B129</f>
@@ -28804,14 +28804,14 @@
       </c>
       <c r="G132" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (990, 248, 4428, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1126, 248, 4428, null, null, 1);</v>
       </c>
       <c r="H132" s="4"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <f t="shared" si="11"/>
-        <v>991</v>
+        <v>1127</v>
       </c>
       <c r="B133" s="4">
         <f>B129+1</f>
@@ -28831,14 +28831,14 @@
       </c>
       <c r="G133" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (991, 249, 49, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1127, 249, 49, null, null, 2);</v>
       </c>
       <c r="H133" s="4"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <f t="shared" si="11"/>
-        <v>992</v>
+        <v>1128</v>
       </c>
       <c r="B134" s="4">
         <f>B133</f>
@@ -28858,14 +28858,14 @@
       </c>
       <c r="G134" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (992, 249, 49, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1128, 249, 49, null, null, 1);</v>
       </c>
       <c r="H134" s="4"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <f t="shared" si="11"/>
-        <v>993</v>
+        <v>1129</v>
       </c>
       <c r="B135" s="4">
         <f>B133</f>
@@ -28885,14 +28885,14 @@
       </c>
       <c r="G135" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (993, 249, 380, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1129, 249, 380, null, null, 2);</v>
       </c>
       <c r="H135" s="4"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <f t="shared" si="11"/>
-        <v>994</v>
+        <v>1130</v>
       </c>
       <c r="B136" s="4">
         <f>B133</f>
@@ -28912,14 +28912,14 @@
       </c>
       <c r="G136" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (994, 249, 380, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1130, 249, 380, null, null, 1);</v>
       </c>
       <c r="H136" s="4"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <f t="shared" si="11"/>
-        <v>995</v>
+        <v>1131</v>
       </c>
       <c r="B137" s="4">
         <f>B133+1</f>
@@ -28939,14 +28939,14 @@
       </c>
       <c r="G137" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (995, 250, 380, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1131, 250, 380, null, null, 2);</v>
       </c>
       <c r="H137" s="4"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <f t="shared" si="11"/>
-        <v>996</v>
+        <v>1132</v>
       </c>
       <c r="B138" s="4">
         <f>B137</f>
@@ -28966,14 +28966,14 @@
       </c>
       <c r="G138" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (996, 250, 380, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1132, 250, 380, null, null, 1);</v>
       </c>
       <c r="H138" s="4"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <f t="shared" si="11"/>
-        <v>997</v>
+        <v>1133</v>
       </c>
       <c r="B139" s="4">
         <f>B137</f>
@@ -28993,14 +28993,14 @@
       </c>
       <c r="G139" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (997, 250, 4428, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1133, 250, 4428, null, null, 2);</v>
       </c>
       <c r="H139" s="4"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <f t="shared" si="11"/>
-        <v>998</v>
+        <v>1134</v>
       </c>
       <c r="B140" s="4">
         <f>B137</f>
@@ -29020,14 +29020,14 @@
       </c>
       <c r="G140" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (998, 250, 4428, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1134, 250, 4428, null, null, 1);</v>
       </c>
       <c r="H140" s="4"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <f t="shared" si="11"/>
-        <v>999</v>
+        <v>1135</v>
       </c>
       <c r="B141" s="4">
         <f>B137+1</f>
@@ -29047,14 +29047,14 @@
       </c>
       <c r="G141" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (999, 251, 49, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1135, 251, 49, null, null, 2);</v>
       </c>
       <c r="H141" s="4"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <f t="shared" si="11"/>
-        <v>1000</v>
+        <v>1136</v>
       </c>
       <c r="B142" s="4">
         <f>B141</f>
@@ -29074,14 +29074,14 @@
       </c>
       <c r="G142" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1000, 251, 49, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1136, 251, 49, null, null, 1);</v>
       </c>
       <c r="H142" s="4"/>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <f t="shared" si="11"/>
-        <v>1001</v>
+        <v>1137</v>
       </c>
       <c r="B143" s="4">
         <f>B141</f>
@@ -29101,14 +29101,14 @@
       </c>
       <c r="G143" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1001, 251, 48, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1137, 251, 48, null, null, 2);</v>
       </c>
       <c r="H143" s="4"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <f t="shared" si="11"/>
-        <v>1002</v>
+        <v>1138</v>
       </c>
       <c r="B144" s="4">
         <f>B141</f>
@@ -29128,14 +29128,14 @@
       </c>
       <c r="G144" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1002, 251, 48, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1138, 251, 48, null, null, 1);</v>
       </c>
       <c r="H144" s="4"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <f t="shared" si="11"/>
-        <v>1003</v>
+        <v>1139</v>
       </c>
       <c r="B145" s="4">
         <f>B141+1</f>
@@ -29155,14 +29155,14 @@
       </c>
       <c r="G145" s="4" t="str">
         <f t="shared" ref="G145:G192" si="12">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A145 &amp; ", " &amp; B145 &amp; ", " &amp; C145 &amp; ", " &amp; D145 &amp; ", " &amp; E145 &amp; ", " &amp; F145 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1003, 252, 380, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1139, 252, 380, null, null, 2);</v>
       </c>
       <c r="H145" s="4"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <f t="shared" si="11"/>
-        <v>1004</v>
+        <v>1140</v>
       </c>
       <c r="B146" s="4">
         <f>B145</f>
@@ -29182,14 +29182,14 @@
       </c>
       <c r="G146" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1004, 252, 380, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1140, 252, 380, null, null, 1);</v>
       </c>
       <c r="H146" s="4"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <f t="shared" ref="A147:A210" si="13">A146+1</f>
-        <v>1005</v>
+        <v>1141</v>
       </c>
       <c r="B147" s="4">
         <f>B145</f>
@@ -29209,14 +29209,14 @@
       </c>
       <c r="G147" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1005, 252, 48, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1141, 252, 48, null, null, 2);</v>
       </c>
       <c r="H147" s="4"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <f t="shared" si="13"/>
-        <v>1006</v>
+        <v>1142</v>
       </c>
       <c r="B148" s="4">
         <f>B145</f>
@@ -29236,13 +29236,13 @@
       </c>
       <c r="G148" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1006, 252, 48, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1142, 252, 48, null, null, 1);</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <f t="shared" si="13"/>
-        <v>1007</v>
+        <v>1143</v>
       </c>
       <c r="B149" s="4">
         <f>B145+1</f>
@@ -29262,13 +29262,13 @@
       </c>
       <c r="G149" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1007, 253, 4428, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1143, 253, 4428, null, null, 2);</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <f t="shared" si="13"/>
-        <v>1008</v>
+        <v>1144</v>
       </c>
       <c r="B150" s="4">
         <f>B149</f>
@@ -29288,13 +29288,13 @@
       </c>
       <c r="G150" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1008, 253, 4428, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1144, 253, 4428, null, null, 1);</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <f t="shared" si="13"/>
-        <v>1009</v>
+        <v>1145</v>
       </c>
       <c r="B151" s="4">
         <f>B149</f>
@@ -29314,13 +29314,13 @@
       </c>
       <c r="G151" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1009, 253, 49, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1145, 253, 49, null, null, 2);</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <f t="shared" si="13"/>
-        <v>1010</v>
+        <v>1146</v>
       </c>
       <c r="B152" s="4">
         <f>B149</f>
@@ -29340,13 +29340,13 @@
       </c>
       <c r="G152" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1010, 253, 49, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1146, 253, 49, null, null, 1);</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <f t="shared" si="13"/>
-        <v>1011</v>
+        <v>1147</v>
       </c>
       <c r="B153" s="4">
         <f>B149+1</f>
@@ -29366,13 +29366,13 @@
       </c>
       <c r="G153" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1011, 254, 90, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1147, 254, 90, null, null, 2);</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <f t="shared" si="13"/>
-        <v>1012</v>
+        <v>1148</v>
       </c>
       <c r="B154" s="4">
         <f>B153</f>
@@ -29392,13 +29392,13 @@
       </c>
       <c r="G154" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1012, 254, 90, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1148, 254, 90, null, null, 1);</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <f t="shared" si="13"/>
-        <v>1013</v>
+        <v>1149</v>
       </c>
       <c r="B155" s="4">
         <f>B153</f>
@@ -29418,13 +29418,13 @@
       </c>
       <c r="G155" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1013, 254, 385, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1149, 254, 385, null, null, 2);</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <f t="shared" si="13"/>
-        <v>1014</v>
+        <v>1150</v>
       </c>
       <c r="B156" s="4">
         <f>B153</f>
@@ -29444,13 +29444,13 @@
       </c>
       <c r="G156" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1014, 254, 385, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1150, 254, 385, null, null, 1);</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <f t="shared" si="13"/>
-        <v>1015</v>
+        <v>1151</v>
       </c>
       <c r="B157" s="4">
         <f>B153+1</f>
@@ -29470,13 +29470,13 @@
       </c>
       <c r="G157" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1015, 255, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1151, 255, 34, null, null, 2);</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <f t="shared" si="13"/>
-        <v>1016</v>
+        <v>1152</v>
       </c>
       <c r="B158" s="4">
         <f>B157</f>
@@ -29496,13 +29496,13 @@
       </c>
       <c r="G158" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1016, 255, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1152, 255, 34, null, null, 1);</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <f t="shared" si="13"/>
-        <v>1017</v>
+        <v>1153</v>
       </c>
       <c r="B159" s="4">
         <f>B157</f>
@@ -29522,13 +29522,13 @@
       </c>
       <c r="G159" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1017, 255, 420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1153, 255, 420, null, null, 2);</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <f t="shared" si="13"/>
-        <v>1018</v>
+        <v>1154</v>
       </c>
       <c r="B160" s="4">
         <f>B157</f>
@@ -29548,13 +29548,13 @@
       </c>
       <c r="G160" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1018, 255, 420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1154, 255, 420, null, null, 1);</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <f t="shared" si="13"/>
-        <v>1019</v>
+        <v>1155</v>
       </c>
       <c r="B161" s="4">
         <f>B157+1</f>
@@ -29574,13 +29574,13 @@
       </c>
       <c r="G161" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1019, 256, 420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1155, 256, 420, null, null, 2);</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <f t="shared" si="13"/>
-        <v>1020</v>
+        <v>1156</v>
       </c>
       <c r="B162" s="4">
         <f>B161</f>
@@ -29600,13 +29600,13 @@
       </c>
       <c r="G162" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1020, 256, 420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1156, 256, 420, null, null, 1);</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <f t="shared" si="13"/>
-        <v>1021</v>
+        <v>1157</v>
       </c>
       <c r="B163" s="4">
         <f>B161</f>
@@ -29626,13 +29626,13 @@
       </c>
       <c r="G163" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1021, 256, 385, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1157, 256, 385, null, null, 2);</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <f t="shared" si="13"/>
-        <v>1022</v>
+        <v>1158</v>
       </c>
       <c r="B164" s="4">
         <f>B161</f>
@@ -29652,13 +29652,13 @@
       </c>
       <c r="G164" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1022, 256, 385, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1158, 256, 385, null, null, 1);</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <f t="shared" si="13"/>
-        <v>1023</v>
+        <v>1159</v>
       </c>
       <c r="B165" s="4">
         <f>B161+1</f>
@@ -29678,13 +29678,13 @@
       </c>
       <c r="G165" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1023, 257, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1159, 257, 34, null, null, 2);</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <f t="shared" si="13"/>
-        <v>1024</v>
+        <v>1160</v>
       </c>
       <c r="B166" s="4">
         <f>B165</f>
@@ -29704,13 +29704,13 @@
       </c>
       <c r="G166" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1024, 257, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1160, 257, 34, null, null, 1);</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <f t="shared" si="13"/>
-        <v>1025</v>
+        <v>1161</v>
       </c>
       <c r="B167" s="4">
         <f>B165</f>
@@ -29730,13 +29730,13 @@
       </c>
       <c r="G167" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1025, 257, 90, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1161, 257, 90, null, null, 2);</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <f t="shared" si="13"/>
-        <v>1026</v>
+        <v>1162</v>
       </c>
       <c r="B168" s="4">
         <f>B165</f>
@@ -29756,13 +29756,13 @@
       </c>
       <c r="G168" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1026, 257, 90, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1162, 257, 90, null, null, 1);</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <f t="shared" si="13"/>
-        <v>1027</v>
+        <v>1163</v>
       </c>
       <c r="B169" s="4">
         <f>B165+1</f>
@@ -29782,13 +29782,13 @@
       </c>
       <c r="G169" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1027, 258, 420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1163, 258, 420, null, null, 2);</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <f t="shared" si="13"/>
-        <v>1028</v>
+        <v>1164</v>
       </c>
       <c r="B170" s="4">
         <f>B169</f>
@@ -29808,13 +29808,13 @@
       </c>
       <c r="G170" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1028, 258, 420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1164, 258, 420, null, null, 1);</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <f t="shared" si="13"/>
-        <v>1029</v>
+        <v>1165</v>
       </c>
       <c r="B171" s="4">
         <f>B169</f>
@@ -29834,13 +29834,13 @@
       </c>
       <c r="G171" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1029, 258, 90, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1165, 258, 90, null, null, 2);</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <f t="shared" si="13"/>
-        <v>1030</v>
+        <v>1166</v>
       </c>
       <c r="B172" s="4">
         <f>B169</f>
@@ -29860,13 +29860,13 @@
       </c>
       <c r="G172" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1030, 258, 90, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1166, 258, 90, null, null, 1);</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <f t="shared" si="13"/>
-        <v>1031</v>
+        <v>1167</v>
       </c>
       <c r="B173" s="4">
         <f>B169+1</f>
@@ -29886,13 +29886,13 @@
       </c>
       <c r="G173" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1031, 259, 385, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1167, 259, 385, null, null, 2);</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <f t="shared" si="13"/>
-        <v>1032</v>
+        <v>1168</v>
       </c>
       <c r="B174" s="4">
         <f>B173</f>
@@ -29912,13 +29912,13 @@
       </c>
       <c r="G174" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1032, 259, 385, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1168, 259, 385, null, null, 1);</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <f t="shared" si="13"/>
-        <v>1033</v>
+        <v>1169</v>
       </c>
       <c r="B175" s="4">
         <f>B173</f>
@@ -29938,13 +29938,13 @@
       </c>
       <c r="G175" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1033, 259, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1169, 259, 34, null, null, 2);</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <f t="shared" si="13"/>
-        <v>1034</v>
+        <v>1170</v>
       </c>
       <c r="B176" s="4">
         <f>B174</f>
@@ -29964,13 +29964,13 @@
       </c>
       <c r="G176" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1034, 259, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1170, 259, 34, null, null, 1);</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <f t="shared" si="13"/>
-        <v>1035</v>
+        <v>1171</v>
       </c>
       <c r="B177" s="4">
         <f>B173+1</f>
@@ -29990,13 +29990,13 @@
       </c>
       <c r="G177" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1035, 260, 353, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1171, 260, 353, null, null, 2);</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <f t="shared" si="13"/>
-        <v>1036</v>
+        <v>1172</v>
       </c>
       <c r="B178" s="4">
         <f>B177</f>
@@ -30016,13 +30016,13 @@
       </c>
       <c r="G178" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1036, 260, 353, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1172, 260, 353, null, null, 1);</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <f t="shared" si="13"/>
-        <v>1037</v>
+        <v>1173</v>
       </c>
       <c r="B179" s="4">
         <f>B177</f>
@@ -30042,13 +30042,13 @@
       </c>
       <c r="G179" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1037, 260, 46, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1173, 260, 46, null, null, 2);</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <f t="shared" si="13"/>
-        <v>1038</v>
+        <v>1174</v>
       </c>
       <c r="B180" s="4">
         <f>B178</f>
@@ -30068,13 +30068,13 @@
       </c>
       <c r="G180" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1038, 260, 46, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1174, 260, 46, null, null, 1);</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <f t="shared" si="13"/>
-        <v>1039</v>
+        <v>1175</v>
       </c>
       <c r="B181" s="4">
         <f>B177+1</f>
@@ -30094,13 +30094,13 @@
       </c>
       <c r="G181" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1039, 261, 32, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1175, 261, 32, null, null, 2);</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <f t="shared" si="13"/>
-        <v>1040</v>
+        <v>1176</v>
       </c>
       <c r="B182" s="4">
         <f>B181</f>
@@ -30120,13 +30120,13 @@
       </c>
       <c r="G182" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1040, 261, 32, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1176, 261, 32, null, null, 1);</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <f t="shared" si="13"/>
-        <v>1041</v>
+        <v>1177</v>
       </c>
       <c r="B183" s="4">
         <f>B181</f>
@@ -30146,13 +30146,13 @@
       </c>
       <c r="G183" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1041, 261, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1177, 261, 39, null, null, 2);</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <f t="shared" si="13"/>
-        <v>1042</v>
+        <v>1178</v>
       </c>
       <c r="B184" s="4">
         <f>B182</f>
@@ -30172,13 +30172,13 @@
       </c>
       <c r="G184" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1042, 261, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1178, 261, 39, null, null, 1);</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <f t="shared" si="13"/>
-        <v>1043</v>
+        <v>1179</v>
       </c>
       <c r="B185" s="4">
         <f>B181+1</f>
@@ -30198,13 +30198,13 @@
       </c>
       <c r="G185" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1043, 262, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1179, 262, 39, null, null, 2);</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <f t="shared" si="13"/>
-        <v>1044</v>
+        <v>1180</v>
       </c>
       <c r="B186" s="4">
         <f>B185</f>
@@ -30224,13 +30224,13 @@
       </c>
       <c r="G186" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1044, 262, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1180, 262, 39, null, null, 1);</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <f t="shared" si="13"/>
-        <v>1045</v>
+        <v>1181</v>
       </c>
       <c r="B187" s="4">
         <f>B185</f>
@@ -30250,13 +30250,13 @@
       </c>
       <c r="G187" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1045, 262, 46, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1181, 262, 46, null, null, 2);</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <f t="shared" si="13"/>
-        <v>1046</v>
+        <v>1182</v>
       </c>
       <c r="B188" s="4">
         <f>B186</f>
@@ -30276,13 +30276,13 @@
       </c>
       <c r="G188" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1046, 262, 46, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1182, 262, 46, null, null, 1);</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <f t="shared" si="13"/>
-        <v>1047</v>
+        <v>1183</v>
       </c>
       <c r="B189" s="4">
         <f>B185+1</f>
@@ -30302,13 +30302,13 @@
       </c>
       <c r="G189" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1047, 263, 32, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1183, 263, 32, null, null, 2);</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <f t="shared" si="13"/>
-        <v>1048</v>
+        <v>1184</v>
       </c>
       <c r="B190" s="4">
         <f>B189</f>
@@ -30328,13 +30328,13 @@
       </c>
       <c r="G190" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1048, 263, 32, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1184, 263, 32, null, null, 1);</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <f t="shared" si="13"/>
-        <v>1049</v>
+        <v>1185</v>
       </c>
       <c r="B191" s="4">
         <f t="shared" ref="B191:B192" si="14">B189</f>
@@ -30354,13 +30354,13 @@
       </c>
       <c r="G191" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1049, 263, 353, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1185, 263, 353, null, null, 2);</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <f t="shared" si="13"/>
-        <v>1050</v>
+        <v>1186</v>
       </c>
       <c r="B192" s="4">
         <f t="shared" si="14"/>
@@ -30380,13 +30380,13 @@
       </c>
       <c r="G192" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1050, 263, 353, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1186, 263, 353, null, null, 1);</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <f t="shared" si="13"/>
-        <v>1051</v>
+        <v>1187</v>
       </c>
       <c r="B193" s="4">
         <f>B189+1</f>
@@ -30406,13 +30406,13 @@
       </c>
       <c r="G193" s="4" t="str">
         <f t="shared" ref="G193:G256" si="15">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A193 &amp; ", " &amp; B193 &amp; ", " &amp; C193 &amp; ", " &amp; D193 &amp; ", " &amp; E193 &amp; ", " &amp; F193 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1051, 264, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1187, 264, 39, null, null, 2);</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <f t="shared" si="13"/>
-        <v>1052</v>
+        <v>1188</v>
       </c>
       <c r="B194" s="4">
         <f>B193</f>
@@ -30432,13 +30432,13 @@
       </c>
       <c r="G194" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1052, 264, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1188, 264, 39, null, null, 1);</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <f t="shared" si="13"/>
-        <v>1053</v>
+        <v>1189</v>
       </c>
       <c r="B195" s="4">
         <f t="shared" ref="B195:B196" si="16">B193</f>
@@ -30458,13 +30458,13 @@
       </c>
       <c r="G195" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1053, 264, 353, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1189, 264, 353, null, null, 2);</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <f t="shared" si="13"/>
-        <v>1054</v>
+        <v>1190</v>
       </c>
       <c r="B196" s="4">
         <f t="shared" si="16"/>
@@ -30484,13 +30484,13 @@
       </c>
       <c r="G196" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1054, 264, 353, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1190, 264, 353, null, null, 1);</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <f t="shared" si="13"/>
-        <v>1055</v>
+        <v>1191</v>
       </c>
       <c r="B197" s="4">
         <f>B193+1</f>
@@ -30510,13 +30510,13 @@
       </c>
       <c r="G197" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1055, 265, 46, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1191, 265, 46, null, null, 2);</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <f t="shared" si="13"/>
-        <v>1056</v>
+        <v>1192</v>
       </c>
       <c r="B198" s="4">
         <f>B197</f>
@@ -30536,13 +30536,13 @@
       </c>
       <c r="G198" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1056, 265, 46, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1192, 265, 46, null, null, 1);</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <f t="shared" si="13"/>
-        <v>1057</v>
+        <v>1193</v>
       </c>
       <c r="B199" s="4">
         <f t="shared" ref="B199:B200" si="17">B197</f>
@@ -30562,13 +30562,13 @@
       </c>
       <c r="G199" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1057, 265, 32, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1193, 265, 32, null, null, 2);</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <f t="shared" si="13"/>
-        <v>1058</v>
+        <v>1194</v>
       </c>
       <c r="B200" s="4">
         <f t="shared" si="17"/>
@@ -30588,13 +30588,13 @@
       </c>
       <c r="G200" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1058, 265, 32, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1194, 265, 32, null, null, 1);</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <f t="shared" si="13"/>
-        <v>1059</v>
+        <v>1195</v>
       </c>
       <c r="B201" s="4">
         <f>B197+1</f>
@@ -30614,13 +30614,13 @@
       </c>
       <c r="G201" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1059, 266, 43, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1195, 266, 43, null, null, 2);</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <f t="shared" si="13"/>
-        <v>1060</v>
+        <v>1196</v>
       </c>
       <c r="B202" s="4">
         <f>B201</f>
@@ -30640,13 +30640,13 @@
       </c>
       <c r="G202" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1060, 266, 43, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1196, 266, 43, null, null, 1);</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <f t="shared" si="13"/>
-        <v>1061</v>
+        <v>1197</v>
       </c>
       <c r="B203" s="4">
         <f t="shared" ref="B203:B204" si="18">B201</f>
@@ -30666,13 +30666,13 @@
       </c>
       <c r="G203" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1061, 266, 36, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1197, 266, 36, null, null, 2);</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <f t="shared" si="13"/>
-        <v>1062</v>
+        <v>1198</v>
       </c>
       <c r="B204" s="4">
         <f t="shared" si="18"/>
@@ -30692,13 +30692,13 @@
       </c>
       <c r="G204" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1062, 266, 36, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1198, 266, 36, null, null, 1);</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
         <f t="shared" si="13"/>
-        <v>1063</v>
+        <v>1199</v>
       </c>
       <c r="B205" s="4">
         <f>B201+1</f>
@@ -30718,13 +30718,13 @@
       </c>
       <c r="G205" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1063, 267, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1199, 267, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <f t="shared" si="13"/>
-        <v>1064</v>
+        <v>1200</v>
       </c>
       <c r="B206" s="4">
         <f>B205</f>
@@ -30744,13 +30744,13 @@
       </c>
       <c r="G206" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1064, 267, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1200, 267, 351, null, null, 1);</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <f t="shared" si="13"/>
-        <v>1065</v>
+        <v>1201</v>
       </c>
       <c r="B207" s="4">
         <f t="shared" ref="B207:B208" si="19">B205</f>
@@ -30770,13 +30770,13 @@
       </c>
       <c r="G207" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1065, 267, 354, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1201, 267, 354, null, null, 2);</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
         <f t="shared" si="13"/>
-        <v>1066</v>
+        <v>1202</v>
       </c>
       <c r="B208" s="4">
         <f t="shared" si="19"/>
@@ -30796,13 +30796,13 @@
       </c>
       <c r="G208" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1066, 267, 354, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1202, 267, 354, null, null, 1);</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <f t="shared" si="13"/>
-        <v>1067</v>
+        <v>1203</v>
       </c>
       <c r="B209" s="4">
         <f>B205+1</f>
@@ -30822,13 +30822,13 @@
       </c>
       <c r="G209" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1067, 268, 354, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1203, 268, 354, null, null, 2);</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <f t="shared" si="13"/>
-        <v>1068</v>
+        <v>1204</v>
       </c>
       <c r="B210" s="4">
         <f>B209</f>
@@ -30848,13 +30848,13 @@
       </c>
       <c r="G210" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1068, 268, 354, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1204, 268, 354, null, null, 1);</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="4">
         <f t="shared" ref="A211:A274" si="20">A210+1</f>
-        <v>1069</v>
+        <v>1205</v>
       </c>
       <c r="B211" s="4">
         <f t="shared" ref="B211:B212" si="21">B209</f>
@@ -30874,13 +30874,13 @@
       </c>
       <c r="G211" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1069, 268, 36, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1205, 268, 36, null, null, 2);</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
         <f t="shared" si="20"/>
-        <v>1070</v>
+        <v>1206</v>
       </c>
       <c r="B212" s="4">
         <f t="shared" si="21"/>
@@ -30900,13 +30900,13 @@
       </c>
       <c r="G212" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1070, 268, 36, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1206, 268, 36, null, null, 1);</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="4">
         <f t="shared" si="20"/>
-        <v>1071</v>
+        <v>1207</v>
       </c>
       <c r="B213" s="4">
         <f>B209+1</f>
@@ -30926,13 +30926,13 @@
       </c>
       <c r="G213" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1071, 269, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1207, 269, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
         <f t="shared" si="20"/>
-        <v>1072</v>
+        <v>1208</v>
       </c>
       <c r="B214" s="4">
         <f>B213</f>
@@ -30952,13 +30952,13 @@
       </c>
       <c r="G214" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1072, 269, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1208, 269, 351, null, null, 1);</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="4">
         <f t="shared" si="20"/>
-        <v>1073</v>
+        <v>1209</v>
       </c>
       <c r="B215" s="4">
         <f t="shared" ref="B215:B216" si="22">B213</f>
@@ -30978,13 +30978,13 @@
       </c>
       <c r="G215" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1073, 269, 43, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1209, 269, 43, null, null, 2);</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
         <f t="shared" si="20"/>
-        <v>1074</v>
+        <v>1210</v>
       </c>
       <c r="B216" s="4">
         <f t="shared" si="22"/>
@@ -31004,13 +31004,13 @@
       </c>
       <c r="G216" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1074, 269, 43, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1210, 269, 43, null, null, 1);</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="4">
         <f t="shared" si="20"/>
-        <v>1075</v>
+        <v>1211</v>
       </c>
       <c r="B217" s="4">
         <f>B213+1</f>
@@ -31030,13 +31030,13 @@
       </c>
       <c r="G217" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1075, 270, 354, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1211, 270, 354, null, null, 2);</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <f t="shared" si="20"/>
-        <v>1076</v>
+        <v>1212</v>
       </c>
       <c r="B218" s="4">
         <f>B217</f>
@@ -31056,13 +31056,13 @@
       </c>
       <c r="G218" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1076, 270, 354, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1212, 270, 354, null, null, 1);</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
         <f t="shared" si="20"/>
-        <v>1077</v>
+        <v>1213</v>
       </c>
       <c r="B219" s="4">
         <f t="shared" ref="B219:B220" si="23">B217</f>
@@ -31082,13 +31082,13 @@
       </c>
       <c r="G219" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1077, 270, 43, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1213, 270, 43, null, null, 2);</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
         <f t="shared" si="20"/>
-        <v>1078</v>
+        <v>1214</v>
       </c>
       <c r="B220" s="4">
         <f t="shared" si="23"/>
@@ -31108,13 +31108,13 @@
       </c>
       <c r="G220" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1078, 270, 43, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1214, 270, 43, null, null, 1);</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
         <f t="shared" si="20"/>
-        <v>1079</v>
+        <v>1215</v>
       </c>
       <c r="B221" s="4">
         <f>B217+1</f>
@@ -31134,13 +31134,13 @@
       </c>
       <c r="G221" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1079, 271, 36, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1215, 271, 36, null, null, 2);</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="4">
         <f t="shared" si="20"/>
-        <v>1080</v>
+        <v>1216</v>
       </c>
       <c r="B222" s="4">
         <f>B221</f>
@@ -31160,13 +31160,13 @@
       </c>
       <c r="G222" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1080, 271, 36, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1216, 271, 36, null, null, 1);</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="4">
         <f t="shared" si="20"/>
-        <v>1081</v>
+        <v>1217</v>
       </c>
       <c r="B223" s="4">
         <f t="shared" ref="B223:B224" si="24">B221</f>
@@ -31186,13 +31186,13 @@
       </c>
       <c r="G223" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1081, 271, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1217, 271, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="4">
         <f t="shared" si="20"/>
-        <v>1082</v>
+        <v>1218</v>
       </c>
       <c r="B224" s="4">
         <f t="shared" si="24"/>
@@ -31212,13 +31212,13 @@
       </c>
       <c r="G224" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1082, 271, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1218, 271, 351, null, null, 1);</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="4">
         <f t="shared" si="20"/>
-        <v>1083</v>
+        <v>1219</v>
       </c>
       <c r="B225" s="4">
         <f>B221+1</f>
@@ -31238,13 +31238,13 @@
       </c>
       <c r="G225" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1083, 272, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1219, 272, null, null, null, 2);</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="4">
         <f t="shared" si="20"/>
-        <v>1084</v>
+        <v>1220</v>
       </c>
       <c r="B226" s="4">
         <f>B225</f>
@@ -31264,13 +31264,13 @@
       </c>
       <c r="G226" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1084, 272, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1220, 272, null, null, null, 1);</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="4">
         <f t="shared" si="20"/>
-        <v>1085</v>
+        <v>1221</v>
       </c>
       <c r="B227" s="4">
         <f t="shared" ref="B227:B228" si="25">B225</f>
@@ -31290,13 +31290,13 @@
       </c>
       <c r="G227" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1085, 272, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1221, 272, null, null, null, 2);</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="4">
         <f t="shared" si="20"/>
-        <v>1086</v>
+        <v>1222</v>
       </c>
       <c r="B228" s="4">
         <f t="shared" si="25"/>
@@ -31316,13 +31316,13 @@
       </c>
       <c r="G228" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1086, 272, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1222, 272, null, null, null, 1);</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="4">
         <f t="shared" si="20"/>
-        <v>1087</v>
+        <v>1223</v>
       </c>
       <c r="B229" s="4">
         <f>B225+1</f>
@@ -31342,13 +31342,13 @@
       </c>
       <c r="G229" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1087, 273, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1223, 273, null, null, null, 2);</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="4">
         <f t="shared" si="20"/>
-        <v>1088</v>
+        <v>1224</v>
       </c>
       <c r="B230" s="4">
         <f>B229</f>
@@ -31368,13 +31368,13 @@
       </c>
       <c r="G230" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1088, 273, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1224, 273, null, null, null, 1);</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="4">
         <f t="shared" si="20"/>
-        <v>1089</v>
+        <v>1225</v>
       </c>
       <c r="B231" s="4">
         <f t="shared" ref="B231:B232" si="26">B229</f>
@@ -31394,13 +31394,13 @@
       </c>
       <c r="G231" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1089, 273, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1225, 273, null, null, null, 2);</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="4">
         <f t="shared" si="20"/>
-        <v>1090</v>
+        <v>1226</v>
       </c>
       <c r="B232" s="4">
         <f t="shared" si="26"/>
@@ -31420,13 +31420,13 @@
       </c>
       <c r="G232" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1090, 273, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1226, 273, null, null, null, 1);</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="4">
         <f t="shared" si="20"/>
-        <v>1091</v>
+        <v>1227</v>
       </c>
       <c r="B233" s="4">
         <f>B229+1</f>
@@ -31446,13 +31446,13 @@
       </c>
       <c r="G233" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1091, 274, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1227, 274, null, null, null, 2);</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="4">
         <f t="shared" si="20"/>
-        <v>1092</v>
+        <v>1228</v>
       </c>
       <c r="B234" s="4">
         <f>B233</f>
@@ -31472,13 +31472,13 @@
       </c>
       <c r="G234" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1092, 274, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1228, 274, null, null, null, 1);</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="4">
         <f t="shared" si="20"/>
-        <v>1093</v>
+        <v>1229</v>
       </c>
       <c r="B235" s="4">
         <f t="shared" ref="B235:B236" si="27">B233</f>
@@ -31498,13 +31498,13 @@
       </c>
       <c r="G235" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1093, 274, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1229, 274, null, null, null, 2);</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="4">
         <f t="shared" si="20"/>
-        <v>1094</v>
+        <v>1230</v>
       </c>
       <c r="B236" s="4">
         <f t="shared" si="27"/>
@@ -31524,13 +31524,13 @@
       </c>
       <c r="G236" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1094, 274, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1230, 274, null, null, null, 1);</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="4">
         <f t="shared" si="20"/>
-        <v>1095</v>
+        <v>1231</v>
       </c>
       <c r="B237" s="4">
         <f>B233+1</f>
@@ -31550,13 +31550,13 @@
       </c>
       <c r="G237" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1095, 275, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1231, 275, null, null, null, 2);</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="4">
         <f t="shared" si="20"/>
-        <v>1096</v>
+        <v>1232</v>
       </c>
       <c r="B238" s="4">
         <f>B237</f>
@@ -31576,13 +31576,13 @@
       </c>
       <c r="G238" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1096, 275, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1232, 275, null, null, null, 1);</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="4">
         <f t="shared" si="20"/>
-        <v>1097</v>
+        <v>1233</v>
       </c>
       <c r="B239" s="4">
         <f t="shared" ref="B239:B240" si="28">B237</f>
@@ -31602,13 +31602,13 @@
       </c>
       <c r="G239" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1097, 275, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1233, 275, null, null, null, 2);</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="4">
         <f t="shared" si="20"/>
-        <v>1098</v>
+        <v>1234</v>
       </c>
       <c r="B240" s="4">
         <f t="shared" si="28"/>
@@ -31628,13 +31628,13 @@
       </c>
       <c r="G240" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1098, 275, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1234, 275, null, null, null, 1);</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="4">
         <f t="shared" si="20"/>
-        <v>1099</v>
+        <v>1235</v>
       </c>
       <c r="B241" s="4">
         <f>B237+1</f>
@@ -31654,13 +31654,13 @@
       </c>
       <c r="G241" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1099, 276, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1235, 276, null, null, null, 2);</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="4">
         <f t="shared" si="20"/>
-        <v>1100</v>
+        <v>1236</v>
       </c>
       <c r="B242" s="4">
         <f>B241</f>
@@ -31680,13 +31680,13 @@
       </c>
       <c r="G242" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1100, 276, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1236, 276, null, null, null, 1);</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="4">
         <f t="shared" si="20"/>
-        <v>1101</v>
+        <v>1237</v>
       </c>
       <c r="B243" s="4">
         <f t="shared" ref="B243:B244" si="29">B241</f>
@@ -31706,13 +31706,13 @@
       </c>
       <c r="G243" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1101, 276, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1237, 276, null, null, null, 2);</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="4">
         <f t="shared" si="20"/>
-        <v>1102</v>
+        <v>1238</v>
       </c>
       <c r="B244" s="4">
         <f t="shared" si="29"/>
@@ -31732,13 +31732,13 @@
       </c>
       <c r="G244" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1102, 276, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1238, 276, null, null, null, 1);</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="4">
         <f t="shared" si="20"/>
-        <v>1103</v>
+        <v>1239</v>
       </c>
       <c r="B245" s="4">
         <f>B241+1</f>
@@ -31758,13 +31758,13 @@
       </c>
       <c r="G245" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1103, 277, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1239, 277, null, null, null, 2);</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246" s="4">
         <f t="shared" si="20"/>
-        <v>1104</v>
+        <v>1240</v>
       </c>
       <c r="B246" s="4">
         <f>B245</f>
@@ -31784,13 +31784,13 @@
       </c>
       <c r="G246" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1104, 277, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1240, 277, null, null, null, 1);</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="4">
         <f t="shared" si="20"/>
-        <v>1105</v>
+        <v>1241</v>
       </c>
       <c r="B247" s="4">
         <f t="shared" ref="B247:B248" si="30">B245</f>
@@ -31810,13 +31810,13 @@
       </c>
       <c r="G247" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1105, 277, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1241, 277, null, null, null, 2);</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248" s="4">
         <f t="shared" si="20"/>
-        <v>1106</v>
+        <v>1242</v>
       </c>
       <c r="B248" s="4">
         <f t="shared" si="30"/>
@@ -31836,13 +31836,13 @@
       </c>
       <c r="G248" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1106, 277, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1242, 277, null, null, null, 1);</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249" s="4">
         <f t="shared" si="20"/>
-        <v>1107</v>
+        <v>1243</v>
       </c>
       <c r="B249" s="4">
         <f>B245+1</f>
@@ -31862,13 +31862,13 @@
       </c>
       <c r="G249" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1107, 278, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1243, 278, null, null, null, 2);</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250" s="4">
         <f t="shared" si="20"/>
-        <v>1108</v>
+        <v>1244</v>
       </c>
       <c r="B250" s="4">
         <f>B249</f>
@@ -31888,13 +31888,13 @@
       </c>
       <c r="G250" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1108, 278, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1244, 278, null, null, null, 1);</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251" s="4">
         <f t="shared" si="20"/>
-        <v>1109</v>
+        <v>1245</v>
       </c>
       <c r="B251" s="4">
         <f t="shared" ref="B251:B252" si="31">B249</f>
@@ -31914,13 +31914,13 @@
       </c>
       <c r="G251" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1109, 278, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1245, 278, null, null, null, 2);</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252" s="4">
         <f t="shared" si="20"/>
-        <v>1110</v>
+        <v>1246</v>
       </c>
       <c r="B252" s="4">
         <f t="shared" si="31"/>
@@ -31940,13 +31940,13 @@
       </c>
       <c r="G252" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1110, 278, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1246, 278, null, null, null, 1);</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253" s="4">
         <f t="shared" si="20"/>
-        <v>1111</v>
+        <v>1247</v>
       </c>
       <c r="B253" s="4">
         <f>B249+1</f>
@@ -31966,13 +31966,13 @@
       </c>
       <c r="G253" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1111, 279, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1247, 279, null, null, null, 2);</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254" s="4">
         <f t="shared" si="20"/>
-        <v>1112</v>
+        <v>1248</v>
       </c>
       <c r="B254" s="4">
         <f>B253</f>
@@ -31992,13 +31992,13 @@
       </c>
       <c r="G254" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1112, 279, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1248, 279, null, null, null, 1);</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255" s="4">
         <f t="shared" si="20"/>
-        <v>1113</v>
+        <v>1249</v>
       </c>
       <c r="B255" s="4">
         <f t="shared" ref="B255:B256" si="32">B253</f>
@@ -32018,13 +32018,13 @@
       </c>
       <c r="G255" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1113, 279, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1249, 279, null, null, null, 2);</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256" s="4">
         <f t="shared" si="20"/>
-        <v>1114</v>
+        <v>1250</v>
       </c>
       <c r="B256" s="4">
         <f t="shared" si="32"/>
@@ -32044,13 +32044,13 @@
       </c>
       <c r="G256" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1114, 279, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1250, 279, null, null, null, 1);</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="4">
         <f t="shared" si="20"/>
-        <v>1115</v>
+        <v>1251</v>
       </c>
       <c r="B257" s="4">
         <f>B253+1</f>
@@ -32070,13 +32070,13 @@
       </c>
       <c r="G257" s="4" t="str">
         <f t="shared" ref="G257:G284" si="33">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A257 &amp; ", " &amp; B257 &amp; ", " &amp; C257 &amp; ", " &amp; D257 &amp; ", " &amp; E257 &amp; ", " &amp; F257 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1115, 280, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1251, 280, null, null, null, 2);</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="4">
         <f t="shared" si="20"/>
-        <v>1116</v>
+        <v>1252</v>
       </c>
       <c r="B258" s="4">
         <f>B257</f>
@@ -32096,13 +32096,13 @@
       </c>
       <c r="G258" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1116, 280, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1252, 280, null, null, null, 1);</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="4">
         <f t="shared" si="20"/>
-        <v>1117</v>
+        <v>1253</v>
       </c>
       <c r="B259" s="4">
         <f t="shared" ref="B259:B260" si="34">B257</f>
@@ -32122,13 +32122,13 @@
       </c>
       <c r="G259" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1117, 280, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1253, 280, null, null, null, 2);</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260" s="4">
         <f t="shared" si="20"/>
-        <v>1118</v>
+        <v>1254</v>
       </c>
       <c r="B260" s="4">
         <f t="shared" si="34"/>
@@ -32148,13 +32148,13 @@
       </c>
       <c r="G260" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1118, 280, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1254, 280, null, null, null, 1);</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="4">
         <f t="shared" si="20"/>
-        <v>1119</v>
+        <v>1255</v>
       </c>
       <c r="B261" s="4">
         <f>B257+1</f>
@@ -32174,13 +32174,13 @@
       </c>
       <c r="G261" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1119, 281, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1255, 281, null, null, null, 2);</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="4">
         <f t="shared" si="20"/>
-        <v>1120</v>
+        <v>1256</v>
       </c>
       <c r="B262" s="4">
         <f>B261</f>
@@ -32200,13 +32200,13 @@
       </c>
       <c r="G262" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1120, 281, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1256, 281, null, null, null, 1);</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263" s="4">
         <f t="shared" si="20"/>
-        <v>1121</v>
+        <v>1257</v>
       </c>
       <c r="B263" s="4">
         <f t="shared" ref="B263:B264" si="35">B261</f>
@@ -32226,13 +32226,13 @@
       </c>
       <c r="G263" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1121, 281, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1257, 281, null, null, null, 2);</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264" s="4">
         <f t="shared" si="20"/>
-        <v>1122</v>
+        <v>1258</v>
       </c>
       <c r="B264" s="4">
         <f t="shared" si="35"/>
@@ -32252,13 +32252,13 @@
       </c>
       <c r="G264" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1122, 281, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1258, 281, null, null, null, 1);</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265" s="4">
         <f t="shared" si="20"/>
-        <v>1123</v>
+        <v>1259</v>
       </c>
       <c r="B265" s="4">
         <f>B261+1</f>
@@ -32278,13 +32278,13 @@
       </c>
       <c r="G265" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1123, 282, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1259, 282, null, null, null, 2);</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266" s="4">
         <f t="shared" si="20"/>
-        <v>1124</v>
+        <v>1260</v>
       </c>
       <c r="B266" s="4">
         <f>B265</f>
@@ -32304,13 +32304,13 @@
       </c>
       <c r="G266" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1124, 282, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1260, 282, null, null, null, 1);</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267" s="4">
         <f t="shared" si="20"/>
-        <v>1125</v>
+        <v>1261</v>
       </c>
       <c r="B267" s="4">
         <f t="shared" ref="B267:B268" si="36">B265</f>
@@ -32330,13 +32330,13 @@
       </c>
       <c r="G267" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1125, 282, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1261, 282, null, null, null, 2);</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268" s="4">
         <f t="shared" si="20"/>
-        <v>1126</v>
+        <v>1262</v>
       </c>
       <c r="B268" s="4">
         <f t="shared" si="36"/>
@@ -32356,13 +32356,13 @@
       </c>
       <c r="G268" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1126, 282, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1262, 282, null, null, null, 1);</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269" s="4">
         <f t="shared" si="20"/>
-        <v>1127</v>
+        <v>1263</v>
       </c>
       <c r="B269" s="4">
         <f>B265+1</f>
@@ -32382,13 +32382,13 @@
       </c>
       <c r="G269" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1127, 283, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1263, 283, null, null, null, 2);</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270" s="4">
         <f t="shared" si="20"/>
-        <v>1128</v>
+        <v>1264</v>
       </c>
       <c r="B270" s="4">
         <f>B269</f>
@@ -32408,13 +32408,13 @@
       </c>
       <c r="G270" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1128, 283, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1264, 283, null, null, null, 1);</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271" s="4">
         <f t="shared" si="20"/>
-        <v>1129</v>
+        <v>1265</v>
       </c>
       <c r="B271" s="4">
         <f t="shared" ref="B271:B272" si="37">B269</f>
@@ -32434,13 +32434,13 @@
       </c>
       <c r="G271" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1129, 283, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1265, 283, null, null, null, 2);</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="4">
         <f t="shared" si="20"/>
-        <v>1130</v>
+        <v>1266</v>
       </c>
       <c r="B272" s="4">
         <f t="shared" si="37"/>
@@ -32460,13 +32460,13 @@
       </c>
       <c r="G272" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1130, 283, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1266, 283, null, null, null, 1);</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="4">
         <f t="shared" si="20"/>
-        <v>1131</v>
+        <v>1267</v>
       </c>
       <c r="B273" s="4">
         <f>B269+1</f>
@@ -32486,13 +32486,13 @@
       </c>
       <c r="G273" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1131, 284, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1267, 284, null, null, null, 2);</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="4">
         <f t="shared" si="20"/>
-        <v>1132</v>
+        <v>1268</v>
       </c>
       <c r="B274" s="4">
         <f>B273</f>
@@ -32512,13 +32512,13 @@
       </c>
       <c r="G274" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1132, 284, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1268, 284, null, null, null, 1);</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="4">
         <f t="shared" ref="A275:A284" si="38">A274+1</f>
-        <v>1133</v>
+        <v>1269</v>
       </c>
       <c r="B275" s="4">
         <f t="shared" ref="B275:B276" si="39">B273</f>
@@ -32538,13 +32538,13 @@
       </c>
       <c r="G275" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1133, 284, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1269, 284, null, null, null, 2);</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="4">
         <f t="shared" si="38"/>
-        <v>1134</v>
+        <v>1270</v>
       </c>
       <c r="B276" s="4">
         <f t="shared" si="39"/>
@@ -32564,13 +32564,13 @@
       </c>
       <c r="G276" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1134, 284, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1270, 284, null, null, null, 1);</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="4">
         <f t="shared" si="38"/>
-        <v>1135</v>
+        <v>1271</v>
       </c>
       <c r="B277" s="4">
         <f>B273+1</f>
@@ -32590,13 +32590,13 @@
       </c>
       <c r="G277" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1135, 285, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1271, 285, null, null, null, 2);</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="4">
         <f t="shared" si="38"/>
-        <v>1136</v>
+        <v>1272</v>
       </c>
       <c r="B278" s="4">
         <f>B277</f>
@@ -32616,13 +32616,13 @@
       </c>
       <c r="G278" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1136, 285, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1272, 285, null, null, null, 1);</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="4">
         <f t="shared" si="38"/>
-        <v>1137</v>
+        <v>1273</v>
       </c>
       <c r="B279" s="4">
         <f t="shared" ref="B279:B280" si="40">B277</f>
@@ -32642,13 +32642,13 @@
       </c>
       <c r="G279" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1137, 285, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1273, 285, null, null, null, 2);</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="4">
         <f t="shared" si="38"/>
-        <v>1138</v>
+        <v>1274</v>
       </c>
       <c r="B280" s="4">
         <f t="shared" si="40"/>
@@ -32668,13 +32668,13 @@
       </c>
       <c r="G280" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1138, 285, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1274, 285, null, null, null, 1);</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="4">
         <f t="shared" si="38"/>
-        <v>1139</v>
+        <v>1275</v>
       </c>
       <c r="B281" s="4">
         <f>B277+1</f>
@@ -32694,13 +32694,13 @@
       </c>
       <c r="G281" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1139, 286, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1275, 286, null, null, null, 2);</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="4">
         <f t="shared" si="38"/>
-        <v>1140</v>
+        <v>1276</v>
       </c>
       <c r="B282" s="4">
         <f>B281</f>
@@ -32720,13 +32720,13 @@
       </c>
       <c r="G282" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1140, 286, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1276, 286, null, null, null, 1);</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="4">
         <f t="shared" si="38"/>
-        <v>1141</v>
+        <v>1277</v>
       </c>
       <c r="B283" s="4">
         <f t="shared" ref="B283:B284" si="41">B281</f>
@@ -32746,13 +32746,13 @@
       </c>
       <c r="G283" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1141, 286, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1277, 286, null, null, null, 2);</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="4">
         <f t="shared" si="38"/>
-        <v>1142</v>
+        <v>1278</v>
       </c>
       <c r="B284" s="4">
         <f t="shared" si="41"/>
@@ -32772,7 +32772,7 @@
       </c>
       <c r="G284" s="4" t="str">
         <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1142, 286, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1278, 286, null, null, null, 1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Group A and B Eurocopa and HTML review
Group A and B Eurocopa and HTML review
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -27416,18 +27416,18 @@
       <c r="C81" s="3">
         <v>33</v>
       </c>
-      <c r="D81" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>17</v>
+      <c r="D81" s="3">
+        <v>2</v>
+      </c>
+      <c r="E81" s="3">
+        <v>3</v>
       </c>
       <c r="F81" s="3">
         <v>2</v>
       </c>
       <c r="G81" s="3" t="str">
         <f t="shared" ref="G81:G144" si="10">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A81 &amp; ", " &amp; B81 &amp; ", " &amp; C81 &amp; ", " &amp; D81 &amp; ", " &amp; E81 &amp; ", " &amp; F81 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1075, 236, 33, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1075, 236, 33, 2, 3, 2);</v>
       </c>
       <c r="H81" s="4"/>
     </row>
@@ -27443,18 +27443,18 @@
       <c r="C82" s="3">
         <v>33</v>
       </c>
-      <c r="D82" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>17</v>
+      <c r="D82" s="3">
+        <v>0</v>
+      </c>
+      <c r="E82" s="3">
+        <v>0</v>
       </c>
       <c r="F82" s="3">
         <v>1</v>
       </c>
       <c r="G82" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1076, 236, 33, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1076, 236, 33, 0, 0, 1);</v>
       </c>
       <c r="H82" s="4"/>
     </row>
@@ -27470,18 +27470,18 @@
       <c r="C83" s="3">
         <v>40</v>
       </c>
-      <c r="D83" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>17</v>
+      <c r="D83" s="3">
+        <v>1</v>
+      </c>
+      <c r="E83" s="3">
+        <v>0</v>
       </c>
       <c r="F83" s="3">
         <v>2</v>
       </c>
       <c r="G83" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1077, 236, 40, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1077, 236, 40, 1, 0, 2);</v>
       </c>
       <c r="H83" s="4"/>
     </row>
@@ -27497,18 +27497,18 @@
       <c r="C84" s="3">
         <v>40</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E84" s="3" t="s">
-        <v>17</v>
+      <c r="D84" s="3">
+        <v>0</v>
+      </c>
+      <c r="E84" s="3">
+        <v>0</v>
       </c>
       <c r="F84" s="3">
         <v>1</v>
       </c>
       <c r="G84" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1078, 236, 40, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1078, 236, 40, 0, 0, 1);</v>
       </c>
       <c r="H84" s="4"/>
     </row>
@@ -27524,18 +27524,18 @@
       <c r="C85" s="4">
         <v>355</v>
       </c>
-      <c r="D85" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>17</v>
+      <c r="D85" s="4">
+        <v>0</v>
+      </c>
+      <c r="E85" s="4">
+        <v>0</v>
       </c>
       <c r="F85" s="4">
         <v>2</v>
       </c>
       <c r="G85" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1079, 237, 355, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1079, 237, 355, 0, 0, 2);</v>
       </c>
       <c r="H85" s="4"/>
     </row>
@@ -27551,18 +27551,18 @@
       <c r="C86" s="4">
         <v>355</v>
       </c>
-      <c r="D86" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>17</v>
+      <c r="D86" s="4">
+        <v>0</v>
+      </c>
+      <c r="E86" s="4">
+        <v>0</v>
       </c>
       <c r="F86" s="4">
         <v>1</v>
       </c>
       <c r="G86" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1080, 237, 355, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1080, 237, 355, 0, 0, 1);</v>
       </c>
       <c r="H86" s="4"/>
     </row>
@@ -27578,18 +27578,18 @@
       <c r="C87" s="4">
         <v>41</v>
       </c>
-      <c r="D87" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>17</v>
+      <c r="D87" s="4">
+        <v>1</v>
+      </c>
+      <c r="E87" s="4">
+        <v>3</v>
       </c>
       <c r="F87" s="4">
         <v>2</v>
       </c>
       <c r="G87" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1081, 237, 41, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1081, 237, 41, 1, 3, 2);</v>
       </c>
       <c r="H87" s="4"/>
     </row>
@@ -27605,18 +27605,18 @@
       <c r="C88" s="4">
         <v>41</v>
       </c>
-      <c r="D88" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E88" s="4" t="s">
-        <v>17</v>
+      <c r="D88" s="4">
+        <v>1</v>
+      </c>
+      <c r="E88" s="4">
+        <v>0</v>
       </c>
       <c r="F88" s="4">
         <v>1</v>
       </c>
       <c r="G88" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1082, 237, 41, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1082, 237, 41, 1, 0, 1);</v>
       </c>
       <c r="H88" s="4"/>
     </row>
@@ -28064,18 +28064,18 @@
       <c r="C105" s="3">
         <v>4429</v>
       </c>
-      <c r="D105" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>17</v>
+      <c r="D105" s="3">
+        <v>2</v>
+      </c>
+      <c r="E105" s="3">
+        <v>3</v>
       </c>
       <c r="F105" s="3">
         <v>2</v>
       </c>
       <c r="G105" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1099, 242, 4429, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1099, 242, 4429, 2, 3, 2);</v>
       </c>
       <c r="H105" s="4"/>
     </row>
@@ -28091,18 +28091,18 @@
       <c r="C106" s="3">
         <v>4429</v>
       </c>
-      <c r="D106" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>17</v>
+      <c r="D106" s="3">
+        <v>1</v>
+      </c>
+      <c r="E106" s="3">
+        <v>0</v>
       </c>
       <c r="F106" s="3">
         <v>1</v>
       </c>
       <c r="G106" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1100, 242, 4429, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1100, 242, 4429, 1, 0, 1);</v>
       </c>
       <c r="H106" s="4"/>
     </row>
@@ -28118,18 +28118,18 @@
       <c r="C107" s="3">
         <v>421</v>
       </c>
-      <c r="D107" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>17</v>
+      <c r="D107" s="3">
+        <v>1</v>
+      </c>
+      <c r="E107" s="3">
+        <v>0</v>
       </c>
       <c r="F107" s="3">
         <v>2</v>
       </c>
       <c r="G107" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1101, 242, 421, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1101, 242, 421, 1, 0, 2);</v>
       </c>
       <c r="H107" s="4"/>
     </row>
@@ -28145,18 +28145,18 @@
       <c r="C108" s="3">
         <v>421</v>
       </c>
-      <c r="D108" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>17</v>
+      <c r="D108" s="3">
+        <v>0</v>
+      </c>
+      <c r="E108" s="3">
+        <v>0</v>
       </c>
       <c r="F108" s="3">
         <v>1</v>
       </c>
       <c r="G108" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1102, 242, 421, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1102, 242, 421, 0, 0, 1);</v>
       </c>
       <c r="H108" s="4"/>
     </row>
@@ -28172,18 +28172,18 @@
       <c r="C109" s="4">
         <v>4420</v>
       </c>
-      <c r="D109" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E109" s="4" t="s">
-        <v>17</v>
+      <c r="D109" s="4">
+        <v>1</v>
+      </c>
+      <c r="E109" s="4">
+        <v>1</v>
       </c>
       <c r="F109" s="4">
         <v>2</v>
       </c>
       <c r="G109" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1103, 243, 4420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1103, 243, 4420, 1, 1, 2);</v>
       </c>
       <c r="H109" s="4"/>
     </row>
@@ -28199,18 +28199,18 @@
       <c r="C110" s="4">
         <v>4420</v>
       </c>
-      <c r="D110" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E110" s="4" t="s">
-        <v>17</v>
+      <c r="D110" s="4">
+        <v>0</v>
+      </c>
+      <c r="E110" s="4">
+        <v>0</v>
       </c>
       <c r="F110" s="4">
         <v>1</v>
       </c>
       <c r="G110" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1104, 243, 4420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1104, 243, 4420, 0, 0, 1);</v>
       </c>
       <c r="H110" s="4"/>
     </row>
@@ -28226,18 +28226,18 @@
       <c r="C111" s="4">
         <v>7</v>
       </c>
-      <c r="D111" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E111" s="4" t="s">
-        <v>17</v>
+      <c r="D111" s="4">
+        <v>1</v>
+      </c>
+      <c r="E111" s="4">
+        <v>1</v>
       </c>
       <c r="F111" s="4">
         <v>2</v>
       </c>
       <c r="G111" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1105, 243, 7, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1105, 243, 7, 1, 1, 2);</v>
       </c>
       <c r="H111" s="4"/>
     </row>
@@ -28253,18 +28253,18 @@
       <c r="C112" s="4">
         <v>7</v>
       </c>
-      <c r="D112" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E112" s="4" t="s">
-        <v>17</v>
+      <c r="D112" s="4">
+        <v>0</v>
+      </c>
+      <c r="E112" s="4">
+        <v>0</v>
       </c>
       <c r="F112" s="4">
         <v>1</v>
       </c>
       <c r="G112" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1106, 243, 7, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1106, 243, 7, 0, 0, 1);</v>
       </c>
       <c r="H112" s="4"/>
     </row>

</xml_diff>

<commit_message>
CSS + Day 3 Eurocopa + Date3 Group D Copa America
CSS + Day 3 Eurocopa + Date3 Group D Copa America
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -25496,7 +25496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J284"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="G129" sqref="G129:G136"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -28712,18 +28714,18 @@
       <c r="C129" s="3">
         <v>48</v>
       </c>
-      <c r="D129" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>17</v>
+      <c r="D129" s="3">
+        <v>1</v>
+      </c>
+      <c r="E129" s="3">
+        <v>3</v>
       </c>
       <c r="F129" s="3">
         <v>2</v>
       </c>
       <c r="G129" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1123, 248, 48, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1123, 248, 48, 1, 3, 2);</v>
       </c>
       <c r="H129" s="4"/>
     </row>
@@ -28739,18 +28741,18 @@
       <c r="C130" s="3">
         <v>48</v>
       </c>
-      <c r="D130" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E130" s="3" t="s">
-        <v>17</v>
+      <c r="D130" s="3">
+        <v>0</v>
+      </c>
+      <c r="E130" s="3">
+        <v>0</v>
       </c>
       <c r="F130" s="3">
         <v>1</v>
       </c>
       <c r="G130" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1124, 248, 48, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1124, 248, 48, 0, 0, 1);</v>
       </c>
       <c r="H130" s="4"/>
     </row>
@@ -28766,18 +28768,18 @@
       <c r="C131" s="3">
         <v>4428</v>
       </c>
-      <c r="D131" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E131" s="3" t="s">
-        <v>17</v>
+      <c r="D131" s="3">
+        <v>0</v>
+      </c>
+      <c r="E131" s="3">
+        <v>0</v>
       </c>
       <c r="F131" s="3">
         <v>2</v>
       </c>
       <c r="G131" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1125, 248, 4428, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1125, 248, 4428, 0, 0, 2);</v>
       </c>
       <c r="H131" s="4"/>
     </row>
@@ -28793,18 +28795,18 @@
       <c r="C132" s="3">
         <v>4428</v>
       </c>
-      <c r="D132" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E132" s="3" t="s">
-        <v>17</v>
+      <c r="D132" s="3">
+        <v>0</v>
+      </c>
+      <c r="E132" s="3">
+        <v>0</v>
       </c>
       <c r="F132" s="3">
         <v>1</v>
       </c>
       <c r="G132" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1126, 248, 4428, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1126, 248, 4428, 0, 0, 1);</v>
       </c>
       <c r="H132" s="4"/>
     </row>
@@ -28820,18 +28822,18 @@
       <c r="C133" s="4">
         <v>49</v>
       </c>
-      <c r="D133" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E133" s="4" t="s">
-        <v>17</v>
+      <c r="D133" s="4">
+        <v>2</v>
+      </c>
+      <c r="E133" s="4">
+        <v>3</v>
       </c>
       <c r="F133" s="4">
         <v>2</v>
       </c>
       <c r="G133" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1127, 249, 49, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1127, 249, 49, 2, 3, 2);</v>
       </c>
       <c r="H133" s="4"/>
     </row>
@@ -28847,18 +28849,18 @@
       <c r="C134" s="4">
         <v>49</v>
       </c>
-      <c r="D134" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E134" s="4" t="s">
-        <v>17</v>
+      <c r="D134" s="4">
+        <v>1</v>
+      </c>
+      <c r="E134" s="4">
+        <v>0</v>
       </c>
       <c r="F134" s="4">
         <v>1</v>
       </c>
       <c r="G134" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1128, 249, 49, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1128, 249, 49, 1, 0, 1);</v>
       </c>
       <c r="H134" s="4"/>
     </row>
@@ -28874,18 +28876,18 @@
       <c r="C135" s="4">
         <v>380</v>
       </c>
-      <c r="D135" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E135" s="4" t="s">
-        <v>17</v>
+      <c r="D135" s="4">
+        <v>0</v>
+      </c>
+      <c r="E135" s="4">
+        <v>0</v>
       </c>
       <c r="F135" s="4">
         <v>2</v>
       </c>
       <c r="G135" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1129, 249, 380, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1129, 249, 380, 0, 0, 2);</v>
       </c>
       <c r="H135" s="4"/>
     </row>
@@ -28901,18 +28903,18 @@
       <c r="C136" s="4">
         <v>380</v>
       </c>
-      <c r="D136" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E136" s="4" t="s">
-        <v>17</v>
+      <c r="D136" s="4">
+        <v>0</v>
+      </c>
+      <c r="E136" s="4">
+        <v>0</v>
       </c>
       <c r="F136" s="4">
         <v>1</v>
       </c>
       <c r="G136" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1130, 249, 380, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1130, 249, 380, 0, 0, 1);</v>
       </c>
       <c r="H136" s="4"/>
     </row>
@@ -29355,18 +29357,18 @@
       <c r="C153" s="3">
         <v>90</v>
       </c>
-      <c r="D153" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E153" s="3" t="s">
-        <v>17</v>
+      <c r="D153" s="3">
+        <v>0</v>
+      </c>
+      <c r="E153" s="3">
+        <v>0</v>
       </c>
       <c r="F153" s="3">
         <v>2</v>
       </c>
       <c r="G153" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1147, 254, 90, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1147, 254, 90, 0, 0, 2);</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -29381,18 +29383,18 @@
       <c r="C154" s="3">
         <v>90</v>
       </c>
-      <c r="D154" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>17</v>
+      <c r="D154" s="3">
+        <v>0</v>
+      </c>
+      <c r="E154" s="3">
+        <v>0</v>
       </c>
       <c r="F154" s="3">
         <v>1</v>
       </c>
       <c r="G154" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1148, 254, 90, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1148, 254, 90, 0, 0, 1);</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -29407,18 +29409,18 @@
       <c r="C155" s="3">
         <v>385</v>
       </c>
-      <c r="D155" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E155" s="3" t="s">
-        <v>17</v>
+      <c r="D155" s="3">
+        <v>1</v>
+      </c>
+      <c r="E155" s="3">
+        <v>3</v>
       </c>
       <c r="F155" s="3">
         <v>2</v>
       </c>
       <c r="G155" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1149, 254, 385, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1149, 254, 385, 1, 3, 2);</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -29433,18 +29435,18 @@
       <c r="C156" s="3">
         <v>385</v>
       </c>
-      <c r="D156" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E156" s="3" t="s">
-        <v>17</v>
+      <c r="D156" s="3">
+        <v>1</v>
+      </c>
+      <c r="E156" s="3">
+        <v>0</v>
       </c>
       <c r="F156" s="3">
         <v>1</v>
       </c>
       <c r="G156" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1150, 254, 385, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1150, 254, 385, 1, 0, 1);</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Date 3 Group C
Date 3 Group C
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -25496,9 +25496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="G129" sqref="G129:G136"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29461,18 +29459,18 @@
       <c r="C157" s="4">
         <v>34</v>
       </c>
-      <c r="D157" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E157" s="4" t="s">
-        <v>17</v>
+      <c r="D157" s="4">
+        <v>1</v>
+      </c>
+      <c r="E157" s="4">
+        <v>3</v>
       </c>
       <c r="F157" s="4">
         <v>2</v>
       </c>
       <c r="G157" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1151, 255, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1151, 255, 34, 1, 3, 2);</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -29487,18 +29485,18 @@
       <c r="C158" s="4">
         <v>34</v>
       </c>
-      <c r="D158" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E158" s="4" t="s">
-        <v>17</v>
+      <c r="D158" s="4">
+        <v>0</v>
+      </c>
+      <c r="E158" s="4">
+        <v>0</v>
       </c>
       <c r="F158" s="4">
         <v>1</v>
       </c>
       <c r="G158" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1152, 255, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1152, 255, 34, 0, 0, 1);</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -29513,18 +29511,18 @@
       <c r="C159" s="4">
         <v>420</v>
       </c>
-      <c r="D159" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E159" s="4" t="s">
-        <v>17</v>
+      <c r="D159" s="4">
+        <v>0</v>
+      </c>
+      <c r="E159" s="4">
+        <v>0</v>
       </c>
       <c r="F159" s="4">
         <v>2</v>
       </c>
       <c r="G159" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1153, 255, 420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1153, 255, 420, 0, 0, 2);</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -29539,18 +29537,18 @@
       <c r="C160" s="4">
         <v>420</v>
       </c>
-      <c r="D160" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E160" s="4" t="s">
-        <v>17</v>
+      <c r="D160" s="4">
+        <v>0</v>
+      </c>
+      <c r="E160" s="4">
+        <v>0</v>
       </c>
       <c r="F160" s="4">
         <v>1</v>
       </c>
       <c r="G160" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1154, 255, 420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1154, 255, 420, 0, 0, 1);</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -29981,18 +29979,18 @@
       <c r="C177" s="3">
         <v>353</v>
       </c>
-      <c r="D177" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E177" s="3" t="s">
-        <v>17</v>
+      <c r="D177" s="3">
+        <v>1</v>
+      </c>
+      <c r="E177" s="3">
+        <v>1</v>
       </c>
       <c r="F177" s="3">
         <v>2</v>
       </c>
       <c r="G177" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1171, 260, 353, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1171, 260, 353, 1, 1, 2);</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -30007,18 +30005,18 @@
       <c r="C178" s="3">
         <v>353</v>
       </c>
-      <c r="D178" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E178" s="3" t="s">
-        <v>17</v>
+      <c r="D178" s="3">
+        <v>0</v>
+      </c>
+      <c r="E178" s="3">
+        <v>0</v>
       </c>
       <c r="F178" s="3">
         <v>1</v>
       </c>
       <c r="G178" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1172, 260, 353, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1172, 260, 353, 0, 0, 1);</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -30033,18 +30031,18 @@
       <c r="C179" s="3">
         <v>46</v>
       </c>
-      <c r="D179" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E179" s="3" t="s">
-        <v>17</v>
+      <c r="D179" s="3">
+        <v>1</v>
+      </c>
+      <c r="E179" s="3">
+        <v>1</v>
       </c>
       <c r="F179" s="3">
         <v>2</v>
       </c>
       <c r="G179" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1173, 260, 46, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1173, 260, 46, 1, 1, 2);</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -30059,18 +30057,18 @@
       <c r="C180" s="3">
         <v>46</v>
       </c>
-      <c r="D180" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E180" s="3" t="s">
-        <v>17</v>
+      <c r="D180" s="3">
+        <v>0</v>
+      </c>
+      <c r="E180" s="3">
+        <v>0</v>
       </c>
       <c r="F180" s="3">
         <v>1</v>
       </c>
       <c r="G180" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1174, 260, 46, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1174, 260, 46, 0, 0, 1);</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -30085,18 +30083,18 @@
       <c r="C181" s="4">
         <v>32</v>
       </c>
-      <c r="D181" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E181" s="4" t="s">
-        <v>17</v>
+      <c r="D181" s="4">
+        <v>0</v>
+      </c>
+      <c r="E181" s="4">
+        <v>0</v>
       </c>
       <c r="F181" s="4">
         <v>2</v>
       </c>
       <c r="G181" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1175, 261, 32, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1175, 261, 32, 0, 0, 2);</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -30111,18 +30109,18 @@
       <c r="C182" s="4">
         <v>32</v>
       </c>
-      <c r="D182" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E182" s="4" t="s">
-        <v>17</v>
+      <c r="D182" s="4">
+        <v>0</v>
+      </c>
+      <c r="E182" s="4">
+        <v>0</v>
       </c>
       <c r="F182" s="4">
         <v>1</v>
       </c>
       <c r="G182" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1176, 261, 32, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1176, 261, 32, 0, 0, 1);</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
@@ -30137,18 +30135,18 @@
       <c r="C183" s="4">
         <v>39</v>
       </c>
-      <c r="D183" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E183" s="4" t="s">
-        <v>17</v>
+      <c r="D183" s="4">
+        <v>2</v>
+      </c>
+      <c r="E183" s="4">
+        <v>3</v>
       </c>
       <c r="F183" s="4">
         <v>2</v>
       </c>
       <c r="G183" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1177, 261, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1177, 261, 39, 2, 3, 2);</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -30163,18 +30161,18 @@
       <c r="C184" s="4">
         <v>39</v>
       </c>
-      <c r="D184" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E184" s="4" t="s">
-        <v>17</v>
+      <c r="D184" s="4">
+        <v>1</v>
+      </c>
+      <c r="E184" s="4">
+        <v>0</v>
       </c>
       <c r="F184" s="4">
         <v>1</v>
       </c>
       <c r="G184" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1178, 261, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1178, 261, 39, 1, 0, 1);</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Date 1 Group F Eurocopa and CSS
Date 1 Group F Eurocopa and CSS
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -30603,18 +30603,18 @@
       <c r="C201" s="3">
         <v>43</v>
       </c>
-      <c r="D201" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E201" s="3" t="s">
-        <v>17</v>
+      <c r="D201" s="3">
+        <v>0</v>
+      </c>
+      <c r="E201" s="3">
+        <v>0</v>
       </c>
       <c r="F201" s="3">
         <v>2</v>
       </c>
       <c r="G201" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1195, 266, 43, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1195, 266, 43, 0, 0, 2);</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -30629,18 +30629,18 @@
       <c r="C202" s="3">
         <v>43</v>
       </c>
-      <c r="D202" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E202" s="3" t="s">
-        <v>17</v>
+      <c r="D202" s="3">
+        <v>0</v>
+      </c>
+      <c r="E202" s="3">
+        <v>0</v>
       </c>
       <c r="F202" s="3">
         <v>1</v>
       </c>
       <c r="G202" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1196, 266, 43, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1196, 266, 43, 0, 0, 1);</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -30655,18 +30655,18 @@
       <c r="C203" s="3">
         <v>36</v>
       </c>
-      <c r="D203" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E203" s="3" t="s">
-        <v>17</v>
+      <c r="D203" s="3">
+        <v>2</v>
+      </c>
+      <c r="E203" s="3">
+        <v>3</v>
       </c>
       <c r="F203" s="3">
         <v>2</v>
       </c>
       <c r="G203" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1197, 266, 36, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1197, 266, 36, 2, 3, 2);</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -30681,18 +30681,18 @@
       <c r="C204" s="3">
         <v>36</v>
       </c>
-      <c r="D204" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E204" s="3" t="s">
-        <v>17</v>
+      <c r="D204" s="3">
+        <v>0</v>
+      </c>
+      <c r="E204" s="3">
+        <v>0</v>
       </c>
       <c r="F204" s="3">
         <v>1</v>
       </c>
       <c r="G204" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1198, 266, 36, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1198, 266, 36, 0, 0, 1);</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
@@ -30707,18 +30707,18 @@
       <c r="C205" s="4">
         <v>351</v>
       </c>
-      <c r="D205" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E205" s="4" t="s">
-        <v>17</v>
+      <c r="D205" s="4">
+        <v>1</v>
+      </c>
+      <c r="E205" s="4">
+        <v>1</v>
       </c>
       <c r="F205" s="4">
         <v>2</v>
       </c>
       <c r="G205" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1199, 267, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1199, 267, 351, 1, 1, 2);</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -30733,18 +30733,18 @@
       <c r="C206" s="4">
         <v>351</v>
       </c>
-      <c r="D206" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E206" s="4" t="s">
-        <v>17</v>
+      <c r="D206" s="4">
+        <v>1</v>
+      </c>
+      <c r="E206" s="4">
+        <v>0</v>
       </c>
       <c r="F206" s="4">
         <v>1</v>
       </c>
       <c r="G206" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1200, 267, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1200, 267, 351, 1, 0, 1);</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
@@ -30759,18 +30759,18 @@
       <c r="C207" s="4">
         <v>354</v>
       </c>
-      <c r="D207" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E207" s="4" t="s">
-        <v>17</v>
+      <c r="D207" s="4">
+        <v>1</v>
+      </c>
+      <c r="E207" s="4">
+        <v>1</v>
       </c>
       <c r="F207" s="4">
         <v>2</v>
       </c>
       <c r="G207" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1201, 267, 354, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1201, 267, 354, 1, 1, 2);</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -30785,18 +30785,18 @@
       <c r="C208" s="4">
         <v>354</v>
       </c>
-      <c r="D208" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E208" s="4" t="s">
-        <v>17</v>
+      <c r="D208" s="4">
+        <v>0</v>
+      </c>
+      <c r="E208" s="4">
+        <v>0</v>
       </c>
       <c r="F208" s="4">
         <v>1</v>
       </c>
       <c r="G208" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1202, 267, 354, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1202, 267, 354, 0, 0, 1);</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Date 2 Group A
Date 2 Group A
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -27632,18 +27632,18 @@
       <c r="C89" s="3">
         <v>40</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>17</v>
+      <c r="D89" s="3">
+        <v>1</v>
+      </c>
+      <c r="E89" s="3">
+        <v>1</v>
       </c>
       <c r="F89" s="3">
         <v>2</v>
       </c>
       <c r="G89" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1083, 238, 40, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1083, 238, 40, 1, 1, 2);</v>
       </c>
       <c r="H89" s="4"/>
     </row>
@@ -27659,18 +27659,18 @@
       <c r="C90" s="3">
         <v>40</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>17</v>
+      <c r="D90" s="3">
+        <v>1</v>
+      </c>
+      <c r="E90" s="3">
+        <v>0</v>
       </c>
       <c r="F90" s="3">
         <v>1</v>
       </c>
       <c r="G90" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1084, 238, 40, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1084, 238, 40, 1, 0, 1);</v>
       </c>
       <c r="H90" s="4"/>
     </row>
@@ -27686,18 +27686,18 @@
       <c r="C91" s="3">
         <v>41</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E91" s="3" t="s">
-        <v>17</v>
+      <c r="D91" s="3">
+        <v>1</v>
+      </c>
+      <c r="E91" s="3">
+        <v>1</v>
       </c>
       <c r="F91" s="3">
         <v>2</v>
       </c>
       <c r="G91" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1085, 238, 41, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1085, 238, 41, 1, 1, 2);</v>
       </c>
       <c r="H91" s="4"/>
     </row>
@@ -27713,18 +27713,18 @@
       <c r="C92" s="3">
         <v>41</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>17</v>
+      <c r="D92" s="3">
+        <v>0</v>
+      </c>
+      <c r="E92" s="3">
+        <v>0</v>
       </c>
       <c r="F92" s="3">
         <v>1</v>
       </c>
       <c r="G92" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1086, 238, 41, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1086, 238, 41, 0, 0, 1);</v>
       </c>
       <c r="H92" s="4"/>
     </row>
@@ -27740,18 +27740,18 @@
       <c r="C93" s="4">
         <v>33</v>
       </c>
-      <c r="D93" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E93" s="4" t="s">
-        <v>17</v>
+      <c r="D93" s="4">
+        <v>2</v>
+      </c>
+      <c r="E93" s="4">
+        <v>3</v>
       </c>
       <c r="F93" s="4">
         <v>2</v>
       </c>
       <c r="G93" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1087, 239, 33, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1087, 239, 33, 2, 3, 2);</v>
       </c>
       <c r="H93" s="4"/>
     </row>
@@ -27767,18 +27767,18 @@
       <c r="C94" s="4">
         <v>33</v>
       </c>
-      <c r="D94" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>17</v>
+      <c r="D94" s="4">
+        <v>0</v>
+      </c>
+      <c r="E94" s="4">
+        <v>0</v>
       </c>
       <c r="F94" s="4">
         <v>1</v>
       </c>
       <c r="G94" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1088, 239, 33, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1088, 239, 33, 0, 0, 1);</v>
       </c>
       <c r="H94" s="4"/>
     </row>
@@ -27794,18 +27794,18 @@
       <c r="C95" s="4">
         <v>355</v>
       </c>
-      <c r="D95" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E95" s="4" t="s">
-        <v>17</v>
+      <c r="D95" s="4">
+        <v>0</v>
+      </c>
+      <c r="E95" s="4">
+        <v>0</v>
       </c>
       <c r="F95" s="4">
         <v>2</v>
       </c>
       <c r="G95" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1089, 239, 355, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1089, 239, 355, 0, 0, 2);</v>
       </c>
       <c r="H95" s="4"/>
     </row>
@@ -27821,18 +27821,18 @@
       <c r="C96" s="4">
         <v>355</v>
       </c>
-      <c r="D96" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E96" s="4" t="s">
-        <v>17</v>
+      <c r="D96" s="4">
+        <v>0</v>
+      </c>
+      <c r="E96" s="4">
+        <v>0</v>
       </c>
       <c r="F96" s="4">
         <v>1</v>
       </c>
       <c r="G96" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1090, 239, 355, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1090, 239, 355, 0, 0, 1);</v>
       </c>
       <c r="H96" s="4"/>
     </row>
@@ -28280,18 +28280,18 @@
       <c r="C113" s="3">
         <v>7</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E113" s="3" t="s">
-        <v>17</v>
+      <c r="D113" s="3">
+        <v>1</v>
+      </c>
+      <c r="E113" s="3">
+        <v>0</v>
       </c>
       <c r="F113" s="3">
         <v>2</v>
       </c>
       <c r="G113" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1107, 244, 7, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1107, 244, 7, 1, 0, 2);</v>
       </c>
       <c r="H113" s="4"/>
     </row>
@@ -28307,18 +28307,18 @@
       <c r="C114" s="3">
         <v>7</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>17</v>
+      <c r="D114" s="3">
+        <v>0</v>
+      </c>
+      <c r="E114" s="3">
+        <v>0</v>
       </c>
       <c r="F114" s="3">
         <v>1</v>
       </c>
       <c r="G114" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1108, 244, 7, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1108, 244, 7, 0, 0, 1);</v>
       </c>
       <c r="H114" s="4"/>
     </row>
@@ -28334,18 +28334,18 @@
       <c r="C115" s="3">
         <v>421</v>
       </c>
-      <c r="D115" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E115" s="3" t="s">
-        <v>17</v>
+      <c r="D115" s="3">
+        <v>2</v>
+      </c>
+      <c r="E115" s="3">
+        <v>3</v>
       </c>
       <c r="F115" s="3">
         <v>2</v>
       </c>
       <c r="G115" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1109, 244, 421, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1109, 244, 421, 2, 3, 2);</v>
       </c>
       <c r="H115" s="4"/>
     </row>
@@ -28361,18 +28361,18 @@
       <c r="C116" s="3">
         <v>421</v>
       </c>
-      <c r="D116" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E116" s="3" t="s">
-        <v>17</v>
+      <c r="D116" s="3">
+        <v>2</v>
+      </c>
+      <c r="E116" s="3">
+        <v>0</v>
       </c>
       <c r="F116" s="3">
         <v>1</v>
       </c>
       <c r="G116" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1110, 244, 421, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1110, 244, 421, 2, 0, 1);</v>
       </c>
       <c r="H116" s="4"/>
     </row>

</xml_diff>

<commit_message>
Date 2 Group C and D Quarterfinals
Date 2 Group C and D Quarterfinals
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -28388,18 +28388,18 @@
       <c r="C117" s="4">
         <v>4420</v>
       </c>
-      <c r="D117" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E117" s="4" t="s">
-        <v>17</v>
+      <c r="D117" s="4">
+        <v>2</v>
+      </c>
+      <c r="E117" s="4">
+        <v>3</v>
       </c>
       <c r="F117" s="4">
         <v>2</v>
       </c>
       <c r="G117" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1111, 245, 4420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1111, 245, 4420, 2, 3, 2);</v>
       </c>
       <c r="H117" s="4"/>
     </row>
@@ -28415,18 +28415,18 @@
       <c r="C118" s="4">
         <v>4420</v>
       </c>
-      <c r="D118" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E118" s="4" t="s">
-        <v>17</v>
+      <c r="D118" s="4">
+        <v>0</v>
+      </c>
+      <c r="E118" s="4">
+        <v>0</v>
       </c>
       <c r="F118" s="4">
         <v>1</v>
       </c>
       <c r="G118" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1112, 245, 4420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1112, 245, 4420, 0, 0, 1);</v>
       </c>
       <c r="H118" s="4"/>
     </row>
@@ -28442,18 +28442,18 @@
       <c r="C119" s="4">
         <v>4429</v>
       </c>
-      <c r="D119" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E119" s="4" t="s">
-        <v>17</v>
+      <c r="D119" s="4">
+        <v>1</v>
+      </c>
+      <c r="E119" s="4">
+        <v>0</v>
       </c>
       <c r="F119" s="4">
         <v>2</v>
       </c>
       <c r="G119" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1113, 245, 4429, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1113, 245, 4429, 1, 0, 2);</v>
       </c>
       <c r="H119" s="4"/>
     </row>
@@ -28469,18 +28469,18 @@
       <c r="C120" s="4">
         <v>4429</v>
       </c>
-      <c r="D120" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E120" s="4" t="s">
-        <v>17</v>
+      <c r="D120" s="4">
+        <v>1</v>
+      </c>
+      <c r="E120" s="4">
+        <v>0</v>
       </c>
       <c r="F120" s="4">
         <v>1</v>
       </c>
       <c r="G120" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1114, 245, 4429, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1114, 245, 4429, 1, 0, 1);</v>
       </c>
       <c r="H120" s="4"/>
     </row>
@@ -28928,18 +28928,18 @@
       <c r="C137" s="3">
         <v>380</v>
       </c>
-      <c r="D137" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>17</v>
+      <c r="D137" s="3">
+        <v>0</v>
+      </c>
+      <c r="E137" s="3">
+        <v>0</v>
       </c>
       <c r="F137" s="3">
         <v>2</v>
       </c>
       <c r="G137" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1131, 250, 380, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1131, 250, 380, 0, 0, 2);</v>
       </c>
       <c r="H137" s="4"/>
     </row>
@@ -28955,18 +28955,18 @@
       <c r="C138" s="3">
         <v>380</v>
       </c>
-      <c r="D138" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>17</v>
+      <c r="D138" s="3">
+        <v>0</v>
+      </c>
+      <c r="E138" s="3">
+        <v>0</v>
       </c>
       <c r="F138" s="3">
         <v>1</v>
       </c>
       <c r="G138" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1132, 250, 380, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1132, 250, 380, 0, 0, 1);</v>
       </c>
       <c r="H138" s="4"/>
     </row>
@@ -28982,18 +28982,18 @@
       <c r="C139" s="3">
         <v>4428</v>
       </c>
-      <c r="D139" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E139" s="3" t="s">
-        <v>17</v>
+      <c r="D139" s="3">
+        <v>2</v>
+      </c>
+      <c r="E139" s="3">
+        <v>3</v>
       </c>
       <c r="F139" s="3">
         <v>2</v>
       </c>
       <c r="G139" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1133, 250, 4428, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1133, 250, 4428, 2, 3, 2);</v>
       </c>
       <c r="H139" s="4"/>
     </row>
@@ -29009,18 +29009,18 @@
       <c r="C140" s="3">
         <v>4428</v>
       </c>
-      <c r="D140" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E140" s="3" t="s">
-        <v>17</v>
+      <c r="D140" s="3">
+        <v>0</v>
+      </c>
+      <c r="E140" s="3">
+        <v>0</v>
       </c>
       <c r="F140" s="3">
         <v>1</v>
       </c>
       <c r="G140" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1134, 250, 4428, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1134, 250, 4428, 0, 0, 1);</v>
       </c>
       <c r="H140" s="4"/>
     </row>
@@ -29036,18 +29036,18 @@
       <c r="C141" s="4">
         <v>49</v>
       </c>
-      <c r="D141" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E141" s="4" t="s">
-        <v>17</v>
+      <c r="D141" s="4">
+        <v>0</v>
+      </c>
+      <c r="E141" s="4">
+        <v>1</v>
       </c>
       <c r="F141" s="4">
         <v>2</v>
       </c>
       <c r="G141" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1135, 251, 49, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1135, 251, 49, 0, 1, 2);</v>
       </c>
       <c r="H141" s="4"/>
     </row>
@@ -29063,18 +29063,18 @@
       <c r="C142" s="4">
         <v>49</v>
       </c>
-      <c r="D142" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E142" s="4" t="s">
-        <v>17</v>
+      <c r="D142" s="4">
+        <v>0</v>
+      </c>
+      <c r="E142" s="4">
+        <v>1</v>
       </c>
       <c r="F142" s="4">
         <v>1</v>
       </c>
       <c r="G142" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1136, 251, 49, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1136, 251, 49, 0, 1, 1);</v>
       </c>
       <c r="H142" s="4"/>
     </row>
@@ -29090,18 +29090,18 @@
       <c r="C143" s="4">
         <v>48</v>
       </c>
-      <c r="D143" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E143" s="4" t="s">
-        <v>17</v>
+      <c r="D143" s="4">
+        <v>0</v>
+      </c>
+      <c r="E143" s="4">
+        <v>1</v>
       </c>
       <c r="F143" s="4">
         <v>2</v>
       </c>
       <c r="G143" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1137, 251, 48, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1137, 251, 48, 0, 1, 2);</v>
       </c>
       <c r="H143" s="4"/>
     </row>
@@ -29117,18 +29117,18 @@
       <c r="C144" s="4">
         <v>48</v>
       </c>
-      <c r="D144" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E144" s="4" t="s">
-        <v>17</v>
+      <c r="D144" s="4">
+        <v>0</v>
+      </c>
+      <c r="E144" s="4">
+        <v>1</v>
       </c>
       <c r="F144" s="4">
         <v>1</v>
       </c>
       <c r="G144" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1138, 251, 48, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1138, 251, 48, 0, 1, 1);</v>
       </c>
       <c r="H144" s="4"/>
     </row>

</xml_diff>

<commit_message>
Semifinales Copa America tercera fecha Grupo A Eurocopa
Semifinales Copa America tercera fecha Grupo A Eurocopa
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -27848,18 +27848,18 @@
       <c r="C97" s="3">
         <v>40</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>17</v>
+      <c r="D97" s="3">
+        <v>0</v>
+      </c>
+      <c r="E97" s="3">
+        <v>0</v>
       </c>
       <c r="F97" s="3">
         <v>2</v>
       </c>
       <c r="G97" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1091, 240, 40, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1091, 240, 40, 0, 0, 2);</v>
       </c>
       <c r="H97" s="4"/>
     </row>
@@ -27875,18 +27875,18 @@
       <c r="C98" s="3">
         <v>40</v>
       </c>
-      <c r="D98" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>17</v>
+      <c r="D98" s="3">
+        <v>0</v>
+      </c>
+      <c r="E98" s="3">
+        <v>0</v>
       </c>
       <c r="F98" s="3">
         <v>1</v>
       </c>
       <c r="G98" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1092, 240, 40, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1092, 240, 40, 0, 0, 1);</v>
       </c>
       <c r="H98" s="4"/>
     </row>
@@ -27902,18 +27902,18 @@
       <c r="C99" s="3">
         <v>355</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>17</v>
+      <c r="D99" s="3">
+        <v>1</v>
+      </c>
+      <c r="E99" s="3">
+        <v>3</v>
       </c>
       <c r="F99" s="3">
         <v>2</v>
       </c>
       <c r="G99" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1093, 240, 355, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1093, 240, 355, 1, 3, 2);</v>
       </c>
       <c r="H99" s="4"/>
     </row>
@@ -27929,18 +27929,18 @@
       <c r="C100" s="3">
         <v>355</v>
       </c>
-      <c r="D100" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>17</v>
+      <c r="D100" s="3">
+        <v>1</v>
+      </c>
+      <c r="E100" s="3">
+        <v>0</v>
       </c>
       <c r="F100" s="3">
         <v>1</v>
       </c>
       <c r="G100" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1094, 240, 355, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1094, 240, 355, 1, 0, 1);</v>
       </c>
       <c r="H100" s="4"/>
     </row>
@@ -27956,18 +27956,18 @@
       <c r="C101" s="4">
         <v>41</v>
       </c>
-      <c r="D101" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E101" s="4" t="s">
-        <v>17</v>
+      <c r="D101" s="4">
+        <v>0</v>
+      </c>
+      <c r="E101" s="4">
+        <v>1</v>
       </c>
       <c r="F101" s="4">
         <v>2</v>
       </c>
       <c r="G101" s="4" t="str">
         <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A101 &amp; ", " &amp; B101 &amp; ", " &amp; C101 &amp; ", " &amp; D101 &amp; ", " &amp; E101 &amp; ", " &amp; F101 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1095, 241, 41, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1095, 241, 41, 0, 1, 2);</v>
       </c>
       <c r="H101" s="4"/>
     </row>
@@ -27983,18 +27983,18 @@
       <c r="C102" s="4">
         <v>41</v>
       </c>
-      <c r="D102" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E102" s="4" t="s">
-        <v>17</v>
+      <c r="D102" s="4">
+        <v>0</v>
+      </c>
+      <c r="E102" s="4">
+        <v>0</v>
       </c>
       <c r="F102" s="4">
         <v>1</v>
       </c>
       <c r="G102" s="4" t="str">
         <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A102 &amp; ", " &amp; B102 &amp; ", " &amp; C102 &amp; ", " &amp; D102 &amp; ", " &amp; E102 &amp; ", " &amp; F102 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1096, 241, 41, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1096, 241, 41, 0, 0, 1);</v>
       </c>
       <c r="H102" s="4"/>
     </row>
@@ -28010,18 +28010,18 @@
       <c r="C103" s="4">
         <v>33</v>
       </c>
-      <c r="D103" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E103" s="4" t="s">
-        <v>17</v>
+      <c r="D103" s="4">
+        <v>0</v>
+      </c>
+      <c r="E103" s="4">
+        <v>1</v>
       </c>
       <c r="F103" s="4">
         <v>2</v>
       </c>
       <c r="G103" s="4" t="str">
         <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A103 &amp; ", " &amp; B103 &amp; ", " &amp; C103 &amp; ", " &amp; D103 &amp; ", " &amp; E103 &amp; ", " &amp; F103 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1097, 241, 33, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1097, 241, 33, 0, 1, 2);</v>
       </c>
       <c r="H103" s="4"/>
     </row>
@@ -28037,18 +28037,18 @@
       <c r="C104" s="4">
         <v>33</v>
       </c>
-      <c r="D104" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E104" s="4" t="s">
-        <v>17</v>
+      <c r="D104" s="4">
+        <v>0</v>
+      </c>
+      <c r="E104" s="4">
+        <v>0</v>
       </c>
       <c r="F104" s="4">
         <v>1</v>
       </c>
       <c r="G104" s="4" t="str">
         <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A104 &amp; ", " &amp; B104 &amp; ", " &amp; C104 &amp; ", " &amp; D104 &amp; ", " &amp; E104 &amp; ", " &amp; F104 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1098, 241, 33, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1098, 241, 33, 0, 0, 1);</v>
       </c>
       <c r="H104" s="4"/>
     </row>
@@ -29563,18 +29563,18 @@
       <c r="C161" s="3">
         <v>420</v>
       </c>
-      <c r="D161" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>17</v>
+      <c r="D161" s="3">
+        <v>2</v>
+      </c>
+      <c r="E161" s="3">
+        <v>1</v>
       </c>
       <c r="F161" s="3">
         <v>2</v>
       </c>
       <c r="G161" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1155, 256, 420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1155, 256, 420, 2, 1, 2);</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -29589,18 +29589,18 @@
       <c r="C162" s="3">
         <v>420</v>
       </c>
-      <c r="D162" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>17</v>
+      <c r="D162" s="3">
+        <v>0</v>
+      </c>
+      <c r="E162" s="3">
+        <v>0</v>
       </c>
       <c r="F162" s="3">
         <v>1</v>
       </c>
       <c r="G162" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1156, 256, 420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1156, 256, 420, 0, 0, 1);</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -29615,18 +29615,18 @@
       <c r="C163" s="3">
         <v>385</v>
       </c>
-      <c r="D163" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>17</v>
+      <c r="D163" s="3">
+        <v>2</v>
+      </c>
+      <c r="E163" s="3">
+        <v>1</v>
       </c>
       <c r="F163" s="3">
         <v>2</v>
       </c>
       <c r="G163" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1157, 256, 385, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1157, 256, 385, 2, 1, 2);</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -29641,18 +29641,18 @@
       <c r="C164" s="3">
         <v>385</v>
       </c>
-      <c r="D164" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>17</v>
+      <c r="D164" s="3">
+        <v>1</v>
+      </c>
+      <c r="E164" s="3">
+        <v>0</v>
       </c>
       <c r="F164" s="3">
         <v>1</v>
       </c>
       <c r="G164" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1158, 256, 385, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1158, 256, 385, 1, 0, 1);</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -29667,18 +29667,18 @@
       <c r="C165" s="4">
         <v>34</v>
       </c>
-      <c r="D165" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E165" s="4" t="s">
-        <v>17</v>
+      <c r="D165" s="4">
+        <v>3</v>
+      </c>
+      <c r="E165" s="4">
+        <v>3</v>
       </c>
       <c r="F165" s="4">
         <v>2</v>
       </c>
       <c r="G165" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1159, 257, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1159, 257, 34, 3, 3, 2);</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -29693,18 +29693,18 @@
       <c r="C166" s="4">
         <v>34</v>
       </c>
-      <c r="D166" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E166" s="4" t="s">
-        <v>17</v>
+      <c r="D166" s="4">
+        <v>2</v>
+      </c>
+      <c r="E166" s="4">
+        <v>0</v>
       </c>
       <c r="F166" s="4">
         <v>1</v>
       </c>
       <c r="G166" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1160, 257, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1160, 257, 34, 2, 0, 1);</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -29719,18 +29719,18 @@
       <c r="C167" s="4">
         <v>90</v>
       </c>
-      <c r="D167" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E167" s="4" t="s">
-        <v>17</v>
+      <c r="D167" s="4">
+        <v>0</v>
+      </c>
+      <c r="E167" s="4">
+        <v>0</v>
       </c>
       <c r="F167" s="4">
         <v>2</v>
       </c>
       <c r="G167" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1161, 257, 90, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1161, 257, 90, 0, 0, 2);</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -29745,18 +29745,18 @@
       <c r="C168" s="4">
         <v>90</v>
       </c>
-      <c r="D168" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E168" s="4" t="s">
-        <v>17</v>
+      <c r="D168" s="4">
+        <v>0</v>
+      </c>
+      <c r="E168" s="4">
+        <v>0</v>
       </c>
       <c r="F168" s="4">
         <v>1</v>
       </c>
       <c r="G168" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1162, 257, 90, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1162, 257, 90, 0, 0, 1);</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -30187,18 +30187,18 @@
       <c r="C185" s="3">
         <v>39</v>
       </c>
-      <c r="D185" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E185" s="3" t="s">
-        <v>17</v>
+      <c r="D185" s="3">
+        <v>1</v>
+      </c>
+      <c r="E185" s="3">
+        <v>3</v>
       </c>
       <c r="F185" s="3">
         <v>2</v>
       </c>
       <c r="G185" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1179, 262, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1179, 262, 39, 1, 3, 2);</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -30213,18 +30213,18 @@
       <c r="C186" s="3">
         <v>39</v>
       </c>
-      <c r="D186" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E186" s="3" t="s">
-        <v>17</v>
+      <c r="D186" s="3">
+        <v>0</v>
+      </c>
+      <c r="E186" s="3">
+        <v>0</v>
       </c>
       <c r="F186" s="3">
         <v>1</v>
       </c>
       <c r="G186" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1180, 262, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1180, 262, 39, 0, 0, 1);</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
@@ -30239,18 +30239,18 @@
       <c r="C187" s="3">
         <v>46</v>
       </c>
-      <c r="D187" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E187" s="3" t="s">
-        <v>17</v>
+      <c r="D187" s="3">
+        <v>0</v>
+      </c>
+      <c r="E187" s="3">
+        <v>0</v>
       </c>
       <c r="F187" s="3">
         <v>2</v>
       </c>
       <c r="G187" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1181, 262, 46, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1181, 262, 46, 0, 0, 2);</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
@@ -30265,18 +30265,18 @@
       <c r="C188" s="3">
         <v>46</v>
       </c>
-      <c r="D188" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E188" s="3" t="s">
-        <v>17</v>
+      <c r="D188" s="3">
+        <v>0</v>
+      </c>
+      <c r="E188" s="3">
+        <v>0</v>
       </c>
       <c r="F188" s="3">
         <v>1</v>
       </c>
       <c r="G188" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1182, 262, 46, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1182, 262, 46, 0, 0, 1);</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -30291,18 +30291,18 @@
       <c r="C189" s="4">
         <v>32</v>
       </c>
-      <c r="D189" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E189" s="4" t="s">
-        <v>17</v>
+      <c r="D189" s="4">
+        <v>3</v>
+      </c>
+      <c r="E189" s="4">
+        <v>3</v>
       </c>
       <c r="F189" s="4">
         <v>2</v>
       </c>
       <c r="G189" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1183, 263, 32, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1183, 263, 32, 3, 3, 2);</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -30317,18 +30317,18 @@
       <c r="C190" s="4">
         <v>32</v>
       </c>
-      <c r="D190" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E190" s="4" t="s">
-        <v>17</v>
+      <c r="D190" s="4">
+        <v>0</v>
+      </c>
+      <c r="E190" s="4">
+        <v>0</v>
       </c>
       <c r="F190" s="4">
         <v>1</v>
       </c>
       <c r="G190" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1184, 263, 32, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1184, 263, 32, 0, 0, 1);</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
@@ -30343,18 +30343,18 @@
       <c r="C191" s="4">
         <v>353</v>
       </c>
-      <c r="D191" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E191" s="4" t="s">
-        <v>17</v>
+      <c r="D191" s="4">
+        <v>0</v>
+      </c>
+      <c r="E191" s="4">
+        <v>0</v>
       </c>
       <c r="F191" s="4">
         <v>2</v>
       </c>
       <c r="G191" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1185, 263, 353, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1185, 263, 353, 0, 0, 2);</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -30369,18 +30369,18 @@
       <c r="C192" s="4">
         <v>353</v>
       </c>
-      <c r="D192" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E192" s="4" t="s">
-        <v>17</v>
+      <c r="D192" s="4">
+        <v>0</v>
+      </c>
+      <c r="E192" s="4">
+        <v>0</v>
       </c>
       <c r="F192" s="4">
         <v>1</v>
       </c>
       <c r="G192" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1186, 263, 353, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1186, 263, 353, 0, 0, 1);</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -30811,18 +30811,18 @@
       <c r="C209" s="3">
         <v>354</v>
       </c>
-      <c r="D209" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E209" s="3" t="s">
-        <v>17</v>
+      <c r="D209" s="3">
+        <v>1</v>
+      </c>
+      <c r="E209" s="3">
+        <v>1</v>
       </c>
       <c r="F209" s="3">
         <v>2</v>
       </c>
       <c r="G209" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1203, 268, 354, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1203, 268, 354, 1, 1, 2);</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -30837,18 +30837,18 @@
       <c r="C210" s="3">
         <v>354</v>
       </c>
-      <c r="D210" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E210" s="3" t="s">
-        <v>17</v>
+      <c r="D210" s="3">
+        <v>1</v>
+      </c>
+      <c r="E210" s="3">
+        <v>0</v>
       </c>
       <c r="F210" s="3">
         <v>1</v>
       </c>
       <c r="G210" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1204, 268, 354, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1204, 268, 354, 1, 0, 1);</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -30863,18 +30863,18 @@
       <c r="C211" s="3">
         <v>36</v>
       </c>
-      <c r="D211" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E211" s="3" t="s">
-        <v>17</v>
+      <c r="D211" s="3">
+        <v>1</v>
+      </c>
+      <c r="E211" s="3">
+        <v>1</v>
       </c>
       <c r="F211" s="3">
         <v>2</v>
       </c>
       <c r="G211" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1205, 268, 36, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1205, 268, 36, 1, 1, 2);</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -30889,18 +30889,18 @@
       <c r="C212" s="3">
         <v>36</v>
       </c>
-      <c r="D212" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E212" s="3" t="s">
-        <v>17</v>
+      <c r="D212" s="3">
+        <v>0</v>
+      </c>
+      <c r="E212" s="3">
+        <v>0</v>
       </c>
       <c r="F212" s="3">
         <v>1</v>
       </c>
       <c r="G212" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1206, 268, 36, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1206, 268, 36, 0, 0, 1);</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -30915,18 +30915,18 @@
       <c r="C213" s="4">
         <v>351</v>
       </c>
-      <c r="D213" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E213" s="4" t="s">
-        <v>17</v>
+      <c r="D213" s="4">
+        <v>0</v>
+      </c>
+      <c r="E213" s="4">
+        <v>1</v>
       </c>
       <c r="F213" s="4">
         <v>2</v>
       </c>
       <c r="G213" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1207, 269, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1207, 269, 351, 0, 1, 2);</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -30941,18 +30941,18 @@
       <c r="C214" s="4">
         <v>351</v>
       </c>
-      <c r="D214" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E214" s="4" t="s">
-        <v>17</v>
+      <c r="D214" s="4">
+        <v>0</v>
+      </c>
+      <c r="E214" s="4">
+        <v>0</v>
       </c>
       <c r="F214" s="4">
         <v>1</v>
       </c>
       <c r="G214" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1208, 269, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1208, 269, 351, 0, 0, 1);</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -30967,18 +30967,18 @@
       <c r="C215" s="4">
         <v>43</v>
       </c>
-      <c r="D215" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E215" s="4" t="s">
-        <v>17</v>
+      <c r="D215" s="4">
+        <v>0</v>
+      </c>
+      <c r="E215" s="4">
+        <v>1</v>
       </c>
       <c r="F215" s="4">
         <v>2</v>
       </c>
       <c r="G215" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1209, 269, 43, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1209, 269, 43, 0, 1, 2);</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -30993,18 +30993,18 @@
       <c r="C216" s="4">
         <v>43</v>
       </c>
-      <c r="D216" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E216" s="4" t="s">
-        <v>17</v>
+      <c r="D216" s="4">
+        <v>0</v>
+      </c>
+      <c r="E216" s="4">
+        <v>0</v>
       </c>
       <c r="F216" s="4">
         <v>1</v>
       </c>
       <c r="G216" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1210, 269, 43, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1210, 269, 43, 0, 0, 1);</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Eurocopa Group B Third Date
Eurocopa Group B Third Date
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -28496,18 +28496,18 @@
       <c r="C121" s="3">
         <v>7</v>
       </c>
-      <c r="D121" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>17</v>
+      <c r="D121" s="3">
+        <v>0</v>
+      </c>
+      <c r="E121" s="3">
+        <v>0</v>
       </c>
       <c r="F121" s="3">
         <v>2</v>
       </c>
       <c r="G121" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1115, 246, 7, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1115, 246, 7, 0, 0, 2);</v>
       </c>
       <c r="H121" s="4"/>
     </row>
@@ -28523,18 +28523,18 @@
       <c r="C122" s="3">
         <v>7</v>
       </c>
-      <c r="D122" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E122" s="3" t="s">
-        <v>17</v>
+      <c r="D122" s="3">
+        <v>0</v>
+      </c>
+      <c r="E122" s="3">
+        <v>0</v>
       </c>
       <c r="F122" s="3">
         <v>1</v>
       </c>
       <c r="G122" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1116, 246, 7, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1116, 246, 7, 0, 0, 1);</v>
       </c>
       <c r="H122" s="4"/>
     </row>
@@ -28550,18 +28550,18 @@
       <c r="C123" s="3">
         <v>4429</v>
       </c>
-      <c r="D123" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>17</v>
+      <c r="D123" s="3">
+        <v>3</v>
+      </c>
+      <c r="E123" s="3">
+        <v>3</v>
       </c>
       <c r="F123" s="3">
         <v>2</v>
       </c>
       <c r="G123" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1117, 246, 4429, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1117, 246, 4429, 3, 3, 2);</v>
       </c>
       <c r="H123" s="4"/>
     </row>
@@ -28577,18 +28577,18 @@
       <c r="C124" s="3">
         <v>4429</v>
       </c>
-      <c r="D124" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E124" s="3" t="s">
-        <v>17</v>
+      <c r="D124" s="3">
+        <v>2</v>
+      </c>
+      <c r="E124" s="3">
+        <v>0</v>
       </c>
       <c r="F124" s="3">
         <v>1</v>
       </c>
       <c r="G124" s="3" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1118, 246, 4429, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1118, 246, 4429, 2, 0, 1);</v>
       </c>
       <c r="H124" s="4"/>
     </row>
@@ -28604,18 +28604,18 @@
       <c r="C125" s="4">
         <v>421</v>
       </c>
-      <c r="D125" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E125" s="4" t="s">
-        <v>17</v>
+      <c r="D125" s="4">
+        <v>0</v>
+      </c>
+      <c r="E125" s="4">
+        <v>1</v>
       </c>
       <c r="F125" s="4">
         <v>2</v>
       </c>
       <c r="G125" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1119, 247, 421, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1119, 247, 421, 0, 1, 2);</v>
       </c>
       <c r="H125" s="4"/>
     </row>
@@ -28631,18 +28631,18 @@
       <c r="C126" s="4">
         <v>421</v>
       </c>
-      <c r="D126" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E126" s="4" t="s">
-        <v>17</v>
+      <c r="D126" s="4">
+        <v>0</v>
+      </c>
+      <c r="E126" s="4">
+        <v>0</v>
       </c>
       <c r="F126" s="4">
         <v>1</v>
       </c>
       <c r="G126" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1120, 247, 421, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1120, 247, 421, 0, 0, 1);</v>
       </c>
       <c r="H126" s="4"/>
     </row>
@@ -28658,18 +28658,18 @@
       <c r="C127" s="4">
         <v>4420</v>
       </c>
-      <c r="D127" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E127" s="4" t="s">
-        <v>17</v>
+      <c r="D127" s="4">
+        <v>0</v>
+      </c>
+      <c r="E127" s="4">
+        <v>1</v>
       </c>
       <c r="F127" s="4">
         <v>2</v>
       </c>
       <c r="G127" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1121, 247, 4420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1121, 247, 4420, 0, 1, 2);</v>
       </c>
       <c r="H127" s="4"/>
     </row>
@@ -28685,18 +28685,18 @@
       <c r="C128" s="4">
         <v>4420</v>
       </c>
-      <c r="D128" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E128" s="4" t="s">
-        <v>17</v>
+      <c r="D128" s="4">
+        <v>0</v>
+      </c>
+      <c r="E128" s="4">
+        <v>0</v>
       </c>
       <c r="F128" s="4">
         <v>1</v>
       </c>
       <c r="G128" s="4" t="str">
         <f t="shared" si="10"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1122, 247, 4420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1122, 247, 4420, 0, 0, 1);</v>
       </c>
       <c r="H128" s="4"/>
     </row>

</xml_diff>

<commit_message>
Copa America 1st semifinal EuroCopa 3 Date Groups C and D
Copa America 1st semifinal EuroCopa 3 Date Groups C and D
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -29144,18 +29144,18 @@
       <c r="C145" s="3">
         <v>380</v>
       </c>
-      <c r="D145" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E145" s="3" t="s">
-        <v>17</v>
+      <c r="D145" s="3">
+        <v>0</v>
+      </c>
+      <c r="E145" s="3">
+        <v>0</v>
       </c>
       <c r="F145" s="3">
         <v>2</v>
       </c>
       <c r="G145" s="3" t="str">
         <f t="shared" ref="G145:G192" si="12">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A145 &amp; ", " &amp; B145 &amp; ", " &amp; C145 &amp; ", " &amp; D145 &amp; ", " &amp; E145 &amp; ", " &amp; F145 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1139, 252, 380, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1139, 252, 380, 0, 0, 2);</v>
       </c>
       <c r="H145" s="4"/>
     </row>
@@ -29171,18 +29171,18 @@
       <c r="C146" s="3">
         <v>380</v>
       </c>
-      <c r="D146" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E146" s="3" t="s">
-        <v>17</v>
+      <c r="D146" s="3">
+        <v>0</v>
+      </c>
+      <c r="E146" s="3">
+        <v>0</v>
       </c>
       <c r="F146" s="3">
         <v>1</v>
       </c>
       <c r="G146" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1140, 252, 380, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1140, 252, 380, 0, 0, 1);</v>
       </c>
       <c r="H146" s="4"/>
     </row>
@@ -29198,18 +29198,18 @@
       <c r="C147" s="3">
         <v>48</v>
       </c>
-      <c r="D147" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>17</v>
+      <c r="D147" s="3">
+        <v>1</v>
+      </c>
+      <c r="E147" s="3">
+        <v>3</v>
       </c>
       <c r="F147" s="3">
         <v>2</v>
       </c>
       <c r="G147" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1141, 252, 48, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1141, 252, 48, 1, 3, 2);</v>
       </c>
       <c r="H147" s="4"/>
     </row>
@@ -29225,18 +29225,18 @@
       <c r="C148" s="3">
         <v>48</v>
       </c>
-      <c r="D148" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E148" s="3" t="s">
-        <v>17</v>
+      <c r="D148" s="3">
+        <v>0</v>
+      </c>
+      <c r="E148" s="3">
+        <v>0</v>
       </c>
       <c r="F148" s="3">
         <v>1</v>
       </c>
       <c r="G148" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1142, 252, 48, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1142, 252, 48, 0, 0, 1);</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -29251,18 +29251,18 @@
       <c r="C149" s="4">
         <v>4428</v>
       </c>
-      <c r="D149" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E149" s="4" t="s">
-        <v>17</v>
+      <c r="D149" s="4">
+        <v>0</v>
+      </c>
+      <c r="E149" s="4">
+        <v>0</v>
       </c>
       <c r="F149" s="4">
         <v>2</v>
       </c>
       <c r="G149" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1143, 253, 4428, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1143, 253, 4428, 0, 0, 2);</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -29277,18 +29277,18 @@
       <c r="C150" s="4">
         <v>4428</v>
       </c>
-      <c r="D150" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E150" s="4" t="s">
-        <v>17</v>
+      <c r="D150" s="4">
+        <v>0</v>
+      </c>
+      <c r="E150" s="4">
+        <v>0</v>
       </c>
       <c r="F150" s="4">
         <v>1</v>
       </c>
       <c r="G150" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1144, 253, 4428, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1144, 253, 4428, 0, 0, 1);</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -29303,18 +29303,18 @@
       <c r="C151" s="4">
         <v>49</v>
       </c>
-      <c r="D151" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E151" s="4" t="s">
-        <v>17</v>
+      <c r="D151" s="4">
+        <v>1</v>
+      </c>
+      <c r="E151" s="4">
+        <v>3</v>
       </c>
       <c r="F151" s="4">
         <v>2</v>
       </c>
       <c r="G151" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1145, 253, 49, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1145, 253, 49, 1, 3, 2);</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -29329,18 +29329,18 @@
       <c r="C152" s="4">
         <v>49</v>
       </c>
-      <c r="D152" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E152" s="4" t="s">
-        <v>17</v>
+      <c r="D152" s="4">
+        <v>1</v>
+      </c>
+      <c r="E152" s="4">
+        <v>0</v>
       </c>
       <c r="F152" s="4">
         <v>1</v>
       </c>
       <c r="G152" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1146, 253, 49, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1146, 253, 49, 1, 0, 1);</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -29771,18 +29771,18 @@
       <c r="C169" s="3">
         <v>420</v>
       </c>
-      <c r="D169" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>17</v>
+      <c r="D169" s="3">
+        <v>0</v>
+      </c>
+      <c r="E169" s="3">
+        <v>0</v>
       </c>
       <c r="F169" s="3">
         <v>2</v>
       </c>
       <c r="G169" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1163, 258, 420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1163, 258, 420, 0, 0, 2);</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -29797,18 +29797,18 @@
       <c r="C170" s="3">
         <v>420</v>
       </c>
-      <c r="D170" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>17</v>
+      <c r="D170" s="3">
+        <v>0</v>
+      </c>
+      <c r="E170" s="3">
+        <v>0</v>
       </c>
       <c r="F170" s="3">
         <v>1</v>
       </c>
       <c r="G170" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1164, 258, 420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1164, 258, 420, 0, 0, 1);</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -29823,18 +29823,18 @@
       <c r="C171" s="3">
         <v>90</v>
       </c>
-      <c r="D171" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>17</v>
+      <c r="D171" s="3">
+        <v>2</v>
+      </c>
+      <c r="E171" s="3">
+        <v>3</v>
       </c>
       <c r="F171" s="3">
         <v>2</v>
       </c>
       <c r="G171" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1165, 258, 90, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1165, 258, 90, 2, 3, 2);</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -29849,18 +29849,18 @@
       <c r="C172" s="3">
         <v>90</v>
       </c>
-      <c r="D172" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>17</v>
+      <c r="D172" s="3">
+        <v>1</v>
+      </c>
+      <c r="E172" s="3">
+        <v>0</v>
       </c>
       <c r="F172" s="3">
         <v>1</v>
       </c>
       <c r="G172" s="3" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1166, 258, 90, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1166, 258, 90, 1, 0, 1);</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -29875,18 +29875,18 @@
       <c r="C173" s="4">
         <v>385</v>
       </c>
-      <c r="D173" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E173" s="4" t="s">
-        <v>17</v>
+      <c r="D173" s="4">
+        <v>2</v>
+      </c>
+      <c r="E173" s="4">
+        <v>3</v>
       </c>
       <c r="F173" s="4">
         <v>2</v>
       </c>
       <c r="G173" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1167, 259, 385, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1167, 259, 385, 2, 3, 2);</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -29901,18 +29901,18 @@
       <c r="C174" s="4">
         <v>385</v>
       </c>
-      <c r="D174" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E174" s="4" t="s">
-        <v>17</v>
+      <c r="D174" s="4">
+        <v>1</v>
+      </c>
+      <c r="E174" s="4">
+        <v>0</v>
       </c>
       <c r="F174" s="4">
         <v>1</v>
       </c>
       <c r="G174" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1168, 259, 385, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1168, 259, 385, 1, 0, 1);</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -29927,18 +29927,18 @@
       <c r="C175" s="4">
         <v>34</v>
       </c>
-      <c r="D175" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E175" s="4" t="s">
-        <v>17</v>
+      <c r="D175" s="4">
+        <v>1</v>
+      </c>
+      <c r="E175" s="4">
+        <v>0</v>
       </c>
       <c r="F175" s="4">
         <v>2</v>
       </c>
       <c r="G175" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1169, 259, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1169, 259, 34, 1, 0, 2);</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -29953,18 +29953,18 @@
       <c r="C176" s="4">
         <v>34</v>
       </c>
-      <c r="D176" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E176" s="4" t="s">
-        <v>17</v>
+      <c r="D176" s="4">
+        <v>1</v>
+      </c>
+      <c r="E176" s="4">
+        <v>0</v>
       </c>
       <c r="F176" s="4">
         <v>1</v>
       </c>
       <c r="G176" s="4" t="str">
         <f t="shared" si="12"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1170, 259, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1170, 259, 34, 1, 0, 1);</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
3rd Date Group E and F Eurocoa Sefmifinal Copa America
3rd Date Group E and F Eurocoa Sefmifinal Copa America
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -25496,7 +25496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J284"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A255" workbookViewId="0">
+      <selection activeCell="F255" sqref="F255"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30395,18 +30397,18 @@
       <c r="C193" s="3">
         <v>39</v>
       </c>
-      <c r="D193" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E193" s="3" t="s">
-        <v>17</v>
+      <c r="D193" s="3">
+        <v>0</v>
+      </c>
+      <c r="E193" s="3">
+        <v>0</v>
       </c>
       <c r="F193" s="3">
         <v>2</v>
       </c>
       <c r="G193" s="3" t="str">
         <f t="shared" ref="G193:G256" si="15">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A193 &amp; ", " &amp; B193 &amp; ", " &amp; C193 &amp; ", " &amp; D193 &amp; ", " &amp; E193 &amp; ", " &amp; F193 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1187, 264, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1187, 264, 39, 0, 0, 2);</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -30421,18 +30423,18 @@
       <c r="C194" s="3">
         <v>39</v>
       </c>
-      <c r="D194" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E194" s="3" t="s">
-        <v>17</v>
+      <c r="D194" s="3">
+        <v>0</v>
+      </c>
+      <c r="E194" s="3">
+        <v>0</v>
       </c>
       <c r="F194" s="3">
         <v>1</v>
       </c>
       <c r="G194" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1188, 264, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1188, 264, 39, 0, 0, 1);</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
@@ -30447,18 +30449,18 @@
       <c r="C195" s="3">
         <v>353</v>
       </c>
-      <c r="D195" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E195" s="3" t="s">
-        <v>17</v>
+      <c r="D195" s="3">
+        <v>1</v>
+      </c>
+      <c r="E195" s="3">
+        <v>3</v>
       </c>
       <c r="F195" s="3">
         <v>2</v>
       </c>
       <c r="G195" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1189, 264, 353, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1189, 264, 353, 1, 3, 2);</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -30473,18 +30475,18 @@
       <c r="C196" s="3">
         <v>353</v>
       </c>
-      <c r="D196" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E196" s="3" t="s">
-        <v>17</v>
+      <c r="D196" s="3">
+        <v>0</v>
+      </c>
+      <c r="E196" s="3">
+        <v>0</v>
       </c>
       <c r="F196" s="3">
         <v>1</v>
       </c>
       <c r="G196" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1190, 264, 353, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1190, 264, 353, 0, 0, 1);</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -30499,18 +30501,18 @@
       <c r="C197" s="4">
         <v>46</v>
       </c>
-      <c r="D197" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E197" s="4" t="s">
-        <v>17</v>
+      <c r="D197" s="4">
+        <v>0</v>
+      </c>
+      <c r="E197" s="4">
+        <v>0</v>
       </c>
       <c r="F197" s="4">
         <v>2</v>
       </c>
       <c r="G197" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1191, 265, 46, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1191, 265, 46, 0, 0, 2);</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -30525,18 +30527,18 @@
       <c r="C198" s="4">
         <v>46</v>
       </c>
-      <c r="D198" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E198" s="4" t="s">
-        <v>17</v>
+      <c r="D198" s="4">
+        <v>0</v>
+      </c>
+      <c r="E198" s="4">
+        <v>0</v>
       </c>
       <c r="F198" s="4">
         <v>1</v>
       </c>
       <c r="G198" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1192, 265, 46, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1192, 265, 46, 0, 0, 1);</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -30551,18 +30553,18 @@
       <c r="C199" s="4">
         <v>32</v>
       </c>
-      <c r="D199" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E199" s="4" t="s">
-        <v>17</v>
+      <c r="D199" s="4">
+        <v>1</v>
+      </c>
+      <c r="E199" s="4">
+        <v>3</v>
       </c>
       <c r="F199" s="4">
         <v>2</v>
       </c>
       <c r="G199" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1193, 265, 32, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1193, 265, 32, 1, 3, 2);</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
@@ -30577,18 +30579,18 @@
       <c r="C200" s="4">
         <v>32</v>
       </c>
-      <c r="D200" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E200" s="4" t="s">
-        <v>17</v>
+      <c r="D200" s="4">
+        <v>0</v>
+      </c>
+      <c r="E200" s="4">
+        <v>0</v>
       </c>
       <c r="F200" s="4">
         <v>1</v>
       </c>
       <c r="G200" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1194, 265, 32, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1194, 265, 32, 0, 0, 1);</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -31019,18 +31021,18 @@
       <c r="C217" s="3">
         <v>354</v>
       </c>
-      <c r="D217" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E217" s="3" t="s">
-        <v>17</v>
+      <c r="D217" s="3">
+        <v>2</v>
+      </c>
+      <c r="E217" s="3">
+        <v>3</v>
       </c>
       <c r="F217" s="3">
         <v>2</v>
       </c>
       <c r="G217" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1211, 270, 354, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1211, 270, 354, 2, 3, 2);</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -31045,18 +31047,18 @@
       <c r="C218" s="3">
         <v>354</v>
       </c>
-      <c r="D218" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E218" s="3" t="s">
-        <v>17</v>
+      <c r="D218" s="3">
+        <v>1</v>
+      </c>
+      <c r="E218" s="3">
+        <v>0</v>
       </c>
       <c r="F218" s="3">
         <v>1</v>
       </c>
       <c r="G218" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1212, 270, 354, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1212, 270, 354, 1, 0, 1);</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
@@ -31071,18 +31073,18 @@
       <c r="C219" s="3">
         <v>43</v>
       </c>
-      <c r="D219" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E219" s="3" t="s">
-        <v>17</v>
+      <c r="D219" s="3">
+        <v>1</v>
+      </c>
+      <c r="E219" s="3">
+        <v>0</v>
       </c>
       <c r="F219" s="3">
         <v>2</v>
       </c>
       <c r="G219" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1213, 270, 43, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1213, 270, 43, 1, 0, 2);</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
@@ -31097,18 +31099,18 @@
       <c r="C220" s="3">
         <v>43</v>
       </c>
-      <c r="D220" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E220" s="3" t="s">
-        <v>17</v>
+      <c r="D220" s="3">
+        <v>0</v>
+      </c>
+      <c r="E220" s="3">
+        <v>0</v>
       </c>
       <c r="F220" s="3">
         <v>1</v>
       </c>
       <c r="G220" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1214, 270, 43, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1214, 270, 43, 0, 0, 1);</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -31123,18 +31125,18 @@
       <c r="C221" s="4">
         <v>36</v>
       </c>
-      <c r="D221" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E221" s="4" t="s">
-        <v>17</v>
+      <c r="D221" s="4">
+        <v>3</v>
+      </c>
+      <c r="E221" s="4">
+        <v>1</v>
       </c>
       <c r="F221" s="4">
         <v>2</v>
       </c>
       <c r="G221" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1215, 271, 36, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1215, 271, 36, 3, 1, 2);</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
@@ -31149,18 +31151,18 @@
       <c r="C222" s="4">
         <v>36</v>
       </c>
-      <c r="D222" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E222" s="4" t="s">
-        <v>17</v>
+      <c r="D222" s="4">
+        <v>1</v>
+      </c>
+      <c r="E222" s="4">
+        <v>0</v>
       </c>
       <c r="F222" s="4">
         <v>1</v>
       </c>
       <c r="G222" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1216, 271, 36, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1216, 271, 36, 1, 0, 1);</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -31175,18 +31177,18 @@
       <c r="C223" s="4">
         <v>351</v>
       </c>
-      <c r="D223" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E223" s="4" t="s">
-        <v>17</v>
+      <c r="D223" s="4">
+        <v>3</v>
+      </c>
+      <c r="E223" s="4">
+        <v>1</v>
       </c>
       <c r="F223" s="4">
         <v>2</v>
       </c>
       <c r="G223" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1217, 271, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1217, 271, 351, 3, 1, 2);</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -31201,18 +31203,18 @@
       <c r="C224" s="4">
         <v>351</v>
       </c>
-      <c r="D224" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E224" s="4" t="s">
-        <v>17</v>
+      <c r="D224" s="4">
+        <v>1</v>
+      </c>
+      <c r="E224" s="4">
+        <v>0</v>
       </c>
       <c r="F224" s="4">
         <v>1</v>
       </c>
       <c r="G224" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1218, 271, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1218, 271, 351, 1, 0, 1);</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
@@ -31224,8 +31226,8 @@
         <f>B221+1</f>
         <v>272</v>
       </c>
-      <c r="C225" s="3" t="s">
-        <v>17</v>
+      <c r="C225" s="3">
+        <v>41</v>
       </c>
       <c r="D225" s="3" t="s">
         <v>17</v>
@@ -31238,7 +31240,7 @@
       </c>
       <c r="G225" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1219, 272, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1219, 272, 41, null, null, 2);</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -31250,8 +31252,8 @@
         <f>B225</f>
         <v>272</v>
       </c>
-      <c r="C226" s="3" t="s">
-        <v>17</v>
+      <c r="C226" s="3">
+        <v>41</v>
       </c>
       <c r="D226" s="3" t="s">
         <v>17</v>
@@ -31264,7 +31266,7 @@
       </c>
       <c r="G226" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1220, 272, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1220, 272, 41, null, null, 1);</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -31276,8 +31278,8 @@
         <f t="shared" ref="B227:B228" si="25">B225</f>
         <v>272</v>
       </c>
-      <c r="C227" s="3" t="s">
-        <v>17</v>
+      <c r="C227" s="3">
+        <v>48</v>
       </c>
       <c r="D227" s="3" t="s">
         <v>17</v>
@@ -31290,7 +31292,7 @@
       </c>
       <c r="G227" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1221, 272, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1221, 272, 48, null, null, 2);</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -31302,8 +31304,8 @@
         <f t="shared" si="25"/>
         <v>272</v>
       </c>
-      <c r="C228" s="3" t="s">
-        <v>17</v>
+      <c r="C228" s="3">
+        <v>48</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>17</v>
@@ -31316,7 +31318,7 @@
       </c>
       <c r="G228" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1222, 272, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1222, 272, 48, null, null, 1);</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
@@ -31328,8 +31330,8 @@
         <f>B225+1</f>
         <v>273</v>
       </c>
-      <c r="C229" s="4" t="s">
-        <v>17</v>
+      <c r="C229" s="4">
+        <v>4429</v>
       </c>
       <c r="D229" s="4" t="s">
         <v>17</v>
@@ -31342,7 +31344,7 @@
       </c>
       <c r="G229" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1223, 273, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1223, 273, 4429, null, null, 2);</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
@@ -31354,8 +31356,8 @@
         <f>B229</f>
         <v>273</v>
       </c>
-      <c r="C230" s="4" t="s">
-        <v>17</v>
+      <c r="C230" s="4">
+        <v>4429</v>
       </c>
       <c r="D230" s="4" t="s">
         <v>17</v>
@@ -31368,7 +31370,7 @@
       </c>
       <c r="G230" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1224, 273, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1224, 273, 4429, null, null, 1);</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -31380,8 +31382,8 @@
         <f t="shared" ref="B231:B232" si="26">B229</f>
         <v>273</v>
       </c>
-      <c r="C231" s="4" t="s">
-        <v>17</v>
+      <c r="C231" s="4">
+        <v>4428</v>
       </c>
       <c r="D231" s="4" t="s">
         <v>17</v>
@@ -31394,7 +31396,7 @@
       </c>
       <c r="G231" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1225, 273, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1225, 273, 4428, null, null, 2);</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -31406,8 +31408,8 @@
         <f t="shared" si="26"/>
         <v>273</v>
       </c>
-      <c r="C232" s="4" t="s">
-        <v>17</v>
+      <c r="C232" s="4">
+        <v>4428</v>
       </c>
       <c r="D232" s="4" t="s">
         <v>17</v>
@@ -31420,7 +31422,7 @@
       </c>
       <c r="G232" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1226, 273, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1226, 273, 4428, null, null, 1);</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
@@ -31432,8 +31434,8 @@
         <f>B229+1</f>
         <v>274</v>
       </c>
-      <c r="C233" s="3" t="s">
-        <v>17</v>
+      <c r="C233" s="3">
+        <v>385</v>
       </c>
       <c r="D233" s="3" t="s">
         <v>17</v>
@@ -31446,7 +31448,7 @@
       </c>
       <c r="G233" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1227, 274, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1227, 274, 385, null, null, 2);</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -31458,8 +31460,8 @@
         <f>B233</f>
         <v>274</v>
       </c>
-      <c r="C234" s="3" t="s">
-        <v>17</v>
+      <c r="C234" s="3">
+        <v>385</v>
       </c>
       <c r="D234" s="3" t="s">
         <v>17</v>
@@ -31472,7 +31474,7 @@
       </c>
       <c r="G234" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1228, 274, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1228, 274, 385, null, null, 1);</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
@@ -31484,8 +31486,8 @@
         <f t="shared" ref="B235:B236" si="27">B233</f>
         <v>274</v>
       </c>
-      <c r="C235" s="3" t="s">
-        <v>17</v>
+      <c r="C235" s="3">
+        <v>351</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>17</v>
@@ -31498,7 +31500,7 @@
       </c>
       <c r="G235" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1229, 274, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1229, 274, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
@@ -31510,8 +31512,8 @@
         <f t="shared" si="27"/>
         <v>274</v>
       </c>
-      <c r="C236" s="3" t="s">
-        <v>17</v>
+      <c r="C236" s="3">
+        <v>361</v>
       </c>
       <c r="D236" s="3" t="s">
         <v>17</v>
@@ -31524,7 +31526,7 @@
       </c>
       <c r="G236" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1230, 274, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1230, 274, 361, null, null, 1);</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
@@ -31536,8 +31538,8 @@
         <f>B233+1</f>
         <v>275</v>
       </c>
-      <c r="C237" s="4" t="s">
-        <v>17</v>
+      <c r="C237" s="4">
+        <v>33</v>
       </c>
       <c r="D237" s="4" t="s">
         <v>17</v>
@@ -31550,7 +31552,7 @@
       </c>
       <c r="G237" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1231, 275, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1231, 275, 33, null, null, 2);</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
@@ -31562,8 +31564,8 @@
         <f>B237</f>
         <v>275</v>
       </c>
-      <c r="C238" s="4" t="s">
-        <v>17</v>
+      <c r="C238" s="4">
+        <v>33</v>
       </c>
       <c r="D238" s="4" t="s">
         <v>17</v>
@@ -31576,7 +31578,7 @@
       </c>
       <c r="G238" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1232, 275, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1232, 275, 33, null, null, 1);</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
@@ -31588,8 +31590,8 @@
         <f t="shared" ref="B239:B240" si="28">B237</f>
         <v>275</v>
       </c>
-      <c r="C239" s="4" t="s">
-        <v>17</v>
+      <c r="C239" s="4">
+        <v>353</v>
       </c>
       <c r="D239" s="4" t="s">
         <v>17</v>
@@ -31602,7 +31604,7 @@
       </c>
       <c r="G239" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1233, 275, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1233, 275, 353, null, null, 2);</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
@@ -31614,8 +31616,8 @@
         <f t="shared" si="28"/>
         <v>275</v>
       </c>
-      <c r="C240" s="4" t="s">
-        <v>17</v>
+      <c r="C240" s="4">
+        <v>353</v>
       </c>
       <c r="D240" s="4" t="s">
         <v>17</v>
@@ -31628,7 +31630,7 @@
       </c>
       <c r="G240" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1234, 275, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1234, 275, 353, null, null, 1);</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
@@ -31640,8 +31642,8 @@
         <f>B237+1</f>
         <v>276</v>
       </c>
-      <c r="C241" s="3" t="s">
-        <v>17</v>
+      <c r="C241" s="3">
+        <v>49</v>
       </c>
       <c r="D241" s="3" t="s">
         <v>17</v>
@@ -31654,7 +31656,7 @@
       </c>
       <c r="G241" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1235, 276, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1235, 276, 49, null, null, 2);</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -31666,8 +31668,8 @@
         <f>B241</f>
         <v>276</v>
       </c>
-      <c r="C242" s="3" t="s">
-        <v>17</v>
+      <c r="C242" s="3">
+        <v>49</v>
       </c>
       <c r="D242" s="3" t="s">
         <v>17</v>
@@ -31680,7 +31682,7 @@
       </c>
       <c r="G242" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1236, 276, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1236, 276, 49, null, null, 1);</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
@@ -31692,8 +31694,8 @@
         <f t="shared" ref="B243:B244" si="29">B241</f>
         <v>276</v>
       </c>
-      <c r="C243" s="3" t="s">
-        <v>17</v>
+      <c r="C243" s="3">
+        <v>421</v>
       </c>
       <c r="D243" s="3" t="s">
         <v>17</v>
@@ -31706,7 +31708,7 @@
       </c>
       <c r="G243" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1237, 276, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1237, 276, 421, null, null, 2);</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
@@ -31718,8 +31720,8 @@
         <f t="shared" si="29"/>
         <v>276</v>
       </c>
-      <c r="C244" s="3" t="s">
-        <v>17</v>
+      <c r="C244" s="3">
+        <v>421</v>
       </c>
       <c r="D244" s="3" t="s">
         <v>17</v>
@@ -31732,7 +31734,7 @@
       </c>
       <c r="G244" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1238, 276, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1238, 276, 421, null, null, 1);</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
@@ -31744,8 +31746,8 @@
         <f>B241+1</f>
         <v>277</v>
       </c>
-      <c r="C245" s="4" t="s">
-        <v>17</v>
+      <c r="C245" s="4">
+        <v>36</v>
       </c>
       <c r="D245" s="4" t="s">
         <v>17</v>
@@ -31758,7 +31760,7 @@
       </c>
       <c r="G245" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1239, 277, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1239, 277, 36, null, null, 2);</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
@@ -31770,8 +31772,8 @@
         <f>B245</f>
         <v>277</v>
       </c>
-      <c r="C246" s="4" t="s">
-        <v>17</v>
+      <c r="C246" s="4">
+        <v>36</v>
       </c>
       <c r="D246" s="4" t="s">
         <v>17</v>
@@ -31784,7 +31786,7 @@
       </c>
       <c r="G246" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1240, 277, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1240, 277, 36, null, null, 1);</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
@@ -31796,8 +31798,8 @@
         <f t="shared" ref="B247:B248" si="30">B245</f>
         <v>277</v>
       </c>
-      <c r="C247" s="4" t="s">
-        <v>17</v>
+      <c r="C247" s="4">
+        <v>32</v>
       </c>
       <c r="D247" s="4" t="s">
         <v>17</v>
@@ -31810,7 +31812,7 @@
       </c>
       <c r="G247" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1241, 277, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1241, 277, 32, null, null, 2);</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -31822,8 +31824,8 @@
         <f t="shared" si="30"/>
         <v>277</v>
       </c>
-      <c r="C248" s="4" t="s">
-        <v>17</v>
+      <c r="C248" s="4">
+        <v>32</v>
       </c>
       <c r="D248" s="4" t="s">
         <v>17</v>
@@ -31836,7 +31838,7 @@
       </c>
       <c r="G248" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1242, 277, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1242, 277, 32, null, null, 1);</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
@@ -31848,8 +31850,8 @@
         <f>B245+1</f>
         <v>278</v>
       </c>
-      <c r="C249" s="3" t="s">
-        <v>17</v>
+      <c r="C249" s="3">
+        <v>39</v>
       </c>
       <c r="D249" s="3" t="s">
         <v>17</v>
@@ -31862,7 +31864,7 @@
       </c>
       <c r="G249" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1243, 278, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1243, 278, 39, null, null, 2);</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -31874,8 +31876,8 @@
         <f>B249</f>
         <v>278</v>
       </c>
-      <c r="C250" s="3" t="s">
-        <v>17</v>
+      <c r="C250" s="3">
+        <v>39</v>
       </c>
       <c r="D250" s="3" t="s">
         <v>17</v>
@@ -31888,7 +31890,7 @@
       </c>
       <c r="G250" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1244, 278, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1244, 278, 39, null, null, 1);</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
@@ -31900,8 +31902,8 @@
         <f t="shared" ref="B251:B252" si="31">B249</f>
         <v>278</v>
       </c>
-      <c r="C251" s="3" t="s">
-        <v>17</v>
+      <c r="C251" s="3">
+        <v>34</v>
       </c>
       <c r="D251" s="3" t="s">
         <v>17</v>
@@ -31914,7 +31916,7 @@
       </c>
       <c r="G251" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1245, 278, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1245, 278, 34, null, null, 2);</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -31926,8 +31928,8 @@
         <f t="shared" si="31"/>
         <v>278</v>
       </c>
-      <c r="C252" s="3" t="s">
-        <v>17</v>
+      <c r="C252" s="3">
+        <v>34</v>
       </c>
       <c r="D252" s="3" t="s">
         <v>17</v>
@@ -31940,7 +31942,7 @@
       </c>
       <c r="G252" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1246, 278, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1246, 278, 34, null, null, 1);</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -31952,8 +31954,8 @@
         <f>B249+1</f>
         <v>279</v>
       </c>
-      <c r="C253" s="4" t="s">
-        <v>17</v>
+      <c r="C253" s="4">
+        <v>4420</v>
       </c>
       <c r="D253" s="4" t="s">
         <v>17</v>
@@ -31966,7 +31968,7 @@
       </c>
       <c r="G253" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1247, 279, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1247, 279, 4420, null, null, 2);</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -31978,8 +31980,8 @@
         <f>B253</f>
         <v>279</v>
       </c>
-      <c r="C254" s="4" t="s">
-        <v>17</v>
+      <c r="C254" s="4">
+        <v>4420</v>
       </c>
       <c r="D254" s="4" t="s">
         <v>17</v>
@@ -31992,7 +31994,7 @@
       </c>
       <c r="G254" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1248, 279, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1248, 279, 4420, null, null, 1);</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -32004,8 +32006,8 @@
         <f t="shared" ref="B255:B256" si="32">B253</f>
         <v>279</v>
       </c>
-      <c r="C255" s="4" t="s">
-        <v>17</v>
+      <c r="C255" s="4">
+        <v>354</v>
       </c>
       <c r="D255" s="4" t="s">
         <v>17</v>
@@ -32018,7 +32020,7 @@
       </c>
       <c r="G255" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1249, 279, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1249, 279, 354, null, null, 2);</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -32030,8 +32032,8 @@
         <f t="shared" si="32"/>
         <v>279</v>
       </c>
-      <c r="C256" s="4" t="s">
-        <v>17</v>
+      <c r="C256" s="4">
+        <v>354</v>
       </c>
       <c r="D256" s="4" t="s">
         <v>17</v>
@@ -32044,7 +32046,7 @@
       </c>
       <c r="G256" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1250, 279, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1250, 279, 354, null, null, 1);</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Eurocopa Round of 16 first date
Eurocopa Round of 16 first date
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -25494,9 +25494,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J284"/>
+  <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -30405,7 +30407,7 @@
         <v>2</v>
       </c>
       <c r="G193" s="3" t="str">
-        <f t="shared" ref="G193:G256" si="15">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A193 &amp; ", " &amp; B193 &amp; ", " &amp; C193 &amp; ", " &amp; D193 &amp; ", " &amp; E193 &amp; ", " &amp; F193 &amp; ");"</f>
+        <f t="shared" ref="G193:G266" si="15">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A193 &amp; ", " &amp; B193 &amp; ", " &amp; C193 &amp; ", " &amp; D193 &amp; ", " &amp; E193 &amp; ", " &amp; F193 &amp; ");"</f>
         <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1187, 264, 39, 0, 0, 2);</v>
       </c>
     </row>
@@ -30853,7 +30855,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
-        <f t="shared" ref="A211:A274" si="20">A210+1</f>
+        <f t="shared" ref="A211:A284" si="20">A210+1</f>
         <v>1205</v>
       </c>
       <c r="B211" s="3">
@@ -31227,18 +31229,18 @@
       <c r="C225" s="3">
         <v>41</v>
       </c>
-      <c r="D225" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E225" s="3" t="s">
-        <v>17</v>
+      <c r="D225" s="3">
+        <v>1</v>
+      </c>
+      <c r="E225" s="3">
+        <v>0</v>
       </c>
       <c r="F225" s="3">
         <v>2</v>
       </c>
       <c r="G225" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1219, 272, 41, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1219, 272, 41, 1, 0, 2);</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -31253,18 +31255,18 @@
       <c r="C226" s="3">
         <v>41</v>
       </c>
-      <c r="D226" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E226" s="3" t="s">
-        <v>17</v>
+      <c r="D226" s="3">
+        <v>0</v>
+      </c>
+      <c r="E226" s="3">
+        <v>0</v>
       </c>
       <c r="F226" s="3">
         <v>1</v>
       </c>
       <c r="G226" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1220, 272, 41, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1220, 272, 41, 0, 0, 1);</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -31273,24 +31275,24 @@
         <v>1221</v>
       </c>
       <c r="B227" s="3">
-        <f t="shared" ref="B227:B228" si="25">B225</f>
+        <f t="shared" ref="B227:B234" si="25">B226</f>
         <v>272</v>
       </c>
       <c r="C227" s="3">
         <v>48</v>
       </c>
-      <c r="D227" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E227" s="3" t="s">
-        <v>17</v>
+      <c r="D227" s="3">
+        <v>1</v>
+      </c>
+      <c r="E227" s="3">
+        <v>0</v>
       </c>
       <c r="F227" s="3">
         <v>2</v>
       </c>
       <c r="G227" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1221, 272, 48, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1221, 272, 48, 1, 0, 2);</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -31305,122 +31307,122 @@
       <c r="C228" s="3">
         <v>48</v>
       </c>
-      <c r="D228" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E228" s="3" t="s">
-        <v>17</v>
+      <c r="D228" s="3">
+        <v>1</v>
+      </c>
+      <c r="E228" s="3">
+        <v>0</v>
       </c>
       <c r="F228" s="3">
         <v>1</v>
       </c>
       <c r="G228" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1222, 272, 48, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1222, 272, 48, 1, 0, 1);</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A229" s="4">
+      <c r="A229" s="3">
         <f t="shared" si="20"/>
         <v>1223</v>
       </c>
-      <c r="B229" s="4">
-        <f>B225+1</f>
-        <v>273</v>
-      </c>
-      <c r="C229" s="4">
-        <v>4429</v>
-      </c>
-      <c r="D229" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E229" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F229" s="4">
-        <v>2</v>
-      </c>
-      <c r="G229" s="4" t="str">
+      <c r="B229" s="3">
+        <f t="shared" si="25"/>
+        <v>272</v>
+      </c>
+      <c r="C229" s="3">
+        <v>41</v>
+      </c>
+      <c r="D229" s="3">
+        <v>1</v>
+      </c>
+      <c r="E229" s="3">
+        <v>1</v>
+      </c>
+      <c r="F229" s="3">
+        <v>4</v>
+      </c>
+      <c r="G229" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1223, 273, 4429, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1223, 272, 41, 1, 1, 4);</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A230" s="4">
+      <c r="A230" s="3">
         <f t="shared" si="20"/>
         <v>1224</v>
       </c>
-      <c r="B230" s="4">
-        <f>B229</f>
-        <v>273</v>
-      </c>
-      <c r="C230" s="4">
-        <v>4429</v>
-      </c>
-      <c r="D230" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E230" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F230" s="4">
-        <v>1</v>
-      </c>
-      <c r="G230" s="4" t="str">
+      <c r="B230" s="3">
+        <f t="shared" si="25"/>
+        <v>272</v>
+      </c>
+      <c r="C230" s="3">
+        <v>41</v>
+      </c>
+      <c r="D230" s="3">
+        <v>1</v>
+      </c>
+      <c r="E230" s="3">
+        <v>0</v>
+      </c>
+      <c r="F230" s="3">
+        <v>3</v>
+      </c>
+      <c r="G230" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1224, 273, 4429, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1224, 272, 41, 1, 0, 3);</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A231" s="4">
+      <c r="A231" s="3">
         <f t="shared" si="20"/>
         <v>1225</v>
       </c>
-      <c r="B231" s="4">
-        <f t="shared" ref="B231:B232" si="26">B229</f>
-        <v>273</v>
-      </c>
-      <c r="C231" s="4">
-        <v>4428</v>
-      </c>
-      <c r="D231" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E231" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F231" s="4">
-        <v>2</v>
-      </c>
-      <c r="G231" s="4" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1225, 273, 4428, null, null, 2);</v>
+      <c r="B231" s="3">
+        <f t="shared" si="25"/>
+        <v>272</v>
+      </c>
+      <c r="C231" s="3">
+        <v>48</v>
+      </c>
+      <c r="D231" s="3">
+        <v>1</v>
+      </c>
+      <c r="E231" s="3">
+        <v>1</v>
+      </c>
+      <c r="F231" s="3">
+        <v>4</v>
+      </c>
+      <c r="G231" s="3" t="str">
+        <f t="shared" ref="G231:G232" si="26">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A231 &amp; ", " &amp; B231 &amp; ", " &amp; C231 &amp; ", " &amp; D231 &amp; ", " &amp; E231 &amp; ", " &amp; F231 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1225, 272, 48, 1, 1, 4);</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A232" s="4">
+      <c r="A232" s="3">
         <f t="shared" si="20"/>
         <v>1226</v>
       </c>
-      <c r="B232" s="4">
+      <c r="B232" s="3">
+        <f t="shared" si="25"/>
+        <v>272</v>
+      </c>
+      <c r="C232" s="3">
+        <v>48</v>
+      </c>
+      <c r="D232" s="3">
+        <v>1</v>
+      </c>
+      <c r="E232" s="3">
+        <v>0</v>
+      </c>
+      <c r="F232" s="3">
+        <v>3</v>
+      </c>
+      <c r="G232" s="3" t="str">
         <f t="shared" si="26"/>
-        <v>273</v>
-      </c>
-      <c r="C232" s="4">
-        <v>4428</v>
-      </c>
-      <c r="D232" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E232" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F232" s="4">
-        <v>1</v>
-      </c>
-      <c r="G232" s="4" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1226, 273, 4428, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1226, 272, 48, 1, 0, 3);</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
@@ -31429,24 +31431,24 @@
         <v>1227</v>
       </c>
       <c r="B233" s="3">
-        <f>B229+1</f>
-        <v>274</v>
+        <f t="shared" si="25"/>
+        <v>272</v>
       </c>
       <c r="C233" s="3">
-        <v>385</v>
-      </c>
-      <c r="D233" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E233" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
+      </c>
+      <c r="D233" s="3">
+        <v>4</v>
+      </c>
+      <c r="E233" s="3">
+        <v>0</v>
       </c>
       <c r="F233" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G233" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1227, 274, 385, null, null, 2);</v>
+        <f t="shared" ref="G233:G234" si="27">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A233 &amp; ", " &amp; B233 &amp; ", " &amp; C233 &amp; ", " &amp; D233 &amp; ", " &amp; E233 &amp; ", " &amp; F233 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1227, 272, 41, 4, 0, 7);</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -31455,76 +31457,76 @@
         <v>1228</v>
       </c>
       <c r="B234" s="3">
-        <f>B233</f>
-        <v>274</v>
+        <f t="shared" si="25"/>
+        <v>272</v>
       </c>
       <c r="C234" s="3">
-        <v>385</v>
-      </c>
-      <c r="D234" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E234" s="3" t="s">
-        <v>17</v>
+        <v>48</v>
+      </c>
+      <c r="D234" s="3">
+        <v>5</v>
+      </c>
+      <c r="E234" s="3">
+        <v>0</v>
       </c>
       <c r="F234" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G234" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1228, 274, 385, null, null, 1);</v>
+        <f t="shared" si="27"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1228, 272, 48, 5, 0, 7);</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A235" s="3">
+      <c r="A235" s="4">
         <f t="shared" si="20"/>
         <v>1229</v>
       </c>
-      <c r="B235" s="3">
-        <f t="shared" ref="B235:B236" si="27">B233</f>
-        <v>274</v>
-      </c>
-      <c r="C235" s="3">
-        <v>351</v>
-      </c>
-      <c r="D235" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E235" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F235" s="3">
-        <v>2</v>
-      </c>
-      <c r="G235" s="3" t="str">
+      <c r="B235" s="4">
+        <f>B225+1</f>
+        <v>273</v>
+      </c>
+      <c r="C235" s="4">
+        <v>4429</v>
+      </c>
+      <c r="D235" s="4">
+        <v>1</v>
+      </c>
+      <c r="E235" s="4">
+        <v>3</v>
+      </c>
+      <c r="F235" s="4">
+        <v>2</v>
+      </c>
+      <c r="G235" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1229, 274, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1229, 273, 4429, 1, 3, 2);</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A236" s="3">
+      <c r="A236" s="4">
         <f t="shared" si="20"/>
         <v>1230</v>
       </c>
-      <c r="B236" s="3">
-        <f t="shared" si="27"/>
-        <v>274</v>
-      </c>
-      <c r="C236" s="3">
-        <v>361</v>
-      </c>
-      <c r="D236" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E236" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F236" s="3">
-        <v>1</v>
-      </c>
-      <c r="G236" s="3" t="str">
+      <c r="B236" s="4">
+        <f>B235</f>
+        <v>273</v>
+      </c>
+      <c r="C236" s="4">
+        <v>4429</v>
+      </c>
+      <c r="D236" s="4">
+        <v>0</v>
+      </c>
+      <c r="E236" s="4">
+        <v>0</v>
+      </c>
+      <c r="F236" s="4">
+        <v>1</v>
+      </c>
+      <c r="G236" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1230, 274, 361, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1230, 273, 4429, 0, 0, 1);</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
@@ -31533,24 +31535,24 @@
         <v>1231</v>
       </c>
       <c r="B237" s="4">
-        <f>B233+1</f>
-        <v>275</v>
+        <f t="shared" ref="B237:B238" si="28">B235</f>
+        <v>273</v>
       </c>
       <c r="C237" s="4">
-        <v>33</v>
-      </c>
-      <c r="D237" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E237" s="4" t="s">
-        <v>17</v>
+        <v>4428</v>
+      </c>
+      <c r="D237" s="4">
+        <v>0</v>
+      </c>
+      <c r="E237" s="4">
+        <v>0</v>
       </c>
       <c r="F237" s="4">
         <v>2</v>
       </c>
       <c r="G237" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1231, 275, 33, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1231, 273, 4428, 0, 0, 2);</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
@@ -31559,76 +31561,76 @@
         <v>1232</v>
       </c>
       <c r="B238" s="4">
-        <f>B237</f>
-        <v>275</v>
+        <f t="shared" si="28"/>
+        <v>273</v>
       </c>
       <c r="C238" s="4">
-        <v>33</v>
-      </c>
-      <c r="D238" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E238" s="4" t="s">
-        <v>17</v>
+        <v>4428</v>
+      </c>
+      <c r="D238" s="4">
+        <v>0</v>
+      </c>
+      <c r="E238" s="4">
+        <v>0</v>
       </c>
       <c r="F238" s="4">
         <v>1</v>
       </c>
       <c r="G238" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1232, 275, 33, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1232, 273, 4428, 0, 0, 1);</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A239" s="4">
+      <c r="A239" s="3">
         <f t="shared" si="20"/>
         <v>1233</v>
       </c>
-      <c r="B239" s="4">
-        <f t="shared" ref="B239:B240" si="28">B237</f>
-        <v>275</v>
-      </c>
-      <c r="C239" s="4">
-        <v>353</v>
-      </c>
-      <c r="D239" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E239" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F239" s="4">
-        <v>2</v>
-      </c>
-      <c r="G239" s="4" t="str">
+      <c r="B239" s="3">
+        <f>B235+1</f>
+        <v>274</v>
+      </c>
+      <c r="C239" s="3">
+        <v>385</v>
+      </c>
+      <c r="D239" s="3">
+        <v>0</v>
+      </c>
+      <c r="E239" s="3">
+        <v>0</v>
+      </c>
+      <c r="F239" s="3">
+        <v>2</v>
+      </c>
+      <c r="G239" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1233, 275, 353, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1233, 274, 385, 0, 0, 2);</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A240" s="4">
+      <c r="A240" s="3">
         <f t="shared" si="20"/>
         <v>1234</v>
       </c>
-      <c r="B240" s="4">
-        <f t="shared" si="28"/>
-        <v>275</v>
-      </c>
-      <c r="C240" s="4">
-        <v>353</v>
-      </c>
-      <c r="D240" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E240" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F240" s="4">
-        <v>1</v>
-      </c>
-      <c r="G240" s="4" t="str">
+      <c r="B240" s="3">
+        <f>B239</f>
+        <v>274</v>
+      </c>
+      <c r="C240" s="3">
+        <v>385</v>
+      </c>
+      <c r="D240" s="3">
+        <v>0</v>
+      </c>
+      <c r="E240" s="3">
+        <v>0</v>
+      </c>
+      <c r="F240" s="3">
+        <v>1</v>
+      </c>
+      <c r="G240" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1234, 275, 353, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1234, 274, 385, 0, 0, 1);</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
@@ -31637,24 +31639,24 @@
         <v>1235</v>
       </c>
       <c r="B241" s="3">
-        <f>B237+1</f>
-        <v>276</v>
+        <f t="shared" ref="B241:B242" si="29">B239</f>
+        <v>274</v>
       </c>
       <c r="C241" s="3">
-        <v>49</v>
-      </c>
-      <c r="D241" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E241" s="3" t="s">
-        <v>17</v>
+        <v>351</v>
+      </c>
+      <c r="D241" s="3">
+        <v>0</v>
+      </c>
+      <c r="E241" s="3">
+        <v>0</v>
       </c>
       <c r="F241" s="3">
         <v>2</v>
       </c>
       <c r="G241" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1235, 276, 49, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1235, 274, 351, 0, 0, 2);</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
@@ -31663,24 +31665,24 @@
         <v>1236</v>
       </c>
       <c r="B242" s="3">
-        <f>B241</f>
-        <v>276</v>
+        <f t="shared" si="29"/>
+        <v>274</v>
       </c>
       <c r="C242" s="3">
-        <v>49</v>
-      </c>
-      <c r="D242" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E242" s="3" t="s">
-        <v>17</v>
+        <v>351</v>
+      </c>
+      <c r="D242" s="3">
+        <v>0</v>
+      </c>
+      <c r="E242" s="3">
+        <v>0</v>
       </c>
       <c r="F242" s="3">
         <v>1</v>
       </c>
       <c r="G242" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1236, 276, 49, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1236, 274, 351, 0, 0, 1);</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
@@ -31689,24 +31691,24 @@
         <v>1237</v>
       </c>
       <c r="B243" s="3">
-        <f t="shared" ref="B243:B244" si="29">B241</f>
-        <v>276</v>
+        <f>B242</f>
+        <v>274</v>
       </c>
       <c r="C243" s="3">
-        <v>421</v>
-      </c>
-      <c r="D243" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E243" s="3" t="s">
-        <v>17</v>
+        <v>385</v>
+      </c>
+      <c r="D243" s="3">
+        <v>0</v>
+      </c>
+      <c r="E243" s="3">
+        <v>0</v>
       </c>
       <c r="F243" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G243" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1237, 276, 421, null, null, 2);</v>
+        <f t="shared" ref="G243:G246" si="30">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A243 &amp; ", " &amp; B243 &amp; ", " &amp; C243 &amp; ", " &amp; D243 &amp; ", " &amp; E243 &amp; ", " &amp; F243 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1237, 274, 385, 0, 0, 4);</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
@@ -31715,89 +31717,89 @@
         <v>1238</v>
       </c>
       <c r="B244" s="3">
-        <f t="shared" si="29"/>
-        <v>276</v>
+        <f>B243</f>
+        <v>274</v>
       </c>
       <c r="C244" s="3">
-        <v>421</v>
-      </c>
-      <c r="D244" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E244" s="3" t="s">
-        <v>17</v>
+        <v>385</v>
+      </c>
+      <c r="D244" s="3">
+        <v>0</v>
+      </c>
+      <c r="E244" s="3">
+        <v>0</v>
       </c>
       <c r="F244" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G244" s="3" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1238, 276, 421, null, null, 1);</v>
+        <f t="shared" si="30"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1238, 274, 385, 0, 0, 3);</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A245" s="4">
+      <c r="A245" s="3">
         <f t="shared" si="20"/>
         <v>1239</v>
       </c>
-      <c r="B245" s="4">
-        <f>B241+1</f>
-        <v>277</v>
-      </c>
-      <c r="C245" s="4">
-        <v>36</v>
-      </c>
-      <c r="D245" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E245" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F245" s="4">
-        <v>2</v>
-      </c>
-      <c r="G245" s="4" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1239, 277, 36, null, null, 2);</v>
+      <c r="B245" s="3">
+        <f t="shared" ref="B245:B246" si="31">B243</f>
+        <v>274</v>
+      </c>
+      <c r="C245" s="3">
+        <v>351</v>
+      </c>
+      <c r="D245" s="3">
+        <v>1</v>
+      </c>
+      <c r="E245" s="3">
+        <v>3</v>
+      </c>
+      <c r="F245" s="3">
+        <v>4</v>
+      </c>
+      <c r="G245" s="3" t="str">
+        <f t="shared" si="30"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1239, 274, 351, 1, 3, 4);</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A246" s="4">
+      <c r="A246" s="3">
         <f t="shared" si="20"/>
         <v>1240</v>
       </c>
-      <c r="B246" s="4">
-        <f>B245</f>
-        <v>277</v>
-      </c>
-      <c r="C246" s="4">
-        <v>36</v>
-      </c>
-      <c r="D246" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E246" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F246" s="4">
-        <v>1</v>
-      </c>
-      <c r="G246" s="4" t="str">
-        <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1240, 277, 36, null, null, 1);</v>
+      <c r="B246" s="3">
+        <f t="shared" si="31"/>
+        <v>274</v>
+      </c>
+      <c r="C246" s="3">
+        <v>351</v>
+      </c>
+      <c r="D246" s="3">
+        <v>0</v>
+      </c>
+      <c r="E246" s="3">
+        <v>0</v>
+      </c>
+      <c r="F246" s="3">
+        <v>3</v>
+      </c>
+      <c r="G246" s="3" t="str">
+        <f t="shared" si="30"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1240, 274, 351, 0, 0, 3);</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247" s="4">
-        <f t="shared" si="20"/>
+        <f>A246+1</f>
         <v>1241</v>
       </c>
       <c r="B247" s="4">
-        <f t="shared" ref="B247:B248" si="30">B245</f>
-        <v>277</v>
+        <f>B239+1</f>
+        <v>275</v>
       </c>
       <c r="C247" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D247" s="4" t="s">
         <v>17</v>
@@ -31810,7 +31812,7 @@
       </c>
       <c r="G247" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1241, 277, 32, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1241, 275, 33, null, null, 2);</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -31819,11 +31821,11 @@
         <v>1242</v>
       </c>
       <c r="B248" s="4">
-        <f t="shared" si="30"/>
-        <v>277</v>
+        <f>B247</f>
+        <v>275</v>
       </c>
       <c r="C248" s="4">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D248" s="4" t="s">
         <v>17</v>
@@ -31836,59 +31838,59 @@
       </c>
       <c r="G248" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1242, 277, 32, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1242, 275, 33, null, null, 1);</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A249" s="3">
+      <c r="A249" s="4">
         <f t="shared" si="20"/>
         <v>1243</v>
       </c>
-      <c r="B249" s="3">
-        <f>B245+1</f>
-        <v>278</v>
-      </c>
-      <c r="C249" s="3">
-        <v>39</v>
-      </c>
-      <c r="D249" s="3" t="s">
+      <c r="B249" s="4">
+        <f t="shared" ref="B249:B250" si="32">B247</f>
+        <v>275</v>
+      </c>
+      <c r="C249" s="4">
+        <v>353</v>
+      </c>
+      <c r="D249" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E249" s="3" t="s">
+      <c r="E249" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F249" s="3">
-        <v>2</v>
-      </c>
-      <c r="G249" s="3" t="str">
+      <c r="F249" s="4">
+        <v>2</v>
+      </c>
+      <c r="G249" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1243, 278, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1243, 275, 353, null, null, 2);</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A250" s="3">
+      <c r="A250" s="4">
         <f t="shared" si="20"/>
         <v>1244</v>
       </c>
-      <c r="B250" s="3">
-        <f>B249</f>
-        <v>278</v>
-      </c>
-      <c r="C250" s="3">
-        <v>39</v>
-      </c>
-      <c r="D250" s="3" t="s">
+      <c r="B250" s="4">
+        <f t="shared" si="32"/>
+        <v>275</v>
+      </c>
+      <c r="C250" s="4">
+        <v>353</v>
+      </c>
+      <c r="D250" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E250" s="3" t="s">
+      <c r="E250" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F250" s="3">
-        <v>1</v>
-      </c>
-      <c r="G250" s="3" t="str">
+      <c r="F250" s="4">
+        <v>1</v>
+      </c>
+      <c r="G250" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1244, 278, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1244, 275, 353, null, null, 1);</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
@@ -31897,11 +31899,11 @@
         <v>1245</v>
       </c>
       <c r="B251" s="3">
-        <f t="shared" ref="B251:B252" si="31">B249</f>
-        <v>278</v>
+        <f>B247+1</f>
+        <v>276</v>
       </c>
       <c r="C251" s="3">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D251" s="3" t="s">
         <v>17</v>
@@ -31914,7 +31916,7 @@
       </c>
       <c r="G251" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1245, 278, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1245, 276, 49, null, null, 2);</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -31923,11 +31925,11 @@
         <v>1246</v>
       </c>
       <c r="B252" s="3">
-        <f t="shared" si="31"/>
-        <v>278</v>
+        <f>B251</f>
+        <v>276</v>
       </c>
       <c r="C252" s="3">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D252" s="3" t="s">
         <v>17</v>
@@ -31940,59 +31942,59 @@
       </c>
       <c r="G252" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1246, 278, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1246, 276, 49, null, null, 1);</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" s="4">
+      <c r="A253" s="3">
         <f t="shared" si="20"/>
         <v>1247</v>
       </c>
-      <c r="B253" s="4">
-        <f>B249+1</f>
-        <v>279</v>
-      </c>
-      <c r="C253" s="4">
-        <v>4420</v>
-      </c>
-      <c r="D253" s="4" t="s">
+      <c r="B253" s="3">
+        <f t="shared" ref="B253:B254" si="33">B251</f>
+        <v>276</v>
+      </c>
+      <c r="C253" s="3">
+        <v>421</v>
+      </c>
+      <c r="D253" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E253" s="4" t="s">
+      <c r="E253" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F253" s="4">
-        <v>2</v>
-      </c>
-      <c r="G253" s="4" t="str">
+      <c r="F253" s="3">
+        <v>2</v>
+      </c>
+      <c r="G253" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1247, 279, 4420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1247, 276, 421, null, null, 2);</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A254" s="4">
+      <c r="A254" s="3">
         <f t="shared" si="20"/>
         <v>1248</v>
       </c>
-      <c r="B254" s="4">
-        <f>B253</f>
-        <v>279</v>
-      </c>
-      <c r="C254" s="4">
-        <v>4420</v>
-      </c>
-      <c r="D254" s="4" t="s">
+      <c r="B254" s="3">
+        <f t="shared" si="33"/>
+        <v>276</v>
+      </c>
+      <c r="C254" s="3">
+        <v>421</v>
+      </c>
+      <c r="D254" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E254" s="4" t="s">
+      <c r="E254" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F254" s="4">
-        <v>1</v>
-      </c>
-      <c r="G254" s="4" t="str">
+      <c r="F254" s="3">
+        <v>1</v>
+      </c>
+      <c r="G254" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1248, 279, 4420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1248, 276, 421, null, null, 1);</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -32001,11 +32003,11 @@
         <v>1249</v>
       </c>
       <c r="B255" s="4">
-        <f t="shared" ref="B255:B256" si="32">B253</f>
-        <v>279</v>
+        <f>B251+1</f>
+        <v>277</v>
       </c>
       <c r="C255" s="4">
-        <v>354</v>
+        <v>36</v>
       </c>
       <c r="D255" s="4" t="s">
         <v>17</v>
@@ -32018,7 +32020,7 @@
       </c>
       <c r="G255" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1249, 279, 354, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1249, 277, 36, null, null, 2);</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -32027,11 +32029,11 @@
         <v>1250</v>
       </c>
       <c r="B256" s="4">
-        <f t="shared" si="32"/>
-        <v>279</v>
+        <f>B255</f>
+        <v>277</v>
       </c>
       <c r="C256" s="4">
-        <v>354</v>
+        <v>36</v>
       </c>
       <c r="D256" s="4" t="s">
         <v>17</v>
@@ -32044,59 +32046,59 @@
       </c>
       <c r="G256" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1250, 279, 354, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1250, 277, 36, null, null, 1);</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A257" s="3">
+      <c r="A257" s="4">
         <f t="shared" si="20"/>
         <v>1251</v>
       </c>
-      <c r="B257" s="3">
-        <f>B253+1</f>
-        <v>280</v>
-      </c>
-      <c r="C257" s="3" t="s">
+      <c r="B257" s="4">
+        <f t="shared" ref="B257:B258" si="34">B255</f>
+        <v>277</v>
+      </c>
+      <c r="C257" s="4">
+        <v>32</v>
+      </c>
+      <c r="D257" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D257" s="3" t="s">
+      <c r="E257" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E257" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F257" s="3">
-        <v>2</v>
-      </c>
-      <c r="G257" s="3" t="str">
-        <f t="shared" ref="G257:G284" si="33">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A257 &amp; ", " &amp; B257 &amp; ", " &amp; C257 &amp; ", " &amp; D257 &amp; ", " &amp; E257 &amp; ", " &amp; F257 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1251, 280, null, null, null, 2);</v>
+      <c r="F257" s="4">
+        <v>2</v>
+      </c>
+      <c r="G257" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1251, 277, 32, null, null, 2);</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A258" s="3">
+      <c r="A258" s="4">
         <f t="shared" si="20"/>
         <v>1252</v>
       </c>
-      <c r="B258" s="3">
-        <f>B257</f>
-        <v>280</v>
-      </c>
-      <c r="C258" s="3" t="s">
+      <c r="B258" s="4">
+        <f t="shared" si="34"/>
+        <v>277</v>
+      </c>
+      <c r="C258" s="4">
+        <v>32</v>
+      </c>
+      <c r="D258" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D258" s="3" t="s">
+      <c r="E258" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E258" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F258" s="3">
-        <v>1</v>
-      </c>
-      <c r="G258" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1252, 280, null, null, null, 1);</v>
+      <c r="F258" s="4">
+        <v>1</v>
+      </c>
+      <c r="G258" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1252, 277, 32, null, null, 1);</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
@@ -32105,11 +32107,11 @@
         <v>1253</v>
       </c>
       <c r="B259" s="3">
-        <f t="shared" ref="B259:B260" si="34">B257</f>
-        <v>280</v>
-      </c>
-      <c r="C259" s="3" t="s">
-        <v>17</v>
+        <f>B255+1</f>
+        <v>278</v>
+      </c>
+      <c r="C259" s="3">
+        <v>39</v>
       </c>
       <c r="D259" s="3" t="s">
         <v>17</v>
@@ -32121,8 +32123,8 @@
         <v>2</v>
       </c>
       <c r="G259" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1253, 280, null, null, null, 2);</v>
+        <f t="shared" si="15"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1253, 278, 39, null, null, 2);</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
@@ -32131,11 +32133,11 @@
         <v>1254</v>
       </c>
       <c r="B260" s="3">
-        <f t="shared" si="34"/>
-        <v>280</v>
-      </c>
-      <c r="C260" s="3" t="s">
-        <v>17</v>
+        <f>B259</f>
+        <v>278</v>
+      </c>
+      <c r="C260" s="3">
+        <v>39</v>
       </c>
       <c r="D260" s="3" t="s">
         <v>17</v>
@@ -32147,60 +32149,60 @@
         <v>1</v>
       </c>
       <c r="G260" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1254, 280, null, null, null, 1);</v>
+        <f t="shared" si="15"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1254, 278, 39, null, null, 1);</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A261" s="4">
+      <c r="A261" s="3">
         <f t="shared" si="20"/>
         <v>1255</v>
       </c>
-      <c r="B261" s="4">
-        <f>B257+1</f>
-        <v>281</v>
-      </c>
-      <c r="C261" s="4" t="s">
+      <c r="B261" s="3">
+        <f t="shared" ref="B261:B262" si="35">B259</f>
+        <v>278</v>
+      </c>
+      <c r="C261" s="3">
+        <v>34</v>
+      </c>
+      <c r="D261" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D261" s="4" t="s">
+      <c r="E261" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E261" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F261" s="4">
-        <v>2</v>
-      </c>
-      <c r="G261" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1255, 281, null, null, null, 2);</v>
+      <c r="F261" s="3">
+        <v>2</v>
+      </c>
+      <c r="G261" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1255, 278, 34, null, null, 2);</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A262" s="4">
+      <c r="A262" s="3">
         <f t="shared" si="20"/>
         <v>1256</v>
       </c>
-      <c r="B262" s="4">
-        <f>B261</f>
-        <v>281</v>
-      </c>
-      <c r="C262" s="4" t="s">
+      <c r="B262" s="3">
+        <f t="shared" si="35"/>
+        <v>278</v>
+      </c>
+      <c r="C262" s="3">
+        <v>34</v>
+      </c>
+      <c r="D262" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D262" s="4" t="s">
+      <c r="E262" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E262" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F262" s="4">
-        <v>1</v>
-      </c>
-      <c r="G262" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1256, 281, null, null, null, 1);</v>
+      <c r="F262" s="3">
+        <v>1</v>
+      </c>
+      <c r="G262" s="3" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1256, 278, 34, null, null, 1);</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
@@ -32209,11 +32211,11 @@
         <v>1257</v>
       </c>
       <c r="B263" s="4">
-        <f t="shared" ref="B263:B264" si="35">B261</f>
-        <v>281</v>
-      </c>
-      <c r="C263" s="4" t="s">
-        <v>17</v>
+        <f>B259+1</f>
+        <v>279</v>
+      </c>
+      <c r="C263" s="4">
+        <v>4420</v>
       </c>
       <c r="D263" s="4" t="s">
         <v>17</v>
@@ -32225,8 +32227,8 @@
         <v>2</v>
       </c>
       <c r="G263" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1257, 281, null, null, null, 2);</v>
+        <f t="shared" si="15"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1257, 279, 4420, null, null, 2);</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
@@ -32235,11 +32237,11 @@
         <v>1258</v>
       </c>
       <c r="B264" s="4">
-        <f t="shared" si="35"/>
-        <v>281</v>
-      </c>
-      <c r="C264" s="4" t="s">
-        <v>17</v>
+        <f>B263</f>
+        <v>279</v>
+      </c>
+      <c r="C264" s="4">
+        <v>4420</v>
       </c>
       <c r="D264" s="4" t="s">
         <v>17</v>
@@ -32251,60 +32253,60 @@
         <v>1</v>
       </c>
       <c r="G264" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1258, 281, null, null, null, 1);</v>
+        <f t="shared" si="15"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1258, 279, 4420, null, null, 1);</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A265" s="3">
+      <c r="A265" s="4">
         <f t="shared" si="20"/>
         <v>1259</v>
       </c>
-      <c r="B265" s="3">
-        <f>B261+1</f>
-        <v>282</v>
-      </c>
-      <c r="C265" s="3" t="s">
+      <c r="B265" s="4">
+        <f t="shared" ref="B265:B266" si="36">B263</f>
+        <v>279</v>
+      </c>
+      <c r="C265" s="4">
+        <v>354</v>
+      </c>
+      <c r="D265" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D265" s="3" t="s">
+      <c r="E265" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E265" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F265" s="3">
-        <v>2</v>
-      </c>
-      <c r="G265" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1259, 282, null, null, null, 2);</v>
+      <c r="F265" s="4">
+        <v>2</v>
+      </c>
+      <c r="G265" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1259, 279, 354, null, null, 2);</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A266" s="3">
+      <c r="A266" s="4">
         <f t="shared" si="20"/>
         <v>1260</v>
       </c>
-      <c r="B266" s="3">
-        <f>B265</f>
-        <v>282</v>
-      </c>
-      <c r="C266" s="3" t="s">
+      <c r="B266" s="4">
+        <f t="shared" si="36"/>
+        <v>279</v>
+      </c>
+      <c r="C266" s="4">
+        <v>354</v>
+      </c>
+      <c r="D266" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D266" s="3" t="s">
+      <c r="E266" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E266" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F266" s="3">
-        <v>1</v>
-      </c>
-      <c r="G266" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1260, 282, null, null, null, 1);</v>
+      <c r="F266" s="4">
+        <v>1</v>
+      </c>
+      <c r="G266" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1260, 279, 354, null, null, 1);</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
@@ -32313,8 +32315,8 @@
         <v>1261</v>
       </c>
       <c r="B267" s="3">
-        <f t="shared" ref="B267:B268" si="36">B265</f>
-        <v>282</v>
+        <f>B263+1</f>
+        <v>280</v>
       </c>
       <c r="C267" s="3" t="s">
         <v>17</v>
@@ -32329,8 +32331,8 @@
         <v>2</v>
       </c>
       <c r="G267" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1261, 282, null, null, null, 2);</v>
+        <f t="shared" ref="G267:G294" si="37">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A267 &amp; ", " &amp; B267 &amp; ", " &amp; C267 &amp; ", " &amp; D267 &amp; ", " &amp; E267 &amp; ", " &amp; F267 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1261, 280, null, null, null, 2);</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
@@ -32339,8 +32341,8 @@
         <v>1262</v>
       </c>
       <c r="B268" s="3">
-        <f t="shared" si="36"/>
-        <v>282</v>
+        <f>B267</f>
+        <v>280</v>
       </c>
       <c r="C268" s="3" t="s">
         <v>17</v>
@@ -32355,60 +32357,60 @@
         <v>1</v>
       </c>
       <c r="G268" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1262, 282, null, null, null, 1);</v>
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1262, 280, null, null, null, 1);</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A269" s="4">
+      <c r="A269" s="3">
         <f t="shared" si="20"/>
         <v>1263</v>
       </c>
-      <c r="B269" s="4">
-        <f>B265+1</f>
-        <v>283</v>
-      </c>
-      <c r="C269" s="4" t="s">
+      <c r="B269" s="3">
+        <f t="shared" ref="B269:B270" si="38">B267</f>
+        <v>280</v>
+      </c>
+      <c r="C269" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D269" s="4" t="s">
+      <c r="D269" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E269" s="4" t="s">
+      <c r="E269" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F269" s="4">
-        <v>2</v>
-      </c>
-      <c r="G269" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1263, 283, null, null, null, 2);</v>
+      <c r="F269" s="3">
+        <v>2</v>
+      </c>
+      <c r="G269" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1263, 280, null, null, null, 2);</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A270" s="4">
+      <c r="A270" s="3">
         <f t="shared" si="20"/>
         <v>1264</v>
       </c>
-      <c r="B270" s="4">
-        <f>B269</f>
-        <v>283</v>
-      </c>
-      <c r="C270" s="4" t="s">
+      <c r="B270" s="3">
+        <f t="shared" si="38"/>
+        <v>280</v>
+      </c>
+      <c r="C270" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D270" s="4" t="s">
+      <c r="D270" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E270" s="4" t="s">
+      <c r="E270" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F270" s="4">
-        <v>1</v>
-      </c>
-      <c r="G270" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1264, 283, null, null, null, 1);</v>
+      <c r="F270" s="3">
+        <v>1</v>
+      </c>
+      <c r="G270" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1264, 280, null, null, null, 1);</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
@@ -32417,8 +32419,8 @@
         <v>1265</v>
       </c>
       <c r="B271" s="4">
-        <f t="shared" ref="B271:B272" si="37">B269</f>
-        <v>283</v>
+        <f>B267+1</f>
+        <v>281</v>
       </c>
       <c r="C271" s="4" t="s">
         <v>17</v>
@@ -32433,8 +32435,8 @@
         <v>2</v>
       </c>
       <c r="G271" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1265, 283, null, null, null, 2);</v>
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1265, 281, null, null, null, 2);</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
@@ -32443,8 +32445,8 @@
         <v>1266</v>
       </c>
       <c r="B272" s="4">
-        <f t="shared" si="37"/>
-        <v>283</v>
+        <f>B271</f>
+        <v>281</v>
       </c>
       <c r="C272" s="4" t="s">
         <v>17</v>
@@ -32459,70 +32461,70 @@
         <v>1</v>
       </c>
       <c r="G272" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1266, 283, null, null, null, 1);</v>
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1266, 281, null, null, null, 1);</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A273" s="3">
+      <c r="A273" s="4">
         <f t="shared" si="20"/>
         <v>1267</v>
       </c>
-      <c r="B273" s="3">
-        <f>B269+1</f>
-        <v>284</v>
-      </c>
-      <c r="C273" s="3" t="s">
+      <c r="B273" s="4">
+        <f t="shared" ref="B273:B274" si="39">B271</f>
+        <v>281</v>
+      </c>
+      <c r="C273" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D273" s="3" t="s">
+      <c r="D273" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E273" s="3" t="s">
+      <c r="E273" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F273" s="3">
-        <v>2</v>
-      </c>
-      <c r="G273" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1267, 284, null, null, null, 2);</v>
+      <c r="F273" s="4">
+        <v>2</v>
+      </c>
+      <c r="G273" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1267, 281, null, null, null, 2);</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A274" s="3">
+      <c r="A274" s="4">
         <f t="shared" si="20"/>
         <v>1268</v>
       </c>
-      <c r="B274" s="3">
-        <f>B273</f>
-        <v>284</v>
-      </c>
-      <c r="C274" s="3" t="s">
+      <c r="B274" s="4">
+        <f t="shared" si="39"/>
+        <v>281</v>
+      </c>
+      <c r="C274" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D274" s="3" t="s">
+      <c r="D274" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E274" s="3" t="s">
+      <c r="E274" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F274" s="3">
-        <v>1</v>
-      </c>
-      <c r="G274" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1268, 284, null, null, null, 1);</v>
+      <c r="F274" s="4">
+        <v>1</v>
+      </c>
+      <c r="G274" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1268, 281, null, null, null, 1);</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="3">
-        <f t="shared" ref="A275:A284" si="38">A274+1</f>
+        <f t="shared" si="20"/>
         <v>1269</v>
       </c>
       <c r="B275" s="3">
-        <f t="shared" ref="B275:B276" si="39">B273</f>
-        <v>284</v>
+        <f>B271+1</f>
+        <v>282</v>
       </c>
       <c r="C275" s="3" t="s">
         <v>17</v>
@@ -32537,18 +32539,18 @@
         <v>2</v>
       </c>
       <c r="G275" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1269, 284, null, null, null, 2);</v>
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1269, 282, null, null, null, 2);</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="20"/>
         <v>1270</v>
       </c>
       <c r="B276" s="3">
-        <f t="shared" si="39"/>
-        <v>284</v>
+        <f>B275</f>
+        <v>282</v>
       </c>
       <c r="C276" s="3" t="s">
         <v>17</v>
@@ -32563,70 +32565,70 @@
         <v>1</v>
       </c>
       <c r="G276" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1270, 284, null, null, null, 1);</v>
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1270, 282, null, null, null, 1);</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A277" s="4">
-        <f t="shared" si="38"/>
+      <c r="A277" s="3">
+        <f t="shared" si="20"/>
         <v>1271</v>
       </c>
-      <c r="B277" s="4">
-        <f>B273+1</f>
-        <v>285</v>
-      </c>
-      <c r="C277" s="4" t="s">
+      <c r="B277" s="3">
+        <f t="shared" ref="B277:B278" si="40">B275</f>
+        <v>282</v>
+      </c>
+      <c r="C277" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D277" s="4" t="s">
+      <c r="D277" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E277" s="4" t="s">
+      <c r="E277" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F277" s="4">
-        <v>2</v>
-      </c>
-      <c r="G277" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1271, 285, null, null, null, 2);</v>
+      <c r="F277" s="3">
+        <v>2</v>
+      </c>
+      <c r="G277" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1271, 282, null, null, null, 2);</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" s="4">
-        <f t="shared" si="38"/>
+      <c r="A278" s="3">
+        <f t="shared" si="20"/>
         <v>1272</v>
       </c>
-      <c r="B278" s="4">
-        <f>B277</f>
-        <v>285</v>
-      </c>
-      <c r="C278" s="4" t="s">
+      <c r="B278" s="3">
+        <f t="shared" si="40"/>
+        <v>282</v>
+      </c>
+      <c r="C278" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D278" s="4" t="s">
+      <c r="D278" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E278" s="4" t="s">
+      <c r="E278" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F278" s="4">
-        <v>1</v>
-      </c>
-      <c r="G278" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1272, 285, null, null, null, 1);</v>
+      <c r="F278" s="3">
+        <v>1</v>
+      </c>
+      <c r="G278" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1272, 282, null, null, null, 1);</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="20"/>
         <v>1273</v>
       </c>
       <c r="B279" s="4">
-        <f t="shared" ref="B279:B280" si="40">B277</f>
-        <v>285</v>
+        <f>B275+1</f>
+        <v>283</v>
       </c>
       <c r="C279" s="4" t="s">
         <v>17</v>
@@ -32641,18 +32643,18 @@
         <v>2</v>
       </c>
       <c r="G279" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1273, 285, null, null, null, 2);</v>
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1273, 283, null, null, null, 2);</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="20"/>
         <v>1274</v>
       </c>
       <c r="B280" s="4">
-        <f t="shared" si="40"/>
-        <v>285</v>
+        <f>B279</f>
+        <v>283</v>
       </c>
       <c r="C280" s="4" t="s">
         <v>17</v>
@@ -32667,70 +32669,70 @@
         <v>1</v>
       </c>
       <c r="G280" s="4" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1274, 285, null, null, null, 1);</v>
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1274, 283, null, null, null, 1);</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A281" s="3">
-        <f t="shared" si="38"/>
+      <c r="A281" s="4">
+        <f t="shared" si="20"/>
         <v>1275</v>
       </c>
-      <c r="B281" s="3">
-        <f>B277+1</f>
-        <v>286</v>
-      </c>
-      <c r="C281" s="3" t="s">
+      <c r="B281" s="4">
+        <f t="shared" ref="B281:B282" si="41">B279</f>
+        <v>283</v>
+      </c>
+      <c r="C281" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D281" s="3" t="s">
+      <c r="D281" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E281" s="3" t="s">
+      <c r="E281" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F281" s="3">
-        <v>2</v>
-      </c>
-      <c r="G281" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1275, 286, null, null, null, 2);</v>
+      <c r="F281" s="4">
+        <v>2</v>
+      </c>
+      <c r="G281" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1275, 283, null, null, null, 2);</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A282" s="3">
-        <f t="shared" si="38"/>
+      <c r="A282" s="4">
+        <f t="shared" si="20"/>
         <v>1276</v>
       </c>
-      <c r="B282" s="3">
-        <f>B281</f>
-        <v>286</v>
-      </c>
-      <c r="C282" s="3" t="s">
+      <c r="B282" s="4">
+        <f t="shared" si="41"/>
+        <v>283</v>
+      </c>
+      <c r="C282" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D282" s="3" t="s">
+      <c r="D282" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E282" s="3" t="s">
+      <c r="E282" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F282" s="3">
-        <v>1</v>
-      </c>
-      <c r="G282" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1276, 286, null, null, null, 1);</v>
+      <c r="F282" s="4">
+        <v>1</v>
+      </c>
+      <c r="G282" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1276, 283, null, null, null, 1);</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="20"/>
         <v>1277</v>
       </c>
       <c r="B283" s="3">
-        <f t="shared" ref="B283:B284" si="41">B281</f>
-        <v>286</v>
+        <f>B279+1</f>
+        <v>284</v>
       </c>
       <c r="C283" s="3" t="s">
         <v>17</v>
@@ -32745,18 +32747,18 @@
         <v>2</v>
       </c>
       <c r="G283" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1277, 286, null, null, null, 2);</v>
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1277, 284, null, null, null, 2);</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="3">
-        <f t="shared" si="38"/>
+        <f t="shared" si="20"/>
         <v>1278</v>
       </c>
       <c r="B284" s="3">
-        <f t="shared" si="41"/>
-        <v>286</v>
+        <f>B283</f>
+        <v>284</v>
       </c>
       <c r="C284" s="3" t="s">
         <v>17</v>
@@ -32771,8 +32773,268 @@
         <v>1</v>
       </c>
       <c r="G284" s="3" t="str">
-        <f t="shared" si="33"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1278, 286, null, null, null, 1);</v>
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1278, 284, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A285" s="3">
+        <f t="shared" ref="A285:A294" si="42">A284+1</f>
+        <v>1279</v>
+      </c>
+      <c r="B285" s="3">
+        <f t="shared" ref="B285:B286" si="43">B283</f>
+        <v>284</v>
+      </c>
+      <c r="C285" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D285" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E285" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F285" s="3">
+        <v>2</v>
+      </c>
+      <c r="G285" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1279, 284, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A286" s="3">
+        <f t="shared" si="42"/>
+        <v>1280</v>
+      </c>
+      <c r="B286" s="3">
+        <f t="shared" si="43"/>
+        <v>284</v>
+      </c>
+      <c r="C286" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D286" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E286" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F286" s="3">
+        <v>1</v>
+      </c>
+      <c r="G286" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1280, 284, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A287" s="4">
+        <f t="shared" si="42"/>
+        <v>1281</v>
+      </c>
+      <c r="B287" s="4">
+        <f>B283+1</f>
+        <v>285</v>
+      </c>
+      <c r="C287" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D287" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E287" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F287" s="4">
+        <v>2</v>
+      </c>
+      <c r="G287" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1281, 285, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A288" s="4">
+        <f t="shared" si="42"/>
+        <v>1282</v>
+      </c>
+      <c r="B288" s="4">
+        <f>B287</f>
+        <v>285</v>
+      </c>
+      <c r="C288" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D288" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E288" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F288" s="4">
+        <v>1</v>
+      </c>
+      <c r="G288" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1282, 285, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289" s="4">
+        <f t="shared" si="42"/>
+        <v>1283</v>
+      </c>
+      <c r="B289" s="4">
+        <f t="shared" ref="B289:B290" si="44">B287</f>
+        <v>285</v>
+      </c>
+      <c r="C289" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D289" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E289" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F289" s="4">
+        <v>2</v>
+      </c>
+      <c r="G289" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1283, 285, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="4">
+        <f t="shared" si="42"/>
+        <v>1284</v>
+      </c>
+      <c r="B290" s="4">
+        <f t="shared" si="44"/>
+        <v>285</v>
+      </c>
+      <c r="C290" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D290" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E290" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F290" s="4">
+        <v>1</v>
+      </c>
+      <c r="G290" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1284, 285, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="3">
+        <f t="shared" si="42"/>
+        <v>1285</v>
+      </c>
+      <c r="B291" s="3">
+        <f>B287+1</f>
+        <v>286</v>
+      </c>
+      <c r="C291" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D291" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E291" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F291" s="3">
+        <v>2</v>
+      </c>
+      <c r="G291" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1285, 286, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="3">
+        <f t="shared" si="42"/>
+        <v>1286</v>
+      </c>
+      <c r="B292" s="3">
+        <f>B291</f>
+        <v>286</v>
+      </c>
+      <c r="C292" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D292" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E292" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F292" s="3">
+        <v>1</v>
+      </c>
+      <c r="G292" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1286, 286, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293" s="3">
+        <f t="shared" si="42"/>
+        <v>1287</v>
+      </c>
+      <c r="B293" s="3">
+        <f t="shared" ref="B293:B294" si="45">B291</f>
+        <v>286</v>
+      </c>
+      <c r="C293" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D293" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E293" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F293" s="3">
+        <v>2</v>
+      </c>
+      <c r="G293" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1287, 286, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="3">
+        <f t="shared" si="42"/>
+        <v>1288</v>
+      </c>
+      <c r="B294" s="3">
+        <f t="shared" si="45"/>
+        <v>286</v>
+      </c>
+      <c r="C294" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D294" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E294" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F294" s="3">
+        <v>1</v>
+      </c>
+      <c r="G294" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1288, 286, null, null, null, 1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Copa America 2da fecha octavos de final Eurocopa
Final Copa America 2da fecha octavos de final Eurocopa
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -25496,7 +25496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -31799,18 +31801,18 @@
       <c r="C247" s="4">
         <v>33</v>
       </c>
-      <c r="D247" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E247" s="4" t="s">
-        <v>17</v>
+      <c r="D247" s="4">
+        <v>2</v>
+      </c>
+      <c r="E247" s="4">
+        <v>3</v>
       </c>
       <c r="F247" s="4">
         <v>2</v>
       </c>
       <c r="G247" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1241, 275, 33, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1241, 275, 33, 2, 3, 2);</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.25">
@@ -31825,18 +31827,18 @@
       <c r="C248" s="4">
         <v>33</v>
       </c>
-      <c r="D248" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E248" s="4" t="s">
-        <v>17</v>
+      <c r="D248" s="4">
+        <v>0</v>
+      </c>
+      <c r="E248" s="4">
+        <v>0</v>
       </c>
       <c r="F248" s="4">
         <v>1</v>
       </c>
       <c r="G248" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1242, 275, 33, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1242, 275, 33, 0, 0, 1);</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.25">
@@ -31851,18 +31853,18 @@
       <c r="C249" s="4">
         <v>353</v>
       </c>
-      <c r="D249" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E249" s="4" t="s">
-        <v>17</v>
+      <c r="D249" s="4">
+        <v>1</v>
+      </c>
+      <c r="E249" s="4">
+        <v>0</v>
       </c>
       <c r="F249" s="4">
         <v>2</v>
       </c>
       <c r="G249" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1243, 275, 353, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1243, 275, 353, 1, 0, 2);</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.25">
@@ -31877,18 +31879,18 @@
       <c r="C250" s="4">
         <v>353</v>
       </c>
-      <c r="D250" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E250" s="4" t="s">
-        <v>17</v>
+      <c r="D250" s="4">
+        <v>1</v>
+      </c>
+      <c r="E250" s="4">
+        <v>0</v>
       </c>
       <c r="F250" s="4">
         <v>1</v>
       </c>
       <c r="G250" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1244, 275, 353, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1244, 275, 353, 1, 0, 1);</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.25">
@@ -31903,18 +31905,18 @@
       <c r="C251" s="3">
         <v>49</v>
       </c>
-      <c r="D251" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E251" s="3" t="s">
-        <v>17</v>
+      <c r="D251" s="3">
+        <v>3</v>
+      </c>
+      <c r="E251" s="3">
+        <v>3</v>
       </c>
       <c r="F251" s="3">
         <v>2</v>
       </c>
       <c r="G251" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1245, 276, 49, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1245, 276, 49, 3, 3, 2);</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.25">
@@ -31929,18 +31931,18 @@
       <c r="C252" s="3">
         <v>49</v>
       </c>
-      <c r="D252" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E252" s="3" t="s">
-        <v>17</v>
+      <c r="D252" s="3">
+        <v>2</v>
+      </c>
+      <c r="E252" s="3">
+        <v>0</v>
       </c>
       <c r="F252" s="3">
         <v>1</v>
       </c>
       <c r="G252" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1246, 276, 49, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1246, 276, 49, 2, 0, 1);</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
@@ -31955,18 +31957,18 @@
       <c r="C253" s="3">
         <v>421</v>
       </c>
-      <c r="D253" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E253" s="3" t="s">
-        <v>17</v>
+      <c r="D253" s="3">
+        <v>0</v>
+      </c>
+      <c r="E253" s="3">
+        <v>0</v>
       </c>
       <c r="F253" s="3">
         <v>2</v>
       </c>
       <c r="G253" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1247, 276, 421, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1247, 276, 421, 0, 0, 2);</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.25">
@@ -31981,18 +31983,18 @@
       <c r="C254" s="3">
         <v>421</v>
       </c>
-      <c r="D254" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E254" s="3" t="s">
-        <v>17</v>
+      <c r="D254" s="3">
+        <v>0</v>
+      </c>
+      <c r="E254" s="3">
+        <v>0</v>
       </c>
       <c r="F254" s="3">
         <v>1</v>
       </c>
       <c r="G254" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1248, 276, 421, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1248, 276, 421, 0, 0, 1);</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.25">
@@ -32007,18 +32009,18 @@
       <c r="C255" s="4">
         <v>36</v>
       </c>
-      <c r="D255" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E255" s="4" t="s">
-        <v>17</v>
+      <c r="D255" s="4">
+        <v>0</v>
+      </c>
+      <c r="E255" s="4">
+        <v>0</v>
       </c>
       <c r="F255" s="4">
         <v>2</v>
       </c>
       <c r="G255" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1249, 277, 36, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1249, 277, 36, 0, 0, 2);</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
@@ -32033,18 +32035,18 @@
       <c r="C256" s="4">
         <v>36</v>
       </c>
-      <c r="D256" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E256" s="4" t="s">
-        <v>17</v>
+      <c r="D256" s="4">
+        <v>0</v>
+      </c>
+      <c r="E256" s="4">
+        <v>0</v>
       </c>
       <c r="F256" s="4">
         <v>1</v>
       </c>
       <c r="G256" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1250, 277, 36, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1250, 277, 36, 0, 0, 1);</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
@@ -32059,18 +32061,18 @@
       <c r="C257" s="4">
         <v>32</v>
       </c>
-      <c r="D257" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E257" s="4" t="s">
-        <v>17</v>
+      <c r="D257" s="4">
+        <v>4</v>
+      </c>
+      <c r="E257" s="4">
+        <v>3</v>
       </c>
       <c r="F257" s="4">
         <v>2</v>
       </c>
       <c r="G257" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1251, 277, 32, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1251, 277, 32, 4, 3, 2);</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
@@ -32085,18 +32087,18 @@
       <c r="C258" s="4">
         <v>32</v>
       </c>
-      <c r="D258" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E258" s="4" t="s">
-        <v>17</v>
+      <c r="D258" s="4">
+        <v>1</v>
+      </c>
+      <c r="E258" s="4">
+        <v>0</v>
       </c>
       <c r="F258" s="4">
         <v>1</v>
       </c>
       <c r="G258" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1252, 277, 32, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1252, 277, 32, 1, 0, 1);</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Date 3 Round of 16 Eurocopa and Quarter-Finals
Date 3 Round of 16 Eurocopa and Quarter-Finals
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -25496,9 +25496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -32113,18 +32111,18 @@
       <c r="C259" s="3">
         <v>39</v>
       </c>
-      <c r="D259" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E259" s="3" t="s">
-        <v>17</v>
+      <c r="D259" s="3">
+        <v>2</v>
+      </c>
+      <c r="E259" s="3">
+        <v>3</v>
       </c>
       <c r="F259" s="3">
         <v>2</v>
       </c>
       <c r="G259" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1253, 278, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1253, 278, 39, 2, 3, 2);</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
@@ -32139,18 +32137,18 @@
       <c r="C260" s="3">
         <v>39</v>
       </c>
-      <c r="D260" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E260" s="3" t="s">
-        <v>17</v>
+      <c r="D260" s="3">
+        <v>1</v>
+      </c>
+      <c r="E260" s="3">
+        <v>0</v>
       </c>
       <c r="F260" s="3">
         <v>1</v>
       </c>
       <c r="G260" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1254, 278, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1254, 278, 39, 1, 0, 1);</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
@@ -32165,18 +32163,18 @@
       <c r="C261" s="3">
         <v>34</v>
       </c>
-      <c r="D261" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E261" s="3" t="s">
-        <v>17</v>
+      <c r="D261" s="3">
+        <v>0</v>
+      </c>
+      <c r="E261" s="3">
+        <v>0</v>
       </c>
       <c r="F261" s="3">
         <v>2</v>
       </c>
       <c r="G261" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1255, 278, 34, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1255, 278, 34, 0, 0, 2);</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
@@ -32191,18 +32189,18 @@
       <c r="C262" s="3">
         <v>34</v>
       </c>
-      <c r="D262" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E262" s="3" t="s">
-        <v>17</v>
+      <c r="D262" s="3">
+        <v>0</v>
+      </c>
+      <c r="E262" s="3">
+        <v>0</v>
       </c>
       <c r="F262" s="3">
         <v>1</v>
       </c>
       <c r="G262" s="3" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1256, 278, 34, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1256, 278, 34, 0, 0, 1);</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
@@ -32217,18 +32215,18 @@
       <c r="C263" s="4">
         <v>4420</v>
       </c>
-      <c r="D263" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E263" s="4" t="s">
-        <v>17</v>
+      <c r="D263" s="4">
+        <v>1</v>
+      </c>
+      <c r="E263" s="4">
+        <v>0</v>
       </c>
       <c r="F263" s="4">
         <v>2</v>
       </c>
       <c r="G263" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1257, 279, 4420, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1257, 279, 4420, 1, 0, 2);</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
@@ -32243,18 +32241,18 @@
       <c r="C264" s="4">
         <v>4420</v>
       </c>
-      <c r="D264" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E264" s="4" t="s">
-        <v>17</v>
+      <c r="D264" s="4">
+        <v>1</v>
+      </c>
+      <c r="E264" s="4">
+        <v>0</v>
       </c>
       <c r="F264" s="4">
         <v>1</v>
       </c>
       <c r="G264" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1258, 279, 4420, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1258, 279, 4420, 1, 0, 1);</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
@@ -32269,18 +32267,18 @@
       <c r="C265" s="4">
         <v>354</v>
       </c>
-      <c r="D265" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E265" s="4" t="s">
-        <v>17</v>
+      <c r="D265" s="4">
+        <v>2</v>
+      </c>
+      <c r="E265" s="4">
+        <v>3</v>
       </c>
       <c r="F265" s="4">
         <v>2</v>
       </c>
       <c r="G265" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1259, 279, 354, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1259, 279, 354, 2, 3, 2);</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
@@ -32295,18 +32293,18 @@
       <c r="C266" s="4">
         <v>354</v>
       </c>
-      <c r="D266" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E266" s="4" t="s">
-        <v>17</v>
+      <c r="D266" s="4">
+        <v>2</v>
+      </c>
+      <c r="E266" s="4">
+        <v>0</v>
       </c>
       <c r="F266" s="4">
         <v>1</v>
       </c>
       <c r="G266" s="4" t="str">
         <f t="shared" si="15"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1260, 279, 354, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1260, 279, 354, 2, 0, 1);</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
@@ -32318,8 +32316,8 @@
         <f>B263+1</f>
         <v>280</v>
       </c>
-      <c r="C267" s="3" t="s">
-        <v>17</v>
+      <c r="C267" s="3">
+        <v>48</v>
       </c>
       <c r="D267" s="3" t="s">
         <v>17</v>
@@ -32332,7 +32330,7 @@
       </c>
       <c r="G267" s="3" t="str">
         <f t="shared" ref="G267:G294" si="37">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A267 &amp; ", " &amp; B267 &amp; ", " &amp; C267 &amp; ", " &amp; D267 &amp; ", " &amp; E267 &amp; ", " &amp; F267 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1261, 280, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1261, 280, 48, null, null, 2);</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
@@ -32344,8 +32342,8 @@
         <f>B267</f>
         <v>280</v>
       </c>
-      <c r="C268" s="3" t="s">
-        <v>17</v>
+      <c r="C268" s="3">
+        <v>48</v>
       </c>
       <c r="D268" s="3" t="s">
         <v>17</v>
@@ -32358,7 +32356,7 @@
       </c>
       <c r="G268" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1262, 280, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1262, 280, 48, null, null, 1);</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
@@ -32370,8 +32368,8 @@
         <f t="shared" ref="B269:B270" si="38">B267</f>
         <v>280</v>
       </c>
-      <c r="C269" s="3" t="s">
-        <v>17</v>
+      <c r="C269" s="3">
+        <v>351</v>
       </c>
       <c r="D269" s="3" t="s">
         <v>17</v>
@@ -32384,7 +32382,7 @@
       </c>
       <c r="G269" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1263, 280, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1263, 280, 351, null, null, 2);</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
@@ -32396,8 +32394,8 @@
         <f t="shared" si="38"/>
         <v>280</v>
       </c>
-      <c r="C270" s="3" t="s">
-        <v>17</v>
+      <c r="C270" s="3">
+        <v>351</v>
       </c>
       <c r="D270" s="3" t="s">
         <v>17</v>
@@ -32410,7 +32408,7 @@
       </c>
       <c r="G270" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1264, 280, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1264, 280, 351, null, null, 1);</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
@@ -32422,8 +32420,8 @@
         <f>B267+1</f>
         <v>281</v>
       </c>
-      <c r="C271" s="4" t="s">
-        <v>17</v>
+      <c r="C271" s="4">
+        <v>4429</v>
       </c>
       <c r="D271" s="4" t="s">
         <v>17</v>
@@ -32436,7 +32434,7 @@
       </c>
       <c r="G271" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1265, 281, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1265, 281, 4429, null, null, 2);</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
@@ -32448,8 +32446,8 @@
         <f>B271</f>
         <v>281</v>
       </c>
-      <c r="C272" s="4" t="s">
-        <v>17</v>
+      <c r="C272" s="4">
+        <v>4429</v>
       </c>
       <c r="D272" s="4" t="s">
         <v>17</v>
@@ -32462,7 +32460,7 @@
       </c>
       <c r="G272" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1266, 281, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1266, 281, 4429, null, null, 1);</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
@@ -32474,8 +32472,8 @@
         <f t="shared" ref="B273:B274" si="39">B271</f>
         <v>281</v>
       </c>
-      <c r="C273" s="4" t="s">
-        <v>17</v>
+      <c r="C273" s="4">
+        <v>32</v>
       </c>
       <c r="D273" s="4" t="s">
         <v>17</v>
@@ -32488,7 +32486,7 @@
       </c>
       <c r="G273" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1267, 281, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1267, 281, 32, null, null, 2);</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
@@ -32500,8 +32498,8 @@
         <f t="shared" si="39"/>
         <v>281</v>
       </c>
-      <c r="C274" s="4" t="s">
-        <v>17</v>
+      <c r="C274" s="4">
+        <v>32</v>
       </c>
       <c r="D274" s="4" t="s">
         <v>17</v>
@@ -32514,7 +32512,7 @@
       </c>
       <c r="G274" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1268, 281, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1268, 281, 32, null, null, 1);</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
@@ -32526,8 +32524,8 @@
         <f>B271+1</f>
         <v>282</v>
       </c>
-      <c r="C275" s="3" t="s">
-        <v>17</v>
+      <c r="C275" s="3">
+        <v>49</v>
       </c>
       <c r="D275" s="3" t="s">
         <v>17</v>
@@ -32540,7 +32538,7 @@
       </c>
       <c r="G275" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1269, 282, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1269, 282, 49, null, null, 2);</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
@@ -32552,8 +32550,8 @@
         <f>B275</f>
         <v>282</v>
       </c>
-      <c r="C276" s="3" t="s">
-        <v>17</v>
+      <c r="C276" s="3">
+        <v>49</v>
       </c>
       <c r="D276" s="3" t="s">
         <v>17</v>
@@ -32566,7 +32564,7 @@
       </c>
       <c r="G276" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1270, 282, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1270, 282, 49, null, null, 1);</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
@@ -32578,8 +32576,8 @@
         <f t="shared" ref="B277:B278" si="40">B275</f>
         <v>282</v>
       </c>
-      <c r="C277" s="3" t="s">
-        <v>17</v>
+      <c r="C277" s="3">
+        <v>39</v>
       </c>
       <c r="D277" s="3" t="s">
         <v>17</v>
@@ -32592,7 +32590,7 @@
       </c>
       <c r="G277" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1271, 282, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1271, 282, 39, null, null, 2);</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
@@ -32604,8 +32602,8 @@
         <f t="shared" si="40"/>
         <v>282</v>
       </c>
-      <c r="C278" s="3" t="s">
-        <v>17</v>
+      <c r="C278" s="3">
+        <v>39</v>
       </c>
       <c r="D278" s="3" t="s">
         <v>17</v>
@@ -32618,7 +32616,7 @@
       </c>
       <c r="G278" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1272, 282, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1272, 282, 39, null, null, 1);</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
@@ -32630,8 +32628,8 @@
         <f>B275+1</f>
         <v>283</v>
       </c>
-      <c r="C279" s="4" t="s">
-        <v>17</v>
+      <c r="C279" s="4">
+        <v>33</v>
       </c>
       <c r="D279" s="4" t="s">
         <v>17</v>
@@ -32644,7 +32642,7 @@
       </c>
       <c r="G279" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1273, 283, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1273, 283, 33, null, null, 2);</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
@@ -32656,8 +32654,8 @@
         <f>B279</f>
         <v>283</v>
       </c>
-      <c r="C280" s="4" t="s">
-        <v>17</v>
+      <c r="C280" s="4">
+        <v>33</v>
       </c>
       <c r="D280" s="4" t="s">
         <v>17</v>
@@ -32670,7 +32668,7 @@
       </c>
       <c r="G280" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1274, 283, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1274, 283, 33, null, null, 1);</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
@@ -32682,8 +32680,8 @@
         <f t="shared" ref="B281:B282" si="41">B279</f>
         <v>283</v>
       </c>
-      <c r="C281" s="4" t="s">
-        <v>17</v>
+      <c r="C281" s="4">
+        <v>354</v>
       </c>
       <c r="D281" s="4" t="s">
         <v>17</v>
@@ -32696,7 +32694,7 @@
       </c>
       <c r="G281" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1275, 283, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1275, 283, 354, null, null, 2);</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
@@ -32708,8 +32706,8 @@
         <f t="shared" si="41"/>
         <v>283</v>
       </c>
-      <c r="C282" s="4" t="s">
-        <v>17</v>
+      <c r="C282" s="4">
+        <v>354</v>
       </c>
       <c r="D282" s="4" t="s">
         <v>17</v>
@@ -32722,7 +32720,7 @@
       </c>
       <c r="G282" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1276, 283, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1276, 283, 354, null, null, 1);</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tournaments, olympics and UEFAEURO quarter-finals
tournaments, olympics and UEFAEURO quarter-finals
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -25494,7 +25494,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J294"/>
+  <dimension ref="A1:J300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
@@ -30853,7 +30853,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
-        <f t="shared" ref="A211:A284" si="20">A210+1</f>
+        <f t="shared" ref="A211:A290" si="20">A210+1</f>
         <v>1205</v>
       </c>
       <c r="B211" s="3">
@@ -32319,18 +32319,18 @@
       <c r="C267" s="3">
         <v>48</v>
       </c>
-      <c r="D267" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E267" s="3" t="s">
-        <v>17</v>
+      <c r="D267" s="3">
+        <v>1</v>
+      </c>
+      <c r="E267" s="3">
+        <v>0</v>
       </c>
       <c r="F267" s="3">
         <v>2</v>
       </c>
       <c r="G267" s="3" t="str">
-        <f t="shared" ref="G267:G294" si="37">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A267 &amp; ", " &amp; B267 &amp; ", " &amp; C267 &amp; ", " &amp; D267 &amp; ", " &amp; E267 &amp; ", " &amp; F267 &amp; ");"</f>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1261, 280, 48, null, null, 2);</v>
+        <f t="shared" ref="G267:G300" si="37">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A267 &amp; ", " &amp; B267 &amp; ", " &amp; C267 &amp; ", " &amp; D267 &amp; ", " &amp; E267 &amp; ", " &amp; F267 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1261, 280, 48, 1, 0, 2);</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
@@ -32345,18 +32345,18 @@
       <c r="C268" s="3">
         <v>48</v>
       </c>
-      <c r="D268" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E268" s="3" t="s">
-        <v>17</v>
+      <c r="D268" s="3">
+        <v>1</v>
+      </c>
+      <c r="E268" s="3">
+        <v>0</v>
       </c>
       <c r="F268" s="3">
         <v>1</v>
       </c>
       <c r="G268" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1262, 280, 48, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1262, 280, 48, 1, 0, 1);</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
@@ -32365,24 +32365,24 @@
         <v>1263</v>
       </c>
       <c r="B269" s="3">
-        <f t="shared" ref="B269:B270" si="38">B267</f>
+        <f>B268</f>
         <v>280</v>
       </c>
       <c r="C269" s="3">
         <v>351</v>
       </c>
-      <c r="D269" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E269" s="3" t="s">
-        <v>17</v>
+      <c r="D269" s="3">
+        <v>1</v>
+      </c>
+      <c r="E269" s="3">
+        <v>0</v>
       </c>
       <c r="F269" s="3">
         <v>2</v>
       </c>
       <c r="G269" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1263, 280, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1263, 280, 351, 1, 0, 2);</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
@@ -32391,128 +32391,128 @@
         <v>1264</v>
       </c>
       <c r="B270" s="3">
-        <f t="shared" si="38"/>
+        <f>B269</f>
         <v>280</v>
       </c>
       <c r="C270" s="3">
         <v>351</v>
       </c>
-      <c r="D270" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E270" s="3" t="s">
-        <v>17</v>
+      <c r="D270" s="3">
+        <v>1</v>
+      </c>
+      <c r="E270" s="3">
+        <v>0</v>
       </c>
       <c r="F270" s="3">
         <v>1</v>
       </c>
       <c r="G270" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1264, 280, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1264, 280, 351, 1, 0, 1);</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A271" s="4">
+      <c r="A271" s="3">
         <f t="shared" si="20"/>
         <v>1265</v>
       </c>
-      <c r="B271" s="4">
-        <f>B267+1</f>
-        <v>281</v>
-      </c>
-      <c r="C271" s="4">
-        <v>4429</v>
-      </c>
-      <c r="D271" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E271" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F271" s="4">
-        <v>2</v>
-      </c>
-      <c r="G271" s="4" t="str">
+      <c r="B271" s="3">
+        <f>B270</f>
+        <v>280</v>
+      </c>
+      <c r="C271" s="3">
+        <v>48</v>
+      </c>
+      <c r="D271" s="3">
+        <v>1</v>
+      </c>
+      <c r="E271" s="3">
+        <v>1</v>
+      </c>
+      <c r="F271" s="3">
+        <v>4</v>
+      </c>
+      <c r="G271" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1265, 281, 4429, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1265, 280, 48, 1, 1, 4);</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A272" s="4">
+      <c r="A272" s="3">
         <f t="shared" si="20"/>
         <v>1266</v>
       </c>
-      <c r="B272" s="4">
+      <c r="B272" s="3">
         <f>B271</f>
-        <v>281</v>
-      </c>
-      <c r="C272" s="4">
-        <v>4429</v>
-      </c>
-      <c r="D272" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E272" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F272" s="4">
-        <v>1</v>
-      </c>
-      <c r="G272" s="4" t="str">
+        <v>280</v>
+      </c>
+      <c r="C272" s="3">
+        <v>48</v>
+      </c>
+      <c r="D272" s="3">
+        <v>1</v>
+      </c>
+      <c r="E272" s="3">
+        <v>0</v>
+      </c>
+      <c r="F272" s="3">
+        <v>3</v>
+      </c>
+      <c r="G272" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1266, 281, 4429, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1266, 280, 48, 1, 0, 3);</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A273" s="4">
+      <c r="A273" s="3">
         <f t="shared" si="20"/>
         <v>1267</v>
       </c>
-      <c r="B273" s="4">
-        <f t="shared" ref="B273:B274" si="39">B271</f>
-        <v>281</v>
-      </c>
-      <c r="C273" s="4">
-        <v>32</v>
-      </c>
-      <c r="D273" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E273" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F273" s="4">
-        <v>2</v>
-      </c>
-      <c r="G273" s="4" t="str">
+      <c r="B273" s="3">
+        <f>B272</f>
+        <v>280</v>
+      </c>
+      <c r="C273" s="3">
+        <v>351</v>
+      </c>
+      <c r="D273" s="3">
+        <v>1</v>
+      </c>
+      <c r="E273" s="3">
+        <v>1</v>
+      </c>
+      <c r="F273" s="3">
+        <v>4</v>
+      </c>
+      <c r="G273" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1267, 281, 32, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1267, 280, 351, 1, 1, 4);</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A274" s="4">
+      <c r="A274" s="3">
         <f t="shared" si="20"/>
         <v>1268</v>
       </c>
-      <c r="B274" s="4">
-        <f t="shared" si="39"/>
-        <v>281</v>
-      </c>
-      <c r="C274" s="4">
-        <v>32</v>
-      </c>
-      <c r="D274" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E274" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F274" s="4">
-        <v>1</v>
-      </c>
-      <c r="G274" s="4" t="str">
+      <c r="B274" s="3">
+        <f>B273</f>
+        <v>280</v>
+      </c>
+      <c r="C274" s="3">
+        <v>351</v>
+      </c>
+      <c r="D274" s="3">
+        <v>1</v>
+      </c>
+      <c r="E274" s="3">
+        <v>0</v>
+      </c>
+      <c r="F274" s="3">
+        <v>3</v>
+      </c>
+      <c r="G274" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1268, 281, 32, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1268, 280, 351, 1, 0, 3);</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
@@ -32521,24 +32521,24 @@
         <v>1269</v>
       </c>
       <c r="B275" s="3">
-        <f>B271+1</f>
-        <v>282</v>
+        <f>B272</f>
+        <v>280</v>
       </c>
       <c r="C275" s="3">
-        <v>49</v>
-      </c>
-      <c r="D275" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E275" s="3" t="s">
-        <v>17</v>
+        <v>48</v>
+      </c>
+      <c r="D275" s="3">
+        <v>3</v>
+      </c>
+      <c r="E275" s="3">
+        <v>0</v>
       </c>
       <c r="F275" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G275" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1269, 282, 49, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1269, 280, 48, 3, 0, 7);</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
@@ -32548,75 +32548,75 @@
       </c>
       <c r="B276" s="3">
         <f>B275</f>
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C276" s="3">
-        <v>49</v>
-      </c>
-      <c r="D276" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E276" s="3" t="s">
-        <v>17</v>
+        <v>351</v>
+      </c>
+      <c r="D276" s="3">
+        <v>5</v>
+      </c>
+      <c r="E276" s="3">
+        <v>0</v>
       </c>
       <c r="F276" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G276" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1270, 282, 49, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1270, 280, 351, 5, 0, 7);</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A277" s="3">
+      <c r="A277" s="4">
         <f t="shared" si="20"/>
         <v>1271</v>
       </c>
-      <c r="B277" s="3">
-        <f t="shared" ref="B277:B278" si="40">B275</f>
-        <v>282</v>
-      </c>
-      <c r="C277" s="3">
-        <v>39</v>
-      </c>
-      <c r="D277" s="3" t="s">
+      <c r="B277" s="4">
+        <f>B267+1</f>
+        <v>281</v>
+      </c>
+      <c r="C277" s="4">
+        <v>4429</v>
+      </c>
+      <c r="D277" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E277" s="3" t="s">
+      <c r="E277" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F277" s="3">
-        <v>2</v>
-      </c>
-      <c r="G277" s="3" t="str">
+      <c r="F277" s="4">
+        <v>2</v>
+      </c>
+      <c r="G277" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1271, 282, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1271, 281, 4429, null, null, 2);</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" s="3">
+      <c r="A278" s="4">
         <f t="shared" si="20"/>
         <v>1272</v>
       </c>
-      <c r="B278" s="3">
-        <f t="shared" si="40"/>
-        <v>282</v>
-      </c>
-      <c r="C278" s="3">
-        <v>39</v>
-      </c>
-      <c r="D278" s="3" t="s">
+      <c r="B278" s="4">
+        <f>B277</f>
+        <v>281</v>
+      </c>
+      <c r="C278" s="4">
+        <v>4429</v>
+      </c>
+      <c r="D278" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E278" s="3" t="s">
+      <c r="E278" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F278" s="3">
-        <v>1</v>
-      </c>
-      <c r="G278" s="3" t="str">
+      <c r="F278" s="4">
+        <v>1</v>
+      </c>
+      <c r="G278" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1272, 282, 39, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1272, 281, 4429, null, null, 1);</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
@@ -32625,11 +32625,11 @@
         <v>1273</v>
       </c>
       <c r="B279" s="4">
-        <f>B275+1</f>
-        <v>283</v>
+        <f t="shared" ref="B279:B280" si="38">B277</f>
+        <v>281</v>
       </c>
       <c r="C279" s="4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D279" s="4" t="s">
         <v>17</v>
@@ -32642,7 +32642,7 @@
       </c>
       <c r="G279" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1273, 283, 33, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1273, 281, 32, null, null, 2);</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
@@ -32651,11 +32651,11 @@
         <v>1274</v>
       </c>
       <c r="B280" s="4">
-        <f>B279</f>
-        <v>283</v>
+        <f t="shared" si="38"/>
+        <v>281</v>
       </c>
       <c r="C280" s="4">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D280" s="4" t="s">
         <v>17</v>
@@ -32668,59 +32668,59 @@
       </c>
       <c r="G280" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1274, 283, 33, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1274, 281, 32, null, null, 1);</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A281" s="4">
+      <c r="A281" s="3">
         <f t="shared" si="20"/>
         <v>1275</v>
       </c>
-      <c r="B281" s="4">
-        <f t="shared" ref="B281:B282" si="41">B279</f>
-        <v>283</v>
-      </c>
-      <c r="C281" s="4">
-        <v>354</v>
-      </c>
-      <c r="D281" s="4" t="s">
+      <c r="B281" s="3">
+        <f>B277+1</f>
+        <v>282</v>
+      </c>
+      <c r="C281" s="3">
+        <v>49</v>
+      </c>
+      <c r="D281" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E281" s="4" t="s">
+      <c r="E281" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F281" s="4">
-        <v>2</v>
-      </c>
-      <c r="G281" s="4" t="str">
+      <c r="F281" s="3">
+        <v>2</v>
+      </c>
+      <c r="G281" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1275, 283, 354, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1275, 282, 49, null, null, 2);</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A282" s="4">
+      <c r="A282" s="3">
         <f t="shared" si="20"/>
         <v>1276</v>
       </c>
-      <c r="B282" s="4">
-        <f t="shared" si="41"/>
-        <v>283</v>
-      </c>
-      <c r="C282" s="4">
-        <v>354</v>
-      </c>
-      <c r="D282" s="4" t="s">
+      <c r="B282" s="3">
+        <f>B281</f>
+        <v>282</v>
+      </c>
+      <c r="C282" s="3">
+        <v>49</v>
+      </c>
+      <c r="D282" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E282" s="4" t="s">
+      <c r="E282" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F282" s="4">
-        <v>1</v>
-      </c>
-      <c r="G282" s="4" t="str">
+      <c r="F282" s="3">
+        <v>1</v>
+      </c>
+      <c r="G282" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1276, 283, 354, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1276, 282, 49, null, null, 1);</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
@@ -32729,11 +32729,11 @@
         <v>1277</v>
       </c>
       <c r="B283" s="3">
-        <f>B279+1</f>
-        <v>284</v>
-      </c>
-      <c r="C283" s="3" t="s">
-        <v>17</v>
+        <f t="shared" ref="B283:B284" si="39">B281</f>
+        <v>282</v>
+      </c>
+      <c r="C283" s="3">
+        <v>39</v>
       </c>
       <c r="D283" s="3" t="s">
         <v>17</v>
@@ -32746,7 +32746,7 @@
       </c>
       <c r="G283" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1277, 284, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1277, 282, 39, null, null, 2);</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
@@ -32755,11 +32755,11 @@
         <v>1278</v>
       </c>
       <c r="B284" s="3">
-        <f>B283</f>
-        <v>284</v>
-      </c>
-      <c r="C284" s="3" t="s">
-        <v>17</v>
+        <f t="shared" si="39"/>
+        <v>282</v>
+      </c>
+      <c r="C284" s="3">
+        <v>39</v>
       </c>
       <c r="D284" s="3" t="s">
         <v>17</v>
@@ -32772,72 +32772,72 @@
       </c>
       <c r="G284" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1278, 284, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1278, 282, 39, null, null, 1);</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A285" s="3">
-        <f t="shared" ref="A285:A294" si="42">A284+1</f>
+      <c r="A285" s="4">
+        <f t="shared" si="20"/>
         <v>1279</v>
       </c>
-      <c r="B285" s="3">
-        <f t="shared" ref="B285:B286" si="43">B283</f>
-        <v>284</v>
-      </c>
-      <c r="C285" s="3" t="s">
+      <c r="B285" s="4">
+        <f>B281+1</f>
+        <v>283</v>
+      </c>
+      <c r="C285" s="4">
+        <v>33</v>
+      </c>
+      <c r="D285" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D285" s="3" t="s">
+      <c r="E285" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E285" s="3" t="s">
+      <c r="F285" s="4">
+        <v>2</v>
+      </c>
+      <c r="G285" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1279, 283, 33, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A286" s="4">
+        <f t="shared" si="20"/>
+        <v>1280</v>
+      </c>
+      <c r="B286" s="4">
+        <f>B285</f>
+        <v>283</v>
+      </c>
+      <c r="C286" s="4">
+        <v>33</v>
+      </c>
+      <c r="D286" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F285" s="3">
-        <v>2</v>
-      </c>
-      <c r="G285" s="3" t="str">
+      <c r="E286" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F286" s="4">
+        <v>1</v>
+      </c>
+      <c r="G286" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1279, 284, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A286" s="3">
-        <f t="shared" si="42"/>
-        <v>1280</v>
-      </c>
-      <c r="B286" s="3">
-        <f t="shared" si="43"/>
-        <v>284</v>
-      </c>
-      <c r="C286" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D286" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E286" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F286" s="3">
-        <v>1</v>
-      </c>
-      <c r="G286" s="3" t="str">
-        <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1280, 284, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1280, 283, 33, null, null, 1);</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" s="4">
-        <f t="shared" si="42"/>
+        <f t="shared" si="20"/>
         <v>1281</v>
       </c>
       <c r="B287" s="4">
-        <f>B283+1</f>
-        <v>285</v>
-      </c>
-      <c r="C287" s="4" t="s">
-        <v>17</v>
+        <f t="shared" ref="B287:B288" si="40">B285</f>
+        <v>283</v>
+      </c>
+      <c r="C287" s="4">
+        <v>354</v>
       </c>
       <c r="D287" s="4" t="s">
         <v>17</v>
@@ -32850,20 +32850,20 @@
       </c>
       <c r="G287" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1281, 285, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1281, 283, 354, null, null, 2);</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="4">
-        <f t="shared" si="42"/>
+        <f t="shared" si="20"/>
         <v>1282</v>
       </c>
       <c r="B288" s="4">
-        <f>B287</f>
-        <v>285</v>
-      </c>
-      <c r="C288" s="4" t="s">
-        <v>17</v>
+        <f t="shared" si="40"/>
+        <v>283</v>
+      </c>
+      <c r="C288" s="4">
+        <v>354</v>
       </c>
       <c r="D288" s="4" t="s">
         <v>17</v>
@@ -32876,69 +32876,69 @@
       </c>
       <c r="G288" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1282, 285, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1282, 283, 354, null, null, 1);</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A289" s="4">
-        <f t="shared" si="42"/>
+      <c r="A289" s="3">
+        <f t="shared" si="20"/>
         <v>1283</v>
       </c>
-      <c r="B289" s="4">
-        <f t="shared" ref="B289:B290" si="44">B287</f>
-        <v>285</v>
-      </c>
-      <c r="C289" s="4" t="s">
+      <c r="B289" s="3">
+        <f>B285+1</f>
+        <v>284</v>
+      </c>
+      <c r="C289" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D289" s="4" t="s">
+      <c r="D289" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E289" s="4" t="s">
+      <c r="E289" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F289" s="4">
-        <v>2</v>
-      </c>
-      <c r="G289" s="4" t="str">
+      <c r="F289" s="3">
+        <v>2</v>
+      </c>
+      <c r="G289" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1283, 285, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1283, 284, null, null, null, 2);</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A290" s="4">
-        <f t="shared" si="42"/>
+      <c r="A290" s="3">
+        <f t="shared" si="20"/>
         <v>1284</v>
       </c>
-      <c r="B290" s="4">
-        <f t="shared" si="44"/>
-        <v>285</v>
-      </c>
-      <c r="C290" s="4" t="s">
+      <c r="B290" s="3">
+        <f>B289</f>
+        <v>284</v>
+      </c>
+      <c r="C290" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D290" s="4" t="s">
+      <c r="D290" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E290" s="4" t="s">
+      <c r="E290" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F290" s="4">
-        <v>1</v>
-      </c>
-      <c r="G290" s="4" t="str">
+      <c r="F290" s="3">
+        <v>1</v>
+      </c>
+      <c r="G290" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1284, 285, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1284, 284, null, null, null, 1);</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="3">
-        <f t="shared" si="42"/>
+        <f t="shared" ref="A291:A300" si="41">A290+1</f>
         <v>1285</v>
       </c>
       <c r="B291" s="3">
-        <f>B287+1</f>
-        <v>286</v>
+        <f t="shared" ref="B291:B292" si="42">B289</f>
+        <v>284</v>
       </c>
       <c r="C291" s="3" t="s">
         <v>17</v>
@@ -32954,17 +32954,17 @@
       </c>
       <c r="G291" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1285, 286, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1285, 284, null, null, null, 2);</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="3">
+        <f t="shared" si="41"/>
+        <v>1286</v>
+      </c>
+      <c r="B292" s="3">
         <f t="shared" si="42"/>
-        <v>1286</v>
-      </c>
-      <c r="B292" s="3">
-        <f>B291</f>
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C292" s="3" t="s">
         <v>17</v>
@@ -32980,59 +32980,215 @@
       </c>
       <c r="G292" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1286, 286, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1286, 284, null, null, null, 1);</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A293" s="3">
-        <f t="shared" si="42"/>
+      <c r="A293" s="4">
+        <f t="shared" si="41"/>
         <v>1287</v>
       </c>
-      <c r="B293" s="3">
-        <f t="shared" ref="B293:B294" si="45">B291</f>
+      <c r="B293" s="4">
+        <f>B289+1</f>
+        <v>285</v>
+      </c>
+      <c r="C293" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D293" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E293" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F293" s="4">
+        <v>2</v>
+      </c>
+      <c r="G293" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1287, 285, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="4">
+        <f t="shared" si="41"/>
+        <v>1288</v>
+      </c>
+      <c r="B294" s="4">
+        <f>B293</f>
+        <v>285</v>
+      </c>
+      <c r="C294" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D294" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E294" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F294" s="4">
+        <v>1</v>
+      </c>
+      <c r="G294" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1288, 285, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" s="4">
+        <f t="shared" si="41"/>
+        <v>1289</v>
+      </c>
+      <c r="B295" s="4">
+        <f t="shared" ref="B295:B296" si="43">B293</f>
+        <v>285</v>
+      </c>
+      <c r="C295" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D295" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E295" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F295" s="4">
+        <v>2</v>
+      </c>
+      <c r="G295" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1289, 285, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="4">
+        <f t="shared" si="41"/>
+        <v>1290</v>
+      </c>
+      <c r="B296" s="4">
+        <f t="shared" si="43"/>
+        <v>285</v>
+      </c>
+      <c r="C296" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D296" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E296" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F296" s="4">
+        <v>1</v>
+      </c>
+      <c r="G296" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1290, 285, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" s="3">
+        <f t="shared" si="41"/>
+        <v>1291</v>
+      </c>
+      <c r="B297" s="3">
+        <f>B293+1</f>
         <v>286</v>
       </c>
-      <c r="C293" s="3" t="s">
+      <c r="C297" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D293" s="3" t="s">
+      <c r="D297" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E293" s="3" t="s">
+      <c r="E297" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F293" s="3">
-        <v>2</v>
-      </c>
-      <c r="G293" s="3" t="str">
+      <c r="F297" s="3">
+        <v>2</v>
+      </c>
+      <c r="G297" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1287, 286, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A294" s="3">
-        <f t="shared" si="42"/>
-        <v>1288</v>
-      </c>
-      <c r="B294" s="3">
-        <f t="shared" si="45"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1291, 286, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" s="3">
+        <f t="shared" si="41"/>
+        <v>1292</v>
+      </c>
+      <c r="B298" s="3">
+        <f>B297</f>
         <v>286</v>
       </c>
-      <c r="C294" s="3" t="s">
+      <c r="C298" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D294" s="3" t="s">
+      <c r="D298" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E294" s="3" t="s">
+      <c r="E298" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F294" s="3">
-        <v>1</v>
-      </c>
-      <c r="G294" s="3" t="str">
+      <c r="F298" s="3">
+        <v>1</v>
+      </c>
+      <c r="G298" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1288, 286, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1292, 286, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="3">
+        <f t="shared" si="41"/>
+        <v>1293</v>
+      </c>
+      <c r="B299" s="3">
+        <f t="shared" ref="B299:B300" si="44">B297</f>
+        <v>286</v>
+      </c>
+      <c r="C299" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D299" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E299" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F299" s="3">
+        <v>2</v>
+      </c>
+      <c r="G299" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1293, 286, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="3">
+        <f t="shared" si="41"/>
+        <v>1294</v>
+      </c>
+      <c r="B300" s="3">
+        <f t="shared" si="44"/>
+        <v>286</v>
+      </c>
+      <c r="C300" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D300" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E300" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F300" s="3">
+        <v>1</v>
+      </c>
+      <c r="G300" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1294, 286, null, null, null, 1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eurocopa 2016 Semifinal matchs and olympics 1908
Eurocopa Semifinal matchs and olympics 1908
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -25494,7 +25494,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J300"/>
+  <dimension ref="A1:J306"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
@@ -30853,7 +30853,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
-        <f t="shared" ref="A211:A290" si="20">A210+1</f>
+        <f t="shared" ref="A211:A296" si="20">A210+1</f>
         <v>1205</v>
       </c>
       <c r="B211" s="3">
@@ -32329,7 +32329,7 @@
         <v>2</v>
       </c>
       <c r="G267" s="3" t="str">
-        <f t="shared" ref="G267:G300" si="37">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A267 &amp; ", " &amp; B267 &amp; ", " &amp; C267 &amp; ", " &amp; D267 &amp; ", " &amp; E267 &amp; ", " &amp; F267 &amp; ");"</f>
+        <f t="shared" ref="G267:G306" si="37">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A267 &amp; ", " &amp; B267 &amp; ", " &amp; C267 &amp; ", " &amp; D267 &amp; ", " &amp; E267 &amp; ", " &amp; F267 &amp; ");"</f>
         <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1261, 280, 48, 1, 0, 2);</v>
       </c>
     </row>
@@ -32339,7 +32339,7 @@
         <v>1262</v>
       </c>
       <c r="B268" s="3">
-        <f>B267</f>
+        <f t="shared" ref="B268:B274" si="38">B267</f>
         <v>280</v>
       </c>
       <c r="C268" s="3">
@@ -32365,7 +32365,7 @@
         <v>1263</v>
       </c>
       <c r="B269" s="3">
-        <f>B268</f>
+        <f t="shared" si="38"/>
         <v>280</v>
       </c>
       <c r="C269" s="3">
@@ -32391,7 +32391,7 @@
         <v>1264</v>
       </c>
       <c r="B270" s="3">
-        <f>B269</f>
+        <f t="shared" si="38"/>
         <v>280</v>
       </c>
       <c r="C270" s="3">
@@ -32417,7 +32417,7 @@
         <v>1265</v>
       </c>
       <c r="B271" s="3">
-        <f>B270</f>
+        <f t="shared" si="38"/>
         <v>280</v>
       </c>
       <c r="C271" s="3">
@@ -32443,7 +32443,7 @@
         <v>1266</v>
       </c>
       <c r="B272" s="3">
-        <f>B271</f>
+        <f t="shared" si="38"/>
         <v>280</v>
       </c>
       <c r="C272" s="3">
@@ -32469,7 +32469,7 @@
         <v>1267</v>
       </c>
       <c r="B273" s="3">
-        <f>B272</f>
+        <f t="shared" si="38"/>
         <v>280</v>
       </c>
       <c r="C273" s="3">
@@ -32495,7 +32495,7 @@
         <v>1268</v>
       </c>
       <c r="B274" s="3">
-        <f>B273</f>
+        <f t="shared" si="38"/>
         <v>280</v>
       </c>
       <c r="C274" s="3">
@@ -32579,18 +32579,18 @@
       <c r="C277" s="4">
         <v>4429</v>
       </c>
-      <c r="D277" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E277" s="4" t="s">
-        <v>17</v>
+      <c r="D277" s="4">
+        <v>3</v>
+      </c>
+      <c r="E277" s="4">
+        <v>3</v>
       </c>
       <c r="F277" s="4">
         <v>2</v>
       </c>
       <c r="G277" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1271, 281, 4429, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1271, 281, 4429, 3, 3, 2);</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
@@ -32605,18 +32605,18 @@
       <c r="C278" s="4">
         <v>4429</v>
       </c>
-      <c r="D278" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E278" s="4" t="s">
-        <v>17</v>
+      <c r="D278" s="4">
+        <v>1</v>
+      </c>
+      <c r="E278" s="4">
+        <v>0</v>
       </c>
       <c r="F278" s="4">
         <v>1</v>
       </c>
       <c r="G278" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1272, 281, 4429, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1272, 281, 4429, 1, 0, 1);</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
@@ -32625,24 +32625,24 @@
         <v>1273</v>
       </c>
       <c r="B279" s="4">
-        <f t="shared" ref="B279:B280" si="38">B277</f>
+        <f t="shared" ref="B279:B280" si="39">B277</f>
         <v>281</v>
       </c>
       <c r="C279" s="4">
         <v>32</v>
       </c>
-      <c r="D279" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E279" s="4" t="s">
-        <v>17</v>
+      <c r="D279" s="4">
+        <v>1</v>
+      </c>
+      <c r="E279" s="4">
+        <v>0</v>
       </c>
       <c r="F279" s="4">
         <v>2</v>
       </c>
       <c r="G279" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1273, 281, 32, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1273, 281, 32, 1, 0, 2);</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
@@ -32651,24 +32651,24 @@
         <v>1274</v>
       </c>
       <c r="B280" s="4">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>281</v>
       </c>
       <c r="C280" s="4">
         <v>32</v>
       </c>
-      <c r="D280" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E280" s="4" t="s">
-        <v>17</v>
+      <c r="D280" s="4">
+        <v>1</v>
+      </c>
+      <c r="E280" s="4">
+        <v>0</v>
       </c>
       <c r="F280" s="4">
         <v>1</v>
       </c>
       <c r="G280" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1274, 281, 32, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1274, 281, 32, 1, 0, 1);</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
@@ -32683,18 +32683,18 @@
       <c r="C281" s="3">
         <v>49</v>
       </c>
-      <c r="D281" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E281" s="3" t="s">
-        <v>17</v>
+      <c r="D281" s="3">
+        <v>1</v>
+      </c>
+      <c r="E281" s="3">
+        <v>0</v>
       </c>
       <c r="F281" s="3">
         <v>2</v>
       </c>
       <c r="G281" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1275, 282, 49, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1275, 282, 49, 1, 0, 2);</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
@@ -32709,18 +32709,18 @@
       <c r="C282" s="3">
         <v>49</v>
       </c>
-      <c r="D282" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E282" s="3" t="s">
-        <v>17</v>
+      <c r="D282" s="3">
+        <v>0</v>
+      </c>
+      <c r="E282" s="3">
+        <v>0</v>
       </c>
       <c r="F282" s="3">
         <v>1</v>
       </c>
       <c r="G282" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1276, 282, 49, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1276, 282, 49, 0, 0, 1);</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
@@ -32729,24 +32729,24 @@
         <v>1277</v>
       </c>
       <c r="B283" s="3">
-        <f t="shared" ref="B283:B284" si="39">B281</f>
+        <f t="shared" ref="B283:B290" si="40">B282</f>
         <v>282</v>
       </c>
       <c r="C283" s="3">
         <v>39</v>
       </c>
-      <c r="D283" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E283" s="3" t="s">
-        <v>17</v>
+      <c r="D283" s="3">
+        <v>1</v>
+      </c>
+      <c r="E283" s="3">
+        <v>0</v>
       </c>
       <c r="F283" s="3">
         <v>2</v>
       </c>
       <c r="G283" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1277, 282, 39, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1277, 282, 39, 1, 0, 2);</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.25">
@@ -32755,128 +32755,128 @@
         <v>1278</v>
       </c>
       <c r="B284" s="3">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>282</v>
       </c>
       <c r="C284" s="3">
         <v>39</v>
       </c>
-      <c r="D284" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E284" s="3" t="s">
-        <v>17</v>
+      <c r="D284" s="3">
+        <v>0</v>
+      </c>
+      <c r="E284" s="3">
+        <v>0</v>
       </c>
       <c r="F284" s="3">
         <v>1</v>
       </c>
       <c r="G284" s="3" t="str">
-        <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1278, 282, 39, null, null, 1);</v>
+        <f t="shared" ref="G284:G287" si="41">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A284 &amp; ", " &amp; B284 &amp; ", " &amp; C284 &amp; ", " &amp; D284 &amp; ", " &amp; E284 &amp; ", " &amp; F284 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1278, 282, 39, 0, 0, 1);</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A285" s="4">
+      <c r="A285" s="3">
         <f t="shared" si="20"/>
         <v>1279</v>
       </c>
-      <c r="B285" s="4">
-        <f>B281+1</f>
-        <v>283</v>
-      </c>
-      <c r="C285" s="4">
-        <v>33</v>
-      </c>
-      <c r="D285" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E285" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F285" s="4">
-        <v>2</v>
-      </c>
-      <c r="G285" s="4" t="str">
-        <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1279, 283, 33, null, null, 2);</v>
+      <c r="B285" s="3">
+        <f t="shared" si="40"/>
+        <v>282</v>
+      </c>
+      <c r="C285" s="3">
+        <v>49</v>
+      </c>
+      <c r="D285" s="3">
+        <v>1</v>
+      </c>
+      <c r="E285" s="3">
+        <v>1</v>
+      </c>
+      <c r="F285" s="3">
+        <v>4</v>
+      </c>
+      <c r="G285" s="3" t="str">
+        <f t="shared" si="41"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1279, 282, 49, 1, 1, 4);</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A286" s="4">
+      <c r="A286" s="3">
         <f t="shared" si="20"/>
         <v>1280</v>
       </c>
-      <c r="B286" s="4">
-        <f>B285</f>
-        <v>283</v>
-      </c>
-      <c r="C286" s="4">
-        <v>33</v>
-      </c>
-      <c r="D286" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E286" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F286" s="4">
-        <v>1</v>
-      </c>
-      <c r="G286" s="4" t="str">
-        <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1280, 283, 33, null, null, 1);</v>
+      <c r="B286" s="3">
+        <f t="shared" si="40"/>
+        <v>282</v>
+      </c>
+      <c r="C286" s="3">
+        <v>49</v>
+      </c>
+      <c r="D286" s="3">
+        <v>1</v>
+      </c>
+      <c r="E286" s="3">
+        <v>0</v>
+      </c>
+      <c r="F286" s="3">
+        <v>3</v>
+      </c>
+      <c r="G286" s="3" t="str">
+        <f t="shared" si="41"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1280, 282, 49, 1, 0, 3);</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A287" s="4">
+      <c r="A287" s="3">
         <f t="shared" si="20"/>
         <v>1281</v>
       </c>
-      <c r="B287" s="4">
-        <f t="shared" ref="B287:B288" si="40">B285</f>
-        <v>283</v>
-      </c>
-      <c r="C287" s="4">
-        <v>354</v>
-      </c>
-      <c r="D287" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E287" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F287" s="4">
-        <v>2</v>
-      </c>
-      <c r="G287" s="4" t="str">
-        <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1281, 283, 354, null, null, 2);</v>
+      <c r="B287" s="3">
+        <f t="shared" si="40"/>
+        <v>282</v>
+      </c>
+      <c r="C287" s="3">
+        <v>39</v>
+      </c>
+      <c r="D287" s="3">
+        <v>1</v>
+      </c>
+      <c r="E287" s="3">
+        <v>1</v>
+      </c>
+      <c r="F287" s="3">
+        <v>4</v>
+      </c>
+      <c r="G287" s="3" t="str">
+        <f t="shared" si="41"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1281, 282, 39, 1, 1, 4);</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A288" s="4">
+      <c r="A288" s="3">
         <f t="shared" si="20"/>
         <v>1282</v>
       </c>
-      <c r="B288" s="4">
+      <c r="B288" s="3">
         <f t="shared" si="40"/>
-        <v>283</v>
-      </c>
-      <c r="C288" s="4">
-        <v>354</v>
-      </c>
-      <c r="D288" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E288" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F288" s="4">
-        <v>1</v>
-      </c>
-      <c r="G288" s="4" t="str">
-        <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1282, 283, 354, null, null, 1);</v>
+        <v>282</v>
+      </c>
+      <c r="C288" s="3">
+        <v>39</v>
+      </c>
+      <c r="D288" s="3">
+        <v>1</v>
+      </c>
+      <c r="E288" s="3">
+        <v>0</v>
+      </c>
+      <c r="F288" s="3">
+        <v>3</v>
+      </c>
+      <c r="G288" s="3" t="str">
+        <f t="shared" ref="G288:G290" si="42">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A288 &amp; ", " &amp; B288 &amp; ", " &amp; C288 &amp; ", " &amp; D288 &amp; ", " &amp; E288 &amp; ", " &amp; F288 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1282, 282, 39, 1, 0, 3);</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.25">
@@ -32885,24 +32885,24 @@
         <v>1283</v>
       </c>
       <c r="B289" s="3">
-        <f>B285+1</f>
-        <v>284</v>
-      </c>
-      <c r="C289" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D289" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E289" s="3" t="s">
-        <v>17</v>
+        <f t="shared" si="40"/>
+        <v>282</v>
+      </c>
+      <c r="C289" s="3">
+        <v>49</v>
+      </c>
+      <c r="D289" s="3">
+        <v>6</v>
+      </c>
+      <c r="E289" s="3">
+        <v>0</v>
       </c>
       <c r="F289" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G289" s="3" t="str">
-        <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1283, 284, null, null, null, 2);</v>
+        <f t="shared" si="42"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1283, 282, 49, 6, 0, 7);</v>
       </c>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.25">
@@ -32911,193 +32911,193 @@
         <v>1284</v>
       </c>
       <c r="B290" s="3">
-        <f>B289</f>
-        <v>284</v>
-      </c>
-      <c r="C290" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D290" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E290" s="3" t="s">
-        <v>17</v>
+        <f t="shared" si="40"/>
+        <v>282</v>
+      </c>
+      <c r="C290" s="3">
+        <v>39</v>
+      </c>
+      <c r="D290" s="3">
+        <v>5</v>
+      </c>
+      <c r="E290" s="3">
+        <v>0</v>
       </c>
       <c r="F290" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G290" s="3" t="str">
+        <f t="shared" si="42"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1284, 282, 39, 5, 0, 7);</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" s="4">
+        <f t="shared" si="20"/>
+        <v>1285</v>
+      </c>
+      <c r="B291" s="4">
+        <f>B281+1</f>
+        <v>283</v>
+      </c>
+      <c r="C291" s="4">
+        <v>33</v>
+      </c>
+      <c r="D291" s="4">
+        <v>5</v>
+      </c>
+      <c r="E291" s="4">
+        <v>3</v>
+      </c>
+      <c r="F291" s="4">
+        <v>2</v>
+      </c>
+      <c r="G291" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1284, 284, null, null, null, 1);</v>
-      </c>
-    </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A291" s="3">
-        <f t="shared" ref="A291:A300" si="41">A290+1</f>
-        <v>1285</v>
-      </c>
-      <c r="B291" s="3">
-        <f t="shared" ref="B291:B292" si="42">B289</f>
-        <v>284</v>
-      </c>
-      <c r="C291" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D291" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E291" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F291" s="3">
-        <v>2</v>
-      </c>
-      <c r="G291" s="3" t="str">
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1285, 283, 33, 5, 3, 2);</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" s="4">
+        <f t="shared" si="20"/>
+        <v>1286</v>
+      </c>
+      <c r="B292" s="4">
+        <f>B291</f>
+        <v>283</v>
+      </c>
+      <c r="C292" s="4">
+        <v>33</v>
+      </c>
+      <c r="D292" s="4">
+        <v>4</v>
+      </c>
+      <c r="E292" s="4">
+        <v>0</v>
+      </c>
+      <c r="F292" s="4">
+        <v>1</v>
+      </c>
+      <c r="G292" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1285, 284, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A292" s="3">
-        <f t="shared" si="41"/>
-        <v>1286</v>
-      </c>
-      <c r="B292" s="3">
-        <f t="shared" si="42"/>
-        <v>284</v>
-      </c>
-      <c r="C292" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D292" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E292" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F292" s="3">
-        <v>1</v>
-      </c>
-      <c r="G292" s="3" t="str">
-        <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1286, 284, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1286, 283, 33, 4, 0, 1);</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="4">
-        <f t="shared" si="41"/>
+        <f t="shared" si="20"/>
         <v>1287</v>
       </c>
       <c r="B293" s="4">
-        <f>B289+1</f>
-        <v>285</v>
-      </c>
-      <c r="C293" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D293" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E293" s="4" t="s">
-        <v>17</v>
+        <f t="shared" ref="B293" si="43">B291</f>
+        <v>283</v>
+      </c>
+      <c r="C293" s="4">
+        <v>354</v>
+      </c>
+      <c r="D293" s="4">
+        <v>2</v>
+      </c>
+      <c r="E293" s="4">
+        <v>0</v>
       </c>
       <c r="F293" s="4">
         <v>2</v>
       </c>
       <c r="G293" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1287, 285, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1287, 283, 354, 2, 0, 2);</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="4">
-        <f t="shared" si="41"/>
+        <f>A293+1</f>
         <v>1288</v>
       </c>
       <c r="B294" s="4">
-        <f>B293</f>
-        <v>285</v>
-      </c>
-      <c r="C294" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D294" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E294" s="4" t="s">
-        <v>17</v>
+        <f>B292</f>
+        <v>283</v>
+      </c>
+      <c r="C294" s="4">
+        <v>354</v>
+      </c>
+      <c r="D294" s="4">
+        <v>0</v>
+      </c>
+      <c r="E294" s="4">
+        <v>0</v>
       </c>
       <c r="F294" s="4">
         <v>1</v>
       </c>
       <c r="G294" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1288, 285, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1288, 283, 354, 0, 0, 1);</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A295" s="4">
-        <f t="shared" si="41"/>
+      <c r="A295" s="3">
+        <f t="shared" si="20"/>
         <v>1289</v>
       </c>
-      <c r="B295" s="4">
-        <f t="shared" ref="B295:B296" si="43">B293</f>
-        <v>285</v>
-      </c>
-      <c r="C295" s="4" t="s">
+      <c r="B295" s="3">
+        <f>B291+1</f>
+        <v>284</v>
+      </c>
+      <c r="C295" s="3">
+        <v>351</v>
+      </c>
+      <c r="D295" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D295" s="4" t="s">
+      <c r="E295" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E295" s="4" t="s">
+      <c r="F295" s="3">
+        <v>2</v>
+      </c>
+      <c r="G295" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1289, 284, 351, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" s="3">
+        <f t="shared" si="20"/>
+        <v>1290</v>
+      </c>
+      <c r="B296" s="3">
+        <f>B295</f>
+        <v>284</v>
+      </c>
+      <c r="C296" s="3">
+        <v>351</v>
+      </c>
+      <c r="D296" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F295" s="4">
-        <v>2</v>
-      </c>
-      <c r="G295" s="4" t="str">
+      <c r="E296" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F296" s="3">
+        <v>1</v>
+      </c>
+      <c r="G296" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1289, 285, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A296" s="4">
-        <f t="shared" si="41"/>
-        <v>1290</v>
-      </c>
-      <c r="B296" s="4">
-        <f t="shared" si="43"/>
-        <v>285</v>
-      </c>
-      <c r="C296" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D296" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E296" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F296" s="4">
-        <v>1</v>
-      </c>
-      <c r="G296" s="4" t="str">
-        <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1290, 285, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1290, 284, 351, null, null, 1);</v>
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="3">
-        <f t="shared" si="41"/>
+        <f t="shared" ref="A297:A306" si="44">A296+1</f>
         <v>1291</v>
       </c>
       <c r="B297" s="3">
-        <f>B293+1</f>
-        <v>286</v>
-      </c>
-      <c r="C297" s="3" t="s">
-        <v>17</v>
+        <f t="shared" ref="B297:B298" si="45">B295</f>
+        <v>284</v>
+      </c>
+      <c r="C297" s="3">
+        <v>4429</v>
       </c>
       <c r="D297" s="3" t="s">
         <v>17</v>
@@ -33110,20 +33110,20 @@
       </c>
       <c r="G297" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1291, 286, null, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1291, 284, 4429, null, null, 2);</v>
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="3">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>1292</v>
       </c>
       <c r="B298" s="3">
-        <f>B297</f>
-        <v>286</v>
-      </c>
-      <c r="C298" s="3" t="s">
-        <v>17</v>
+        <f t="shared" si="45"/>
+        <v>284</v>
+      </c>
+      <c r="C298" s="3">
+        <v>4429</v>
       </c>
       <c r="D298" s="3" t="s">
         <v>17</v>
@@ -33136,59 +33136,215 @@
       </c>
       <c r="G298" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1292, 286, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1292, 284, 4429, null, null, 1);</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A299" s="3">
-        <f t="shared" si="41"/>
+      <c r="A299" s="4">
+        <f t="shared" si="44"/>
         <v>1293</v>
       </c>
-      <c r="B299" s="3">
-        <f t="shared" ref="B299:B300" si="44">B297</f>
+      <c r="B299" s="4">
+        <f>B295+1</f>
+        <v>285</v>
+      </c>
+      <c r="C299" s="4">
+        <v>49</v>
+      </c>
+      <c r="D299" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E299" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F299" s="4">
+        <v>2</v>
+      </c>
+      <c r="G299" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1293, 285, 49, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="4">
+        <f t="shared" si="44"/>
+        <v>1294</v>
+      </c>
+      <c r="B300" s="4">
+        <f>B299</f>
+        <v>285</v>
+      </c>
+      <c r="C300" s="4">
+        <v>49</v>
+      </c>
+      <c r="D300" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E300" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F300" s="4">
+        <v>1</v>
+      </c>
+      <c r="G300" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1294, 285, 49, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="4">
+        <f t="shared" si="44"/>
+        <v>1295</v>
+      </c>
+      <c r="B301" s="4">
+        <f t="shared" ref="B301:B302" si="46">B299</f>
+        <v>285</v>
+      </c>
+      <c r="C301" s="4">
+        <v>33</v>
+      </c>
+      <c r="D301" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E301" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F301" s="4">
+        <v>2</v>
+      </c>
+      <c r="G301" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1295, 285, 33, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="4">
+        <f t="shared" si="44"/>
+        <v>1296</v>
+      </c>
+      <c r="B302" s="4">
+        <f t="shared" si="46"/>
+        <v>285</v>
+      </c>
+      <c r="C302" s="4">
+        <v>33</v>
+      </c>
+      <c r="D302" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E302" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F302" s="4">
+        <v>1</v>
+      </c>
+      <c r="G302" s="4" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1296, 285, 33, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" s="3">
+        <f t="shared" si="44"/>
+        <v>1297</v>
+      </c>
+      <c r="B303" s="3">
+        <f>B299+1</f>
         <v>286</v>
       </c>
-      <c r="C299" s="3" t="s">
+      <c r="C303" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D299" s="3" t="s">
+      <c r="D303" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E299" s="3" t="s">
+      <c r="E303" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F299" s="3">
-        <v>2</v>
-      </c>
-      <c r="G299" s="3" t="str">
+      <c r="F303" s="3">
+        <v>2</v>
+      </c>
+      <c r="G303" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1293, 286, null, null, null, 2);</v>
-      </c>
-    </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A300" s="3">
-        <f t="shared" si="41"/>
-        <v>1294</v>
-      </c>
-      <c r="B300" s="3">
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1297, 286, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A304" s="3">
         <f t="shared" si="44"/>
+        <v>1298</v>
+      </c>
+      <c r="B304" s="3">
+        <f>B303</f>
         <v>286</v>
       </c>
-      <c r="C300" s="3" t="s">
+      <c r="C304" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D300" s="3" t="s">
+      <c r="D304" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E300" s="3" t="s">
+      <c r="E304" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F300" s="3">
-        <v>1</v>
-      </c>
-      <c r="G300" s="3" t="str">
+      <c r="F304" s="3">
+        <v>1</v>
+      </c>
+      <c r="G304" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1294, 286, null, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1298, 286, null, null, null, 1);</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" s="3">
+        <f t="shared" si="44"/>
+        <v>1299</v>
+      </c>
+      <c r="B305" s="3">
+        <f t="shared" ref="B305:B306" si="47">B303</f>
+        <v>286</v>
+      </c>
+      <c r="C305" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D305" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E305" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F305" s="3">
+        <v>2</v>
+      </c>
+      <c r="G305" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1299, 286, null, null, null, 2);</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" s="3">
+        <f t="shared" si="44"/>
+        <v>1300</v>
+      </c>
+      <c r="B306" s="3">
+        <f t="shared" si="47"/>
+        <v>286</v>
+      </c>
+      <c r="C306" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D306" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E306" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F306" s="3">
+        <v>1</v>
+      </c>
+      <c r="G306" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1300, 286, null, null, null, 1);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eurocopa 2016 SemiFinal 1 Olympics 1936 - 1948
Eurocopa 2016 SemiFinal 1 Olympics 1936 - 1948
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -33047,18 +33047,18 @@
       <c r="C295" s="3">
         <v>351</v>
       </c>
-      <c r="D295" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E295" s="3" t="s">
-        <v>17</v>
+      <c r="D295" s="3">
+        <v>2</v>
+      </c>
+      <c r="E295" s="3">
+        <v>3</v>
       </c>
       <c r="F295" s="3">
         <v>2</v>
       </c>
       <c r="G295" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1289, 284, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1289, 284, 351, 2, 3, 2);</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.25">
@@ -33073,18 +33073,18 @@
       <c r="C296" s="3">
         <v>351</v>
       </c>
-      <c r="D296" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E296" s="3" t="s">
-        <v>17</v>
+      <c r="D296" s="3">
+        <v>0</v>
+      </c>
+      <c r="E296" s="3">
+        <v>0</v>
       </c>
       <c r="F296" s="3">
         <v>1</v>
       </c>
       <c r="G296" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1290, 284, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1290, 284, 351, 0, 0, 1);</v>
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
@@ -33099,18 +33099,18 @@
       <c r="C297" s="3">
         <v>4429</v>
       </c>
-      <c r="D297" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E297" s="3" t="s">
-        <v>17</v>
+      <c r="D297" s="3">
+        <v>0</v>
+      </c>
+      <c r="E297" s="3">
+        <v>0</v>
       </c>
       <c r="F297" s="3">
         <v>2</v>
       </c>
       <c r="G297" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1291, 284, 4429, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1291, 284, 4429, 0, 0, 2);</v>
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
@@ -33125,18 +33125,18 @@
       <c r="C298" s="3">
         <v>4429</v>
       </c>
-      <c r="D298" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E298" s="3" t="s">
-        <v>17</v>
+      <c r="D298" s="3">
+        <v>0</v>
+      </c>
+      <c r="E298" s="3">
+        <v>0</v>
       </c>
       <c r="F298" s="3">
         <v>1</v>
       </c>
       <c r="G298" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1292, 284, 4429, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1292, 284, 4429, 0, 0, 1);</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final UEFA Euro 2016
Final UEFA Euro 2016
</commit_message>
<xml_diff>
--- a/Scripts/eurocopa/eurocopa.xlsx
+++ b/Scripts/eurocopa/eurocopa.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>match_number</t>
@@ -25494,7 +25491,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J306"/>
+  <dimension ref="A1:J310"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
@@ -26020,7 +26017,7 @@
         <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G27" t="str">
         <f>"insert into game (matchid, matchdate, game_type, country) values (" &amp; A27 &amp; ", '" &amp; B27 &amp; "', " &amp; C27 &amp; ", " &amp; D27 &amp;  ");"</f>
@@ -32329,7 +32326,7 @@
         <v>2</v>
       </c>
       <c r="G267" s="3" t="str">
-        <f t="shared" ref="G267:G306" si="37">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A267 &amp; ", " &amp; B267 &amp; ", " &amp; C267 &amp; ", " &amp; D267 &amp; ", " &amp; E267 &amp; ", " &amp; F267 &amp; ");"</f>
+        <f t="shared" ref="G267:G310" si="37">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A267 &amp; ", " &amp; B267 &amp; ", " &amp; C267 &amp; ", " &amp; D267 &amp; ", " &amp; E267 &amp; ", " &amp; F267 &amp; ");"</f>
         <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1261, 280, 48, 1, 0, 2);</v>
       </c>
     </row>
@@ -33089,7 +33086,7 @@
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="3">
-        <f t="shared" ref="A297:A306" si="44">A296+1</f>
+        <f t="shared" ref="A297:A310" si="44">A296+1</f>
         <v>1291</v>
       </c>
       <c r="B297" s="3">
@@ -33255,18 +33252,18 @@
       <c r="C303" s="3">
         <v>351</v>
       </c>
-      <c r="D303" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E303" s="3" t="s">
-        <v>17</v>
+      <c r="D303" s="3">
+        <v>0</v>
+      </c>
+      <c r="E303" s="3">
+        <v>0</v>
       </c>
       <c r="F303" s="3">
         <v>2</v>
       </c>
       <c r="G303" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1297, 286, 351, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1297, 286, 351, 0, 0, 2);</v>
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.25">
@@ -33281,18 +33278,18 @@
       <c r="C304" s="3">
         <v>351</v>
       </c>
-      <c r="D304" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E304" s="3" t="s">
-        <v>17</v>
+      <c r="D304" s="3">
+        <v>0</v>
+      </c>
+      <c r="E304" s="3">
+        <v>0</v>
       </c>
       <c r="F304" s="3">
         <v>1</v>
       </c>
       <c r="G304" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1298, 286, 351, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1298, 286, 351, 0, 0, 1);</v>
       </c>
     </row>
     <row r="305" spans="1:7" x14ac:dyDescent="0.25">
@@ -33301,24 +33298,24 @@
         <v>1299</v>
       </c>
       <c r="B305" s="3">
-        <f t="shared" ref="B305:B306" si="47">B303</f>
+        <f t="shared" ref="B305:B310" si="47">B303</f>
         <v>286</v>
       </c>
       <c r="C305" s="3">
         <v>33</v>
       </c>
-      <c r="D305" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E305" s="3" t="s">
-        <v>17</v>
+      <c r="D305" s="3">
+        <v>0</v>
+      </c>
+      <c r="E305" s="3">
+        <v>0</v>
       </c>
       <c r="F305" s="3">
         <v>2</v>
       </c>
       <c r="G305" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1299, 286, 33, null, null, 2);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1299, 286, 33, 0, 0, 2);</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.25">
@@ -33333,18 +33330,122 @@
       <c r="C306" s="3">
         <v>33</v>
       </c>
-      <c r="D306" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E306" s="3" t="s">
-        <v>17</v>
+      <c r="D306" s="3">
+        <v>0</v>
+      </c>
+      <c r="E306" s="3">
+        <v>0</v>
       </c>
       <c r="F306" s="3">
         <v>1</v>
       </c>
       <c r="G306" s="3" t="str">
         <f t="shared" si="37"/>
-        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1300, 286, 33, null, null, 1);</v>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1300, 286, 33, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" s="3">
+        <f t="shared" si="44"/>
+        <v>1301</v>
+      </c>
+      <c r="B307" s="3">
+        <f t="shared" si="47"/>
+        <v>286</v>
+      </c>
+      <c r="C307" s="3">
+        <v>351</v>
+      </c>
+      <c r="D307" s="3">
+        <v>1</v>
+      </c>
+      <c r="E307" s="3">
+        <v>3</v>
+      </c>
+      <c r="F307" s="3">
+        <v>4</v>
+      </c>
+      <c r="G307" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1301, 286, 351, 1, 3, 4);</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A308" s="3">
+        <f t="shared" si="44"/>
+        <v>1302</v>
+      </c>
+      <c r="B308" s="3">
+        <f t="shared" si="47"/>
+        <v>286</v>
+      </c>
+      <c r="C308" s="3">
+        <v>351</v>
+      </c>
+      <c r="D308" s="3">
+        <v>0</v>
+      </c>
+      <c r="E308" s="3">
+        <v>0</v>
+      </c>
+      <c r="F308" s="3">
+        <v>3</v>
+      </c>
+      <c r="G308" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1302, 286, 351, 0, 0, 3);</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A309" s="3">
+        <f t="shared" si="44"/>
+        <v>1303</v>
+      </c>
+      <c r="B309" s="3">
+        <f t="shared" si="47"/>
+        <v>286</v>
+      </c>
+      <c r="C309" s="3">
+        <v>33</v>
+      </c>
+      <c r="D309" s="3">
+        <v>0</v>
+      </c>
+      <c r="E309" s="3">
+        <v>0</v>
+      </c>
+      <c r="F309" s="3">
+        <v>4</v>
+      </c>
+      <c r="G309" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1303, 286, 33, 0, 0, 4);</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" s="3">
+        <f t="shared" si="44"/>
+        <v>1304</v>
+      </c>
+      <c r="B310" s="3">
+        <f t="shared" si="47"/>
+        <v>286</v>
+      </c>
+      <c r="C310" s="3">
+        <v>33</v>
+      </c>
+      <c r="D310" s="3">
+        <v>0</v>
+      </c>
+      <c r="E310" s="3">
+        <v>0</v>
+      </c>
+      <c r="F310" s="3">
+        <v>3</v>
+      </c>
+      <c r="G310" s="3" t="str">
+        <f t="shared" si="37"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (1304, 286, 33, 0, 0, 3);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>